<commit_message>
fix RNN and std linear scale
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\RTSNet_Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB88B72-C0D3-4FDF-A585-C24492C40F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD7906D-E0F3-4FF7-9305-CAA169182792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="88">
   <si>
     <t>N_E=1000, N_CV=100, N_T=200</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t xml:space="preserve">KNet J=5, train on T=100 (n_Epochs=500, n_Batch=100, learningRate=5e-3, weightDecay=1e-4) [dB] </t>
+  </si>
+  <si>
+    <t>RTS J=5 [dB]</t>
   </si>
 </sst>
 </file>
@@ -2076,10 +2079,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FAE463-692A-4AB1-8AB9-770196756CC0}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2532,6 +2535,14 @@
         <v>-48.985799999999998</v>
       </c>
     </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25">
+        <v>-13.9579</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add random sequence length
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\RTSNet_Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424AC929-B96C-4AEB-82E5-47DFD16E0016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC821074-C249-4320-8B35-9A6515A6708B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="107">
   <si>
     <t>N_E=1000, N_CV=100, N_T=200</t>
   </si>
@@ -173,9 +173,6 @@
     <t xml:space="preserve">RTSNet true [dB] </t>
   </si>
   <si>
-    <t>Random initial conditions</t>
-  </si>
-  <si>
     <t>N_E=1000, N_CV=100, N_T=200, 2x2, H=I</t>
   </si>
   <si>
@@ -341,10 +338,25 @@
     <t xml:space="preserve">RTSNet mismatch (trained on fixed init state = [0,0], test on random init but feed with false init state = [0,0] still) [dB] </t>
   </si>
   <si>
-    <t>EKF (test on random and known init) [dB]</t>
-  </si>
-  <si>
     <t>RTS (test on random and known init) [dB]</t>
+  </si>
+  <si>
+    <t>Random initial conditions(x1 and x2 both uniformly distributed on [0,100) )</t>
+  </si>
+  <si>
+    <t>RTS (test on random init, feed with init=[50,50], P0 = [100^2/12, 0; 0, 100^2/12]) [dB]</t>
+  </si>
+  <si>
+    <t>KF (test on random init, feed with init=[50,50], P0 = [100^2/12, 0; 0, 100^2/12]) [dB]</t>
+  </si>
+  <si>
+    <t>KF std [dB]</t>
+  </si>
+  <si>
+    <t>KF (test on random and known init) [dB]</t>
+  </si>
+  <si>
+    <t>Gneralization to long sequence (T_train ~ U[100,1000], T_test ~ U[100,1000])</t>
   </si>
 </sst>
 </file>
@@ -402,7 +414,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -412,12 +424,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -514,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -575,14 +581,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -611,10 +613,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -626,6 +624,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -906,97 +926,97 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I132"/>
+  <dimension ref="A1:I144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="18.36328125" customWidth="1"/>
-    <col min="2" max="2" width="37.7265625" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="1" max="1" width="22.4609375" customWidth="1"/>
+    <col min="2" max="2" width="19.07421875" customWidth="1"/>
+    <col min="3" max="3" width="8.69140625" customWidth="1"/>
+    <col min="6" max="6" width="23.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="23" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="D4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="44" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A5" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="45">
+        <v>10.022600000000001</v>
+      </c>
+      <c r="C5" s="45">
+        <v>5.4199999999999998E-2</v>
+      </c>
+      <c r="D5" s="45">
+        <v>-10.002700000000001</v>
+      </c>
+      <c r="E5" s="45">
+        <v>-19.947399999999998</v>
+      </c>
+      <c r="F5" s="47">
+        <v>-29.9617</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="47">
-        <v>10.022600000000001</v>
-      </c>
-      <c r="C5" s="47">
-        <v>5.4199999999999998E-2</v>
-      </c>
-      <c r="D5" s="47">
-        <v>-10.002700000000001</v>
-      </c>
-      <c r="E5" s="47">
-        <v>-19.947399999999998</v>
-      </c>
-      <c r="F5" s="49">
-        <v>-29.9617</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="47">
+      <c r="B6" s="45">
         <v>0.42399999999999999</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C6" s="45">
         <v>0.4476</v>
       </c>
-      <c r="D6" s="47">
+      <c r="D6" s="45">
         <v>0.42730000000000001</v>
       </c>
-      <c r="E6" s="47">
+      <c r="E6" s="45">
         <v>0.41070000000000001</v>
       </c>
-      <c r="F6" s="49">
+      <c r="F6" s="47">
         <v>0.42949999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="45" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A7" s="43" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="9">
@@ -1015,9 +1035,9 @@
         <v>-31.885899999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="45" t="s">
-        <v>79</v>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A8" s="43" t="s">
+        <v>78</v>
       </c>
       <c r="B8" s="9">
         <v>0.50170000000000003</v>
@@ -1035,8 +1055,8 @@
         <v>0.51370000000000005</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="45" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A9" s="43" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="9">
@@ -1056,9 +1076,9 @@
       </c>
       <c r="G9" s="22"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="45" t="s">
-        <v>80</v>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A10" s="43" t="s">
+        <v>79</v>
       </c>
       <c r="B10" s="9">
         <v>0.4869</v>
@@ -1077,8 +1097,8 @@
       </c>
       <c r="G10" s="22"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="45" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A11" s="43" t="s">
         <v>44</v>
       </c>
       <c r="B11" s="9">
@@ -1087,14 +1107,18 @@
       <c r="C11" s="9">
         <v>-3.6951999999999998</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
+      <c r="D11" s="9">
+        <v>-13.7377</v>
+      </c>
+      <c r="E11" s="9">
+        <v>-23.7318</v>
+      </c>
       <c r="F11" s="34"/>
       <c r="G11" s="22"/>
     </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="46" t="s">
-        <v>89</v>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="44" t="s">
+        <v>88</v>
       </c>
       <c r="B12" s="35">
         <v>0.48709999999999998</v>
@@ -1102,12 +1126,16 @@
       <c r="C12" s="35">
         <v>0.53669999999999995</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="48"/>
+      <c r="D12" s="35">
+        <v>0.46279999999999999</v>
+      </c>
+      <c r="E12" s="35">
+        <v>0.51170000000000004</v>
+      </c>
+      <c r="F12" s="46"/>
       <c r="G12" s="22"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13" s="22"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -1116,76 +1144,76 @@
       <c r="F13" s="30"/>
       <c r="G13" s="22"/>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A14" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G14" s="22"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="26" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="G15" s="22"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A16" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="G15" s="22"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="44" t="s">
+      <c r="B16" s="45">
+        <v>10.004300000000001</v>
+      </c>
+      <c r="C16" s="49">
+        <v>-8.4907000000000005E-5</v>
+      </c>
+      <c r="D16" s="45">
+        <v>-10.0288</v>
+      </c>
+      <c r="E16" s="45">
+        <v>-19.9815</v>
+      </c>
+      <c r="F16" s="47">
+        <v>-29.968599999999999</v>
+      </c>
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A17" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="47">
-        <v>10.004300000000001</v>
-      </c>
-      <c r="C16" s="51">
-        <v>-8.4907000000000005E-5</v>
-      </c>
-      <c r="D16" s="47">
-        <v>-10.0288</v>
-      </c>
-      <c r="E16" s="47">
-        <v>-19.9815</v>
-      </c>
-      <c r="F16" s="49">
-        <v>-29.968599999999999</v>
-      </c>
-      <c r="G16" s="22"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="47">
+      <c r="B17" s="45">
         <v>0.41909999999999997</v>
       </c>
-      <c r="C17" s="47">
+      <c r="C17" s="45">
         <v>0.39150000000000001</v>
       </c>
-      <c r="D17" s="47">
+      <c r="D17" s="45">
         <v>0.43099999999999999</v>
       </c>
-      <c r="E17" s="47">
+      <c r="E17" s="45">
         <v>0.40439999999999998</v>
       </c>
-      <c r="F17" s="49">
+      <c r="F17" s="47">
         <v>0.43509999999999999</v>
       </c>
       <c r="G17" s="22"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A18" s="12" t="s">
         <v>8</v>
       </c>
@@ -1206,9 +1234,9 @@
       </c>
       <c r="G18" s="22"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A19" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" s="9">
         <v>0.70950000000000002</v>
@@ -1227,7 +1255,7 @@
       </c>
       <c r="G19" s="22"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A20" s="12" t="s">
         <v>9</v>
       </c>
@@ -1248,9 +1276,9 @@
       </c>
       <c r="G20" s="22"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A21" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" s="9">
         <v>0.79410000000000003</v>
@@ -1268,27 +1296,47 @@
         <v>0.83679999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A22" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="9">
+        <v>1.8805000000000001</v>
+      </c>
+      <c r="C22" s="9">
+        <v>-8.1684999999999999</v>
+      </c>
+      <c r="D22" s="9">
+        <v>-18.091699999999999</v>
+      </c>
+      <c r="E22" s="9">
+        <v>-27.875299999999999</v>
+      </c>
+      <c r="F22" s="34">
+        <v>-37.189599999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A23" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="38"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="B23" s="35">
+        <v>0.79549999999999998</v>
+      </c>
+      <c r="C23" s="35">
+        <v>0.72040000000000004</v>
+      </c>
+      <c r="D23" s="35">
+        <v>0.79720000000000002</v>
+      </c>
+      <c r="E23" s="35">
+        <v>0.74619999999999997</v>
+      </c>
+      <c r="F23" s="46">
+        <v>0.84540000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A24" s="22"/>
       <c r="B24" s="22"/>
       <c r="C24" s="22"/>
@@ -1296,12 +1344,12 @@
       <c r="E24" s="22"/>
       <c r="F24" s="31"/>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
@@ -1321,52 +1369,52 @@
         <v>7</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A27" s="42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="45">
+        <v>10.011900000000001</v>
+      </c>
+      <c r="C27" s="45">
+        <v>-8.3000000000000001E-3</v>
+      </c>
+      <c r="D27" s="45">
+        <v>-10.004200000000001</v>
+      </c>
+      <c r="E27" s="45">
+        <v>-19.976700000000001</v>
+      </c>
+      <c r="F27" s="45">
+        <v>-30.0029</v>
+      </c>
+      <c r="G27" s="48"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A28" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="47">
-        <v>10.011900000000001</v>
-      </c>
-      <c r="C27" s="47">
-        <v>-8.3000000000000001E-3</v>
-      </c>
-      <c r="D27" s="47">
-        <v>-10.004200000000001</v>
-      </c>
-      <c r="E27" s="47">
-        <v>-19.976700000000001</v>
-      </c>
-      <c r="F27" s="47">
-        <v>-30.0029</v>
-      </c>
-      <c r="G27" s="50"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="B28" s="47">
+      <c r="B28" s="45">
         <v>0.39750000000000002</v>
       </c>
-      <c r="C28" s="47">
+      <c r="C28" s="45">
         <v>0.43390000000000001</v>
       </c>
-      <c r="D28" s="47">
+      <c r="D28" s="45">
         <v>0.44819999999999999</v>
       </c>
-      <c r="E28" s="47">
+      <c r="E28" s="45">
         <v>0.4158</v>
       </c>
-      <c r="F28" s="47">
+      <c r="F28" s="45">
         <v>0.42849999999999999</v>
       </c>
-      <c r="G28" s="50"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G28" s="48"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A29" s="12" t="s">
         <v>8</v>
       </c>
@@ -1390,9 +1438,9 @@
         <v>3.2074406147003152E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A30" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B30" s="9">
         <v>1.0863</v>
@@ -1411,7 +1459,7 @@
       </c>
       <c r="G30" s="34"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A31" s="12" t="s">
         <v>9</v>
       </c>
@@ -1436,9 +1484,9 @@
         <v>6.6839754581451E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A32" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" s="9">
         <v>1.2419</v>
@@ -1457,7 +1505,7 @@
       </c>
       <c r="G32" s="34"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A33" s="12" t="s">
         <v>10</v>
       </c>
@@ -1481,9 +1529,9 @@
         <v>0.28249908566474902</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A34" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B34" s="35">
         <v>1.1987000000000001</v>
@@ -1497,12 +1545,12 @@
       <c r="E34" s="35">
         <v>1.1524000000000001</v>
       </c>
-      <c r="F34" s="39">
+      <c r="F34" s="38">
         <v>1.2285999999999999</v>
       </c>
       <c r="G34" s="36"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A35" s="22"/>
       <c r="B35" s="22"/>
       <c r="C35" s="22"/>
@@ -1511,7 +1559,7 @@
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A36" s="22"/>
       <c r="B36" s="22"/>
       <c r="C36" s="22"/>
@@ -1520,9 +1568,9 @@
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A37" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B37" s="22"/>
       <c r="C37" s="22"/>
@@ -1531,9 +1579,9 @@
       <c r="F37" s="22"/>
       <c r="G37" s="22"/>
     </row>
-    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B38" s="22"/>
       <c r="C38" s="22"/>
@@ -1542,7 +1590,7 @@
       <c r="F38" s="22"/>
       <c r="G38" s="22"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A39" s="2" t="s">
         <v>2</v>
       </c>
@@ -1554,10 +1602,10 @@
       <c r="E39" s="24"/>
       <c r="F39" s="24"/>
       <c r="G39" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A40" s="12" t="s">
         <v>8</v>
       </c>
@@ -1573,9 +1621,9 @@
         <v>9.5532480478286497E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A41" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B41" s="22"/>
       <c r="C41" s="22">
@@ -1586,7 +1634,7 @@
       <c r="F41" s="22"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A42" s="12" t="s">
         <v>9</v>
       </c>
@@ -1602,9 +1650,9 @@
         <v>0.19651466488838149</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A43" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B43" s="22"/>
       <c r="C43" s="22">
@@ -1615,7 +1663,7 @@
       <c r="F43" s="22"/>
       <c r="G43" s="8"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A44" s="12" t="s">
         <v>44</v>
       </c>
@@ -1632,9 +1680,9 @@
         <v>2.9767569208145104</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A45" s="13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B45" s="10"/>
       <c r="C45" s="10">
@@ -1645,7 +1693,7 @@
       <c r="F45" s="10"/>
       <c r="G45" s="11"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A46" s="22"/>
       <c r="B46" s="22"/>
       <c r="C46" s="22"/>
@@ -1654,9 +1702,9 @@
       <c r="F46" s="22"/>
       <c r="G46" s="22"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A47" s="18" t="s">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="B47" s="22"/>
       <c r="C47" s="22"/>
@@ -1665,9 +1713,9 @@
       <c r="F47" s="22"/>
       <c r="G47" s="22"/>
     </row>
-    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A48" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B48" s="22"/>
       <c r="C48" s="22"/>
@@ -1676,154 +1724,119 @@
       <c r="F48" s="22"/>
       <c r="G48" s="22"/>
     </row>
-    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A49" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B49" s="24"/>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="40"/>
-      <c r="F49" s="41"/>
-      <c r="G49" s="40"/>
-      <c r="H49" s="42"/>
-      <c r="I49" s="37"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A50" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="22"/>
+      <c r="C50" s="22">
+        <v>-7.2404999999999999</v>
+      </c>
+      <c r="D50" s="22"/>
+      <c r="E50" s="22"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="8"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A51" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51" s="22"/>
+      <c r="C51" s="22">
+        <v>0.54310000000000003</v>
+      </c>
+      <c r="D51" s="22"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A52" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="22"/>
+      <c r="C52" s="22">
+        <v>-11.852600000000001</v>
+      </c>
+      <c r="D52" s="22"/>
+      <c r="E52" s="22"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="8"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A53" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="22"/>
+      <c r="C53" s="22">
+        <v>0.68740000000000001</v>
+      </c>
+      <c r="D53" s="22"/>
+      <c r="E53" s="22"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="8"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A54" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+      <c r="D54" s="22"/>
+      <c r="E54" s="22"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="8"/>
+    </row>
+    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="11"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A56" s="22"/>
+      <c r="B56" s="22"/>
+      <c r="C56" s="22"/>
+      <c r="D56" s="22"/>
+      <c r="E56" s="22"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A57" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="22"/>
-      <c r="C50" s="8">
-        <v>-7.3005000000000004</v>
-      </c>
-      <c r="D50" s="22"/>
-      <c r="E50" s="40"/>
-      <c r="F50" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="G50" s="57">
-        <v>30.081099999999999</v>
-      </c>
-      <c r="H50" s="40"/>
-      <c r="I50" s="37"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" s="22"/>
-      <c r="C51" s="8">
-        <v>0.91549999999999998</v>
-      </c>
-      <c r="D51" s="22"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="G51" s="8">
-        <v>26.237500000000001</v>
-      </c>
-      <c r="H51" s="40"/>
-      <c r="I51" s="37"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B52" s="22"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="40"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="40"/>
-      <c r="I52" s="37"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="B53" s="22"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="40"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="40"/>
-      <c r="I53" s="37"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" s="52" t="s">
-        <v>98</v>
-      </c>
-      <c r="B54" s="53"/>
-      <c r="C54" s="54">
-        <v>-11.680099999999999</v>
-      </c>
-      <c r="D54" s="22"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G54" s="8">
-        <v>9.0884</v>
-      </c>
-      <c r="H54" s="40"/>
-      <c r="I54" s="37"/>
-    </row>
-    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="52" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" s="53"/>
-      <c r="C55" s="54">
-        <v>1.2060999999999999</v>
-      </c>
-      <c r="D55" s="22"/>
-      <c r="E55" s="40"/>
-      <c r="F55" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="G55" s="11">
-        <v>2.7212000000000001</v>
-      </c>
-      <c r="H55" s="40"/>
-      <c r="I55" s="37"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A56" s="52" t="s">
-        <v>99</v>
-      </c>
-      <c r="B56" s="53"/>
-      <c r="C56" s="55">
-        <v>-11.6053</v>
-      </c>
-      <c r="D56" s="22"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="37"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" s="52" t="s">
-        <v>81</v>
-      </c>
-      <c r="B57" s="53"/>
-      <c r="C57" s="55">
-        <v>1.22</v>
-      </c>
+      <c r="B57" s="22"/>
+      <c r="C57" s="22"/>
       <c r="D57" s="22"/>
       <c r="E57" s="22"/>
       <c r="F57" s="22"/>
       <c r="G57" s="22"/>
-      <c r="H57" s="22"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58" s="22"/>
+    </row>
+    <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A58" s="22" t="s">
+        <v>46</v>
+      </c>
       <c r="B58" s="22"/>
       <c r="C58" s="22"/>
       <c r="D58" s="22"/>
@@ -1831,884 +1844,1089 @@
       <c r="F58" s="22"/>
       <c r="G58" s="22"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A59" s="22"/>
-      <c r="B59" s="22"/>
-      <c r="C59" s="22"/>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A59" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="24"/>
+      <c r="C59" s="26" t="s">
+        <v>4</v>
+      </c>
       <c r="D59" s="22"/>
-      <c r="E59" s="22"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
+      <c r="E59" s="39"/>
+      <c r="F59" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="G59" s="51">
+        <v>30.081099999999999</v>
+      </c>
+      <c r="H59" s="40"/>
+      <c r="I59" s="37"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A60" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="22"/>
+      <c r="C60" s="56">
+        <v>-1.0999999999999999E-2</v>
+      </c>
+      <c r="D60" s="22"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G60" s="8">
+        <v>26.237500000000001</v>
+      </c>
+      <c r="H60" s="40"/>
+      <c r="I60" s="37"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A61" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="22"/>
+      <c r="C61" s="56">
+        <v>0.3891</v>
+      </c>
+      <c r="D61" s="22"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="63"/>
+      <c r="G61" s="64"/>
+      <c r="H61" s="40"/>
+      <c r="I61" s="37"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A62" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" s="22"/>
+      <c r="C62" s="34">
+        <v>-7.2916999999999996</v>
+      </c>
+      <c r="D62" s="22"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G62" s="8">
+        <v>-6.7626999999999997</v>
+      </c>
+      <c r="H62" s="9"/>
+      <c r="I62" s="37"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A63" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B63" s="22"/>
+      <c r="C63" s="34">
+        <v>0.90980000000000005</v>
+      </c>
+      <c r="D63" s="22"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G63" s="8">
+        <v>0.88480000000000003</v>
+      </c>
+      <c r="H63" s="9"/>
+      <c r="I63" s="37"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A64" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B64" s="22"/>
+      <c r="C64" s="34">
+        <v>-11.7737</v>
+      </c>
+      <c r="D64" s="22"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G64" s="8">
+        <v>-11.523199999999999</v>
+      </c>
+      <c r="H64" s="9"/>
+      <c r="I64" s="37"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A65" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" s="22"/>
+      <c r="C65" s="34">
+        <v>1.2115</v>
+      </c>
+      <c r="D65" s="22"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G65" s="8">
+        <v>1.1852</v>
+      </c>
+      <c r="H65" s="9"/>
+      <c r="I65" s="37"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A66" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="B66" s="39"/>
+      <c r="C66" s="58">
+        <v>-11.471500000000001</v>
+      </c>
+      <c r="D66" s="22"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="G66" s="8">
+        <v>9.0884</v>
+      </c>
+      <c r="H66" s="39"/>
+      <c r="I66" s="37"/>
+    </row>
+    <row r="67" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A67" s="57" t="s">
+        <v>81</v>
+      </c>
+      <c r="B67" s="39"/>
+      <c r="C67" s="58">
+        <v>1.2063999999999999</v>
+      </c>
+      <c r="D67" s="22"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G67" s="11">
+        <v>2.7212000000000001</v>
+      </c>
+      <c r="H67" s="39"/>
+      <c r="I67" s="37"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A68" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="B68" s="39"/>
+      <c r="C68" s="59">
+        <v>-11.5383</v>
+      </c>
+      <c r="D68" s="22"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="39"/>
+      <c r="I68" s="37"/>
+    </row>
+    <row r="69" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A69" s="60" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" s="61"/>
+      <c r="C69" s="62">
+        <v>1.1716</v>
+      </c>
+      <c r="D69" s="22"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="22"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A70" s="22"/>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+      <c r="D70" s="22"/>
+      <c r="E70" s="22"/>
+      <c r="F70" s="22"/>
+      <c r="G70" s="22"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A71" s="22"/>
+      <c r="B71" s="22"/>
+      <c r="C71" s="22"/>
+      <c r="D71" s="22"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A73" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" s="17" t="s">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A74" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="1" t="s">
+    <row r="75" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A75" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A76" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B76" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D76" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E76" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="F76" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G64" s="4" t="s">
+      <c r="G76" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="12" t="s">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A77" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B65" s="9">
+      <c r="B77" s="9">
         <v>0.37009999999999998</v>
       </c>
-      <c r="C65" s="9">
+      <c r="C77" s="9">
         <v>-9.5507000000000009</v>
       </c>
-      <c r="D65" s="9">
+      <c r="D77" s="9">
         <v>-19.614100000000001</v>
       </c>
-      <c r="E65" s="9">
+      <c r="E77" s="9">
         <v>-29.642099999999999</v>
       </c>
-      <c r="F65" s="9">
+      <c r="F77" s="9">
         <v>-39.517699999999998</v>
       </c>
-      <c r="G65" s="8">
+      <c r="G77" s="8">
         <f>6.71297335624694/200</f>
         <v>3.3564866781234701E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" s="12" t="s">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A78" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B66" s="9">
+      <c r="B78" s="9">
         <v>-2.0627</v>
       </c>
-      <c r="C66" s="9">
+      <c r="C78" s="9">
         <v>-12.234</v>
       </c>
-      <c r="D66" s="9">
+      <c r="D78" s="9">
         <v>-22.131499999999999</v>
       </c>
-      <c r="E66" s="9">
+      <c r="E78" s="9">
         <v>-32.137099999999997</v>
       </c>
-      <c r="F66" s="9">
+      <c r="F78" s="9">
         <v>-42.033499999999997</v>
       </c>
-      <c r="G66" s="8">
+      <c r="G78" s="8">
         <f>13.8022818565368/200</f>
         <v>6.9011409282683997E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="13" t="s">
+    <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A79" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
-      <c r="E67" s="10"/>
-      <c r="F67" s="10"/>
-      <c r="G67" s="11"/>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" s="23" t="s">
+      <c r="B79" s="10"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="11"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A82" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D82" s="32"/>
+    </row>
+    <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A83" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D70" s="32"/>
-    </row>
-    <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="1" t="s">
+      <c r="B83" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F83" s="32"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A84" s="2"/>
+      <c r="B84" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F71" s="32"/>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="2"/>
-      <c r="B72" s="3" t="s">
+      <c r="C84" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="15" t="s">
+      <c r="D84" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="E84" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E72" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" s="5" t="s">
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A85" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B73" s="33">
+      <c r="B85" s="33">
         <v>-10.795199999999999</v>
       </c>
-      <c r="C73">
+      <c r="C85">
         <f>1.38270020484924/200</f>
         <v>6.9135010242462004E-3</v>
       </c>
-      <c r="D73" s="33">
+      <c r="D85" s="33">
         <v>-11.2011</v>
       </c>
-      <c r="E73" s="27">
+      <c r="E85" s="27">
         <f>1.35998010635375/200</f>
         <v>6.7999005317687499E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" s="5" t="s">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A86" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="33">
+      <c r="B86" s="33">
         <v>-12.548</v>
       </c>
-      <c r="C74">
+      <c r="C86">
         <f>2.79346585273742/200</f>
         <v>1.39673292636871E-2</v>
       </c>
-      <c r="D74" s="33">
+      <c r="D86" s="33">
         <v>-12.3985</v>
       </c>
-      <c r="E74" s="27">
+      <c r="E86" s="27">
         <f>2.5887804031372/200</f>
         <v>1.2943902015686E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B75" s="28">
+    <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A87" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B87" s="28">
         <v>-12.0535</v>
       </c>
-      <c r="C75" s="28">
+      <c r="C87" s="28">
         <f>11.7575964927673/200</f>
         <v>5.87879824638365E-2</v>
       </c>
-      <c r="D75" s="28">
+      <c r="D87" s="28">
         <v>-12.076599999999999</v>
       </c>
-      <c r="E75" s="29">
+      <c r="E87" s="29">
         <f>11.3483390808105/200</f>
         <v>5.6741695404052502E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" s="7" t="s">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A90" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A91" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A92" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A82" s="14" t="s">
+    <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A94" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B82" s="43" t="s">
+      <c r="B94" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C82" s="43" t="s">
+      <c r="C94" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="D82" s="43" t="s">
+      <c r="D94" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="E82" s="43" t="s">
+      <c r="E94" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="F82" s="43" t="s">
+      <c r="F94" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="G82" s="58" t="s">
+      <c r="G94" s="52" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A83" s="5" t="s">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A95" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B83" s="9">
+      <c r="B95" s="9">
         <v>2.7021000000000002</v>
       </c>
-      <c r="C83" s="9">
+      <c r="C95" s="9">
         <v>-7.3941999999999997</v>
       </c>
-      <c r="D83" s="9">
+      <c r="D95" s="9">
         <v>-17.366499999999998</v>
       </c>
-      <c r="E83" s="9">
+      <c r="E95" s="9">
         <v>-27.2926</v>
       </c>
-      <c r="F83" s="9">
+      <c r="F95" s="9">
         <v>-37.272500000000001</v>
       </c>
-      <c r="G83" s="34">
+      <c r="G95" s="34">
         <f>1.87291026115417/200</f>
         <v>9.3645513057708501E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A84" s="5" t="s">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A96" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B84" s="9">
+      <c r="B96" s="9">
         <v>0.88500000000000001</v>
       </c>
-      <c r="C84" s="9">
+      <c r="C96" s="9">
         <v>0.90100000000000002</v>
       </c>
-      <c r="D84" s="9">
+      <c r="D96" s="9">
         <v>0.95669999999999999</v>
       </c>
-      <c r="E84" s="9">
+      <c r="E96" s="9">
         <v>0.96560000000000001</v>
       </c>
-      <c r="F84" s="9">
+      <c r="F96" s="9">
         <v>1.0293000000000001</v>
       </c>
-      <c r="G84" s="59"/>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A85" s="5"/>
-      <c r="B85" s="60"/>
-      <c r="C85" s="9"/>
-      <c r="D85" s="9"/>
-      <c r="E85" s="9"/>
-      <c r="F85" s="9"/>
-      <c r="G85" s="59"/>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A86" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B86" s="9">
-        <v>11.153700000000001</v>
-      </c>
-      <c r="C86" s="9">
-        <v>0.92630000000000001</v>
-      </c>
-      <c r="D86" s="9">
-        <v>-9.1595999999999993</v>
-      </c>
-      <c r="E86" s="9">
-        <v>-18.4282</v>
-      </c>
-      <c r="F86" s="9">
-        <v>-28.785699999999999</v>
-      </c>
-      <c r="G86" s="34">
-        <f>1.73989057540893/200</f>
-        <v>8.6994528770446503E-3</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A87" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B87" s="9">
-        <v>3.0234000000000001</v>
-      </c>
-      <c r="C87" s="9">
-        <v>3.0640999999999998</v>
-      </c>
-      <c r="D87" s="9">
-        <v>3.6509</v>
-      </c>
-      <c r="E87" s="9">
-        <v>3.2534000000000001</v>
-      </c>
-      <c r="F87" s="9">
-        <v>3.3008000000000002</v>
-      </c>
-      <c r="G87" s="59"/>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A88" s="5"/>
-      <c r="B88" s="60"/>
-      <c r="C88" s="9"/>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="9"/>
-      <c r="G88" s="59"/>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A89" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B89" s="9">
-        <v>-1.8754</v>
-      </c>
-      <c r="C89" s="9">
-        <v>-11.879799999999999</v>
-      </c>
-      <c r="D89" s="9">
-        <v>-21.812200000000001</v>
-      </c>
-      <c r="E89" s="9">
-        <v>-31.9605</v>
-      </c>
-      <c r="F89" s="9">
-        <v>-41.809899999999999</v>
-      </c>
-      <c r="G89" s="34">
-        <f>3.64388179779052/200</f>
-        <v>1.82194089889526E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A90" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B90" s="9">
-        <v>1.2853000000000001</v>
-      </c>
-      <c r="C90" s="9">
-        <v>1.2719</v>
-      </c>
-      <c r="D90" s="9">
-        <v>1.1487000000000001</v>
-      </c>
-      <c r="E90" s="9">
-        <v>1.2646999999999999</v>
-      </c>
-      <c r="F90" s="9">
-        <v>1.1558999999999999</v>
-      </c>
-      <c r="G90" s="34"/>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A91" s="5"/>
-      <c r="B91" s="60"/>
-      <c r="C91" s="9"/>
-      <c r="D91" s="9"/>
-      <c r="E91" s="9"/>
-      <c r="F91" s="9"/>
-      <c r="G91" s="34"/>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A92" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B92" s="9">
-        <v>5.5016999999999996</v>
-      </c>
-      <c r="C92" s="9">
-        <v>-4.8254000000000001</v>
-      </c>
-      <c r="D92" s="9">
-        <v>-15.061500000000001</v>
-      </c>
-      <c r="E92" s="9">
-        <v>-24.198</v>
-      </c>
-      <c r="F92" s="9">
-        <v>-34.591799999999999</v>
-      </c>
-      <c r="G92" s="34">
-        <f>3.63707900047302/200</f>
-        <v>1.8185395002365098E-2</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A93" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B93" s="9">
-        <v>2.9416000000000002</v>
-      </c>
-      <c r="C93" s="9">
-        <v>3.2046000000000001</v>
-      </c>
-      <c r="D93" s="9">
-        <v>3.4399000000000002</v>
-      </c>
-      <c r="E93" s="9">
-        <v>3.1190000000000002</v>
-      </c>
-      <c r="F93" s="9">
-        <v>3.133</v>
-      </c>
-      <c r="G93" s="59"/>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A94" s="5"/>
-      <c r="B94" s="60"/>
-      <c r="C94" s="60"/>
-      <c r="D94" s="60"/>
-      <c r="E94" s="60"/>
-      <c r="F94" s="60"/>
-      <c r="G94" s="59"/>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A95" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B95" s="9">
-        <f>-1.7902</f>
-        <v>-1.7902</v>
-      </c>
-      <c r="C95" s="9">
-        <v>-11.8467</v>
-      </c>
-      <c r="D95" s="9">
-        <v>-21.738299999999999</v>
-      </c>
-      <c r="E95" s="9">
-        <v>-31.619900000000001</v>
-      </c>
-      <c r="F95" s="9">
-        <v>-41.830800000000004</v>
-      </c>
-      <c r="G95" s="34">
-        <f>43.5942468643188/200</f>
-        <v>0.21797123432159399</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A96" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B96" s="9">
-        <v>1.2419</v>
-      </c>
-      <c r="C96" s="9">
-        <v>1.1898</v>
-      </c>
-      <c r="D96" s="9">
-        <v>1.2814000000000001</v>
-      </c>
-      <c r="E96" s="9">
-        <v>1.1073</v>
-      </c>
-      <c r="F96" s="30">
-        <v>1.2888999999999999</v>
-      </c>
-      <c r="G96" s="34"/>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G96" s="53"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A97" s="5"/>
-      <c r="B97" s="9"/>
+      <c r="B97" s="54"/>
       <c r="C97" s="9"/>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
       <c r="F97" s="9"/>
-      <c r="G97" s="34"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G97" s="53"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A98" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B98" s="9">
-        <v>-0.77390000000000003</v>
+        <v>11.153700000000001</v>
       </c>
       <c r="C98" s="9">
-        <v>-10.8522</v>
+        <v>0.92630000000000001</v>
       </c>
       <c r="D98" s="9">
-        <v>-21.103899999999999</v>
+        <v>-9.1595999999999993</v>
       </c>
       <c r="E98" s="9">
-        <v>-29.667200000000001</v>
+        <v>-18.4282</v>
       </c>
       <c r="F98" s="9">
-        <v>-38.0655</v>
-      </c>
-      <c r="G98" s="34"/>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+        <v>-28.785699999999999</v>
+      </c>
+      <c r="G98" s="34">
+        <f>1.73989057540893/200</f>
+        <v>8.6994528770446503E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A99" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B99" s="9">
-        <v>1.2433000000000001</v>
+        <v>3.0234000000000001</v>
       </c>
       <c r="C99" s="9">
-        <v>1.1579999999999999</v>
+        <v>3.0640999999999998</v>
       </c>
       <c r="D99" s="9">
-        <v>1.2155</v>
+        <v>3.6509</v>
       </c>
       <c r="E99" s="9">
-        <v>1.2145999999999999</v>
+        <v>3.2534000000000001</v>
       </c>
       <c r="F99" s="9">
-        <v>1.1361000000000001</v>
-      </c>
-      <c r="G99" s="34"/>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+        <v>3.3008000000000002</v>
+      </c>
+      <c r="G99" s="53"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A100" s="5"/>
-      <c r="B100" s="9"/>
+      <c r="B100" s="54"/>
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
       <c r="F100" s="9"/>
-      <c r="G100" s="34"/>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G100" s="53"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A101" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B101" s="9">
+        <v>-1.8754</v>
+      </c>
+      <c r="C101" s="9">
+        <v>-11.879799999999999</v>
+      </c>
+      <c r="D101" s="9">
+        <v>-21.812200000000001</v>
+      </c>
+      <c r="E101" s="9">
+        <v>-31.9605</v>
+      </c>
+      <c r="F101" s="9">
+        <v>-41.809899999999999</v>
+      </c>
+      <c r="G101" s="34">
+        <f>3.64388179779052/200</f>
+        <v>1.82194089889526E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A102" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B102" s="9">
+        <v>1.2853000000000001</v>
+      </c>
+      <c r="C102" s="9">
+        <v>1.2719</v>
+      </c>
+      <c r="D102" s="9">
+        <v>1.1487000000000001</v>
+      </c>
+      <c r="E102" s="9">
+        <v>1.2646999999999999</v>
+      </c>
+      <c r="F102" s="9">
+        <v>1.1558999999999999</v>
+      </c>
+      <c r="G102" s="34"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A103" s="5"/>
+      <c r="B103" s="54"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
+      <c r="G103" s="34"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A104" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B104" s="9">
+        <v>5.5016999999999996</v>
+      </c>
+      <c r="C104" s="9">
+        <v>-4.8254000000000001</v>
+      </c>
+      <c r="D104" s="9">
+        <v>-15.061500000000001</v>
+      </c>
+      <c r="E104" s="9">
+        <v>-24.198</v>
+      </c>
+      <c r="F104" s="9">
+        <v>-34.591799999999999</v>
+      </c>
+      <c r="G104" s="34">
+        <f>3.63707900047302/200</f>
+        <v>1.8185395002365098E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A105" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B105" s="9">
+        <v>2.9416000000000002</v>
+      </c>
+      <c r="C105" s="9">
+        <v>3.2046000000000001</v>
+      </c>
+      <c r="D105" s="9">
+        <v>3.4399000000000002</v>
+      </c>
+      <c r="E105" s="9">
+        <v>3.1190000000000002</v>
+      </c>
+      <c r="F105" s="9">
+        <v>3.133</v>
+      </c>
+      <c r="G105" s="53"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A106" s="5"/>
+      <c r="B106" s="54"/>
+      <c r="C106" s="54"/>
+      <c r="D106" s="54"/>
+      <c r="E106" s="54"/>
+      <c r="F106" s="54"/>
+      <c r="G106" s="53"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A107" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B107" s="9">
+        <f>-1.7902</f>
+        <v>-1.7902</v>
+      </c>
+      <c r="C107" s="9">
+        <v>-11.8467</v>
+      </c>
+      <c r="D107" s="9">
+        <v>-21.738299999999999</v>
+      </c>
+      <c r="E107" s="9">
+        <v>-31.619900000000001</v>
+      </c>
+      <c r="F107" s="9">
+        <v>-41.830800000000004</v>
+      </c>
+      <c r="G107" s="34">
+        <f>43.5942468643188/200</f>
+        <v>0.21797123432159399</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A108" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B108" s="9">
+        <v>1.2419</v>
+      </c>
+      <c r="C108" s="9">
+        <v>1.1898</v>
+      </c>
+      <c r="D108" s="9">
+        <v>1.2814000000000001</v>
+      </c>
+      <c r="E108" s="9">
+        <v>1.1073</v>
+      </c>
+      <c r="F108" s="30">
+        <v>1.2888999999999999</v>
+      </c>
+      <c r="G108" s="34"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A109" s="5"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="34"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A110" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B110" s="9">
+        <v>-0.77390000000000003</v>
+      </c>
+      <c r="C110" s="9">
+        <v>-10.8522</v>
+      </c>
+      <c r="D110" s="9">
+        <v>-21.103899999999999</v>
+      </c>
+      <c r="E110" s="9">
+        <v>-29.667200000000001</v>
+      </c>
+      <c r="F110" s="9">
+        <v>-38.0655</v>
+      </c>
+      <c r="G110" s="34"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A111" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B111" s="9">
+        <v>1.2433000000000001</v>
+      </c>
+      <c r="C111" s="9">
+        <v>1.1579999999999999</v>
+      </c>
+      <c r="D111" s="9">
+        <v>1.2155</v>
+      </c>
+      <c r="E111" s="9">
+        <v>1.2145999999999999</v>
+      </c>
+      <c r="F111" s="9">
+        <v>1.1361000000000001</v>
+      </c>
+      <c r="G111" s="34"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A112" s="5"/>
+      <c r="B112" s="9"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="34"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A113" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B101" s="9">
+      <c r="B113" s="9">
         <v>-1.7432000000000001</v>
       </c>
-      <c r="C101" s="9">
+      <c r="C113" s="9">
         <v>-11.6966</v>
       </c>
-      <c r="D101" s="9">
+      <c r="D113" s="9">
         <v>-21.720500000000001</v>
       </c>
-      <c r="E101" s="9">
+      <c r="E113" s="9">
         <v>-31.185500000000001</v>
       </c>
-      <c r="F101" s="9">
+      <c r="F113" s="9">
         <v>-40.300899999999999</v>
       </c>
-      <c r="G101" s="34"/>
-    </row>
-    <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="6" t="s">
+      <c r="G113" s="34"/>
+    </row>
+    <row r="114" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A114" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B102" s="35">
+      <c r="B114" s="35">
         <v>1.2693000000000001</v>
       </c>
-      <c r="C102" s="35">
+      <c r="C114" s="35">
         <v>1.2414000000000001</v>
       </c>
-      <c r="D102" s="35">
+      <c r="D114" s="35">
         <v>1.1528</v>
       </c>
-      <c r="E102" s="35">
+      <c r="E114" s="35">
         <v>1.2195</v>
       </c>
-      <c r="F102" s="35">
+      <c r="F114" s="35">
         <v>1.1687000000000001</v>
       </c>
-      <c r="G102" s="36"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A103" s="25"/>
-      <c r="B103" s="18"/>
-      <c r="C103" s="18"/>
-      <c r="D103" s="18"/>
-      <c r="E103" s="18"/>
-      <c r="F103" s="18"/>
-      <c r="G103" s="18"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A104" s="37"/>
-      <c r="B104" s="37" t="s">
+      <c r="G114" s="36"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A115" s="25"/>
+      <c r="B115" s="18"/>
+      <c r="C115" s="18"/>
+      <c r="D115" s="18"/>
+      <c r="E115" s="18"/>
+      <c r="F115" s="18"/>
+      <c r="G115" s="18"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A116" s="37"/>
+      <c r="B116" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="D116" s="18"/>
+      <c r="E116" s="18"/>
+      <c r="F116" s="18"/>
+      <c r="G116" s="18"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A117" s="25"/>
+      <c r="B117" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="D104" s="18"/>
-      <c r="E104" s="18"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="18"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A105" s="25"/>
-      <c r="B105" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C105" s="22"/>
-      <c r="D105" s="18"/>
-      <c r="E105" s="18"/>
-      <c r="F105" s="18"/>
-      <c r="G105" s="18"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A108" s="7" t="s">
+      <c r="C117" s="22"/>
+      <c r="D117" s="18"/>
+      <c r="E117" s="18"/>
+      <c r="F117" s="18"/>
+      <c r="G117" s="18"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A120" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C108" s="23"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A109" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A110" t="s">
+      <c r="C120" s="23"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A122" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A112" s="14" t="s">
+    <row r="123" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A124" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B112" s="15" t="s">
+      <c r="B124" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C112" s="15" t="s">
+      <c r="C124" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D112" s="15" t="s">
+      <c r="D124" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E112" s="15" t="s">
+      <c r="E124" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F112" s="15" t="s">
+      <c r="F124" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G112" s="16" t="s">
+      <c r="G124" s="16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A113" s="5" t="s">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A125" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B113" s="22"/>
-      <c r="C113" s="22"/>
-      <c r="D113" s="22"/>
-      <c r="E113" s="22"/>
-      <c r="F113" s="22"/>
-      <c r="G113" s="8"/>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A114" s="5" t="s">
+      <c r="B125" s="22"/>
+      <c r="C125" s="22"/>
+      <c r="D125" s="22"/>
+      <c r="E125" s="22"/>
+      <c r="F125" s="22"/>
+      <c r="G125" s="8"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A126" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B114" s="22"/>
-      <c r="C114" s="22"/>
-      <c r="D114" s="22"/>
-      <c r="E114" s="22"/>
-      <c r="F114" s="22"/>
-      <c r="G114" s="19"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A115" s="5"/>
-      <c r="B115" s="18"/>
-      <c r="C115" s="22"/>
-      <c r="D115" s="22"/>
-      <c r="E115" s="22"/>
-      <c r="F115" s="22"/>
-      <c r="G115" s="19"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A116" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B116" s="22"/>
-      <c r="C116" s="22"/>
-      <c r="D116" s="22"/>
-      <c r="E116" s="22"/>
-      <c r="F116" s="22"/>
-      <c r="G116" s="8"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A117" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B117" s="22"/>
-      <c r="C117" s="22"/>
-      <c r="D117" s="22"/>
-      <c r="E117" s="22"/>
-      <c r="F117" s="22"/>
-      <c r="G117" s="19"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A118" s="5"/>
-      <c r="B118" s="18"/>
-      <c r="C118" s="22"/>
-      <c r="D118" s="22"/>
-      <c r="E118" s="22"/>
-      <c r="F118" s="22"/>
-      <c r="G118" s="19"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A119" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B119" s="22"/>
-      <c r="C119" s="22"/>
-      <c r="D119" s="22"/>
-      <c r="E119" s="22"/>
-      <c r="F119" s="22"/>
-      <c r="G119" s="8"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A120" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B120" s="22"/>
-      <c r="C120" s="22"/>
-      <c r="D120" s="22"/>
-      <c r="E120" s="22"/>
-      <c r="F120" s="22"/>
-      <c r="G120" s="8"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A121" s="5"/>
-      <c r="B121" s="18"/>
-      <c r="C121" s="22"/>
-      <c r="D121" s="22"/>
-      <c r="E121" s="22"/>
-      <c r="F121" s="22"/>
-      <c r="G121" s="8"/>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A122" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B122" s="22"/>
-      <c r="C122" s="22"/>
-      <c r="D122" s="22"/>
-      <c r="E122" s="22"/>
-      <c r="F122" s="22"/>
-      <c r="G122" s="8"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A123" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B123" s="22"/>
-      <c r="C123" s="22"/>
-      <c r="D123" s="22"/>
-      <c r="E123" s="22"/>
-      <c r="F123" s="22"/>
-      <c r="G123" s="19"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A124" s="5"/>
-      <c r="B124" s="18"/>
-      <c r="C124" s="18"/>
-      <c r="D124" s="18"/>
-      <c r="E124" s="18"/>
-      <c r="F124" s="18"/>
-      <c r="G124" s="19"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A125" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B125" s="18"/>
-      <c r="C125" s="18"/>
-      <c r="D125" s="18"/>
-      <c r="E125" s="18"/>
-      <c r="F125" s="18"/>
-      <c r="G125" s="19"/>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A126" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B126" s="18"/>
-      <c r="C126" s="18"/>
-      <c r="D126" s="18"/>
-      <c r="E126" s="18"/>
-      <c r="F126" s="18"/>
+      <c r="B126" s="22"/>
+      <c r="C126" s="22"/>
+      <c r="D126" s="22"/>
+      <c r="E126" s="22"/>
+      <c r="F126" s="22"/>
       <c r="G126" s="19"/>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A127" s="5"/>
       <c r="B127" s="18"/>
-      <c r="C127" s="18"/>
-      <c r="D127" s="18"/>
-      <c r="E127" s="18"/>
-      <c r="F127" s="18"/>
+      <c r="C127" s="22"/>
+      <c r="D127" s="22"/>
+      <c r="E127" s="22"/>
+      <c r="F127" s="22"/>
       <c r="G127" s="19"/>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A128" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B128" s="18"/>
-      <c r="C128" s="18"/>
-      <c r="D128" s="18"/>
-      <c r="E128" s="18"/>
-      <c r="F128" s="18"/>
-      <c r="G128" s="19"/>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+      <c r="B128" s="22"/>
+      <c r="C128" s="22"/>
+      <c r="D128" s="22"/>
+      <c r="E128" s="22"/>
+      <c r="F128" s="22"/>
+      <c r="G128" s="8"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A129" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B129" s="18"/>
-      <c r="C129" s="18"/>
-      <c r="D129" s="18"/>
-      <c r="E129" s="18"/>
-      <c r="F129" s="18"/>
+        <v>37</v>
+      </c>
+      <c r="B129" s="22"/>
+      <c r="C129" s="22"/>
+      <c r="D129" s="22"/>
+      <c r="E129" s="22"/>
+      <c r="F129" s="22"/>
       <c r="G129" s="19"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A130" s="5"/>
       <c r="B130" s="18"/>
-      <c r="C130" s="18"/>
-      <c r="D130" s="18"/>
-      <c r="E130" s="18"/>
-      <c r="F130" s="18"/>
+      <c r="C130" s="22"/>
+      <c r="D130" s="22"/>
+      <c r="E130" s="22"/>
+      <c r="F130" s="22"/>
       <c r="G130" s="19"/>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A131" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B131" s="22"/>
+      <c r="C131" s="22"/>
+      <c r="D131" s="22"/>
+      <c r="E131" s="22"/>
+      <c r="F131" s="22"/>
+      <c r="G131" s="8"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A132" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B132" s="22"/>
+      <c r="C132" s="22"/>
+      <c r="D132" s="22"/>
+      <c r="E132" s="22"/>
+      <c r="F132" s="22"/>
+      <c r="G132" s="8"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A133" s="5"/>
+      <c r="B133" s="18"/>
+      <c r="C133" s="22"/>
+      <c r="D133" s="22"/>
+      <c r="E133" s="22"/>
+      <c r="F133" s="22"/>
+      <c r="G133" s="8"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A134" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B134" s="22"/>
+      <c r="C134" s="22"/>
+      <c r="D134" s="22"/>
+      <c r="E134" s="22"/>
+      <c r="F134" s="22"/>
+      <c r="G134" s="8"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A135" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B135" s="22"/>
+      <c r="C135" s="22"/>
+      <c r="D135" s="22"/>
+      <c r="E135" s="22"/>
+      <c r="F135" s="22"/>
+      <c r="G135" s="19"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A136" s="5"/>
+      <c r="B136" s="18"/>
+      <c r="C136" s="18"/>
+      <c r="D136" s="18"/>
+      <c r="E136" s="18"/>
+      <c r="F136" s="18"/>
+      <c r="G136" s="19"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A137" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B137" s="18"/>
+      <c r="C137" s="18"/>
+      <c r="D137" s="18"/>
+      <c r="E137" s="18"/>
+      <c r="F137" s="18"/>
+      <c r="G137" s="19"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A138" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B138" s="18"/>
+      <c r="C138" s="18"/>
+      <c r="D138" s="18"/>
+      <c r="E138" s="18"/>
+      <c r="F138" s="18"/>
+      <c r="G138" s="19"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A139" s="5"/>
+      <c r="B139" s="18"/>
+      <c r="C139" s="18"/>
+      <c r="D139" s="18"/>
+      <c r="E139" s="18"/>
+      <c r="F139" s="18"/>
+      <c r="G139" s="19"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A140" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B140" s="18"/>
+      <c r="C140" s="18"/>
+      <c r="D140" s="18"/>
+      <c r="E140" s="18"/>
+      <c r="F140" s="18"/>
+      <c r="G140" s="19"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A141" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B141" s="18"/>
+      <c r="C141" s="18"/>
+      <c r="D141" s="18"/>
+      <c r="E141" s="18"/>
+      <c r="F141" s="18"/>
+      <c r="G141" s="19"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A142" s="5"/>
+      <c r="B142" s="18"/>
+      <c r="C142" s="18"/>
+      <c r="D142" s="18"/>
+      <c r="E142" s="18"/>
+      <c r="F142" s="18"/>
+      <c r="G142" s="19"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A143" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B131" s="18"/>
-      <c r="C131" s="18"/>
-      <c r="D131" s="18"/>
-      <c r="E131" s="18"/>
-      <c r="F131" s="18"/>
-      <c r="G131" s="19"/>
-    </row>
-    <row r="132" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A132" s="6" t="s">
+      <c r="B143" s="18"/>
+      <c r="C143" s="18"/>
+      <c r="D143" s="18"/>
+      <c r="E143" s="18"/>
+      <c r="F143" s="18"/>
+      <c r="G143" s="19"/>
+    </row>
+    <row r="144" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A144" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B132" s="20"/>
-      <c r="C132" s="20"/>
-      <c r="D132" s="20"/>
-      <c r="E132" s="20"/>
-      <c r="F132" s="20"/>
-      <c r="G132" s="21"/>
+      <c r="B144" s="20"/>
+      <c r="C144" s="20"/>
+      <c r="D144" s="20"/>
+      <c r="E144" s="20"/>
+      <c r="F144" s="20"/>
+      <c r="G144" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -2722,30 +2940,30 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="37.1796875" customWidth="1"/>
-    <col min="4" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.15234375" customWidth="1"/>
+    <col min="4" max="6" width="11.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>53</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>5</v>
@@ -2757,9 +2975,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="25">
         <v>-10.4223</v>
@@ -2774,16 +2992,16 @@
         <v>-40.424100000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="5"/>
       <c r="B5" s="25"/>
       <c r="C5" s="25"/>
       <c r="D5" s="25"/>
       <c r="E5" s="27"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="25">
         <v>-13.8728</v>
@@ -2798,16 +3016,16 @@
         <v>-43.958799999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7" s="5"/>
       <c r="B7" s="25"/>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
       <c r="E7" s="27"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="25">
         <v>-9.6765000000000008</v>
@@ -2822,16 +3040,16 @@
         <v>-17.808599999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9" s="5"/>
       <c r="B9" s="25"/>
       <c r="C9" s="25"/>
       <c r="D9" s="25"/>
       <c r="E9" s="27"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="25">
         <v>-13.1538</v>
@@ -2846,16 +3064,16 @@
         <v>-21.748200000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11" s="5"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
       <c r="E11" s="27"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="25">
         <v>-13.4038</v>
@@ -2870,9 +3088,9 @@
         <v>-42.509599999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="28">
         <v>-12.888500000000001</v>
@@ -2887,42 +3105,42 @@
         <v>-36.738900000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="14"/>
       <c r="B17" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="5" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
-        <v>63</v>
       </c>
       <c r="B18" s="27">
         <v>0.30146958000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A19" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="27">
         <v>0.61430751900000002</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="29">
         <v>0.39500000000000002</v>

</xml_diff>

<commit_message>
update multipass with H=I since 2nd iteration
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\RTSNet_Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9323F5F9-A6EE-4B7A-88D9-C4ABC64013C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C89DB7E-8B65-40F6-82DE-D39C9AC87CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="186">
   <si>
     <t>N_E=1000, N_CV=100, N_T=200</t>
   </si>
@@ -542,9 +542,6 @@
     <t>2) Decimation (change data:6.7 mark red)</t>
   </si>
   <si>
-    <t>On our dataset: (On Welling's dataset: -15.346)</t>
-  </si>
-  <si>
     <t>ERTS J=5 std, optimized q [dB]</t>
   </si>
   <si>
@@ -587,12 +584,6 @@
     <t>h(x) returns spherical coordinates of x</t>
   </si>
   <si>
-    <t>Training time：</t>
-  </si>
-  <si>
-    <t>3) NL observation (change date 6.22)</t>
-  </si>
-  <si>
     <t>[0, 0]</t>
   </si>
   <si>
@@ -606,6 +597,12 @@
   </si>
   <si>
     <t>T=20, v = 0 dB</t>
+  </si>
+  <si>
+    <t>On our dataset: -8.47414493560791</t>
+  </si>
+  <si>
+    <t>3) NL observation (change date 6.23)</t>
   </si>
 </sst>
 </file>
@@ -4302,7 +4299,7 @@
   <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="F90" sqref="F90"/>
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4314,7 +4311,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -4334,28 +4331,28 @@
       <c r="A4" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="48" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" s="63">
         <v>10.016999999999999</v>
@@ -4782,7 +4779,7 @@
         <v>40</v>
       </c>
       <c r="H34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -4823,7 +4820,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C37" s="19">
         <v>0.19120000000000001</v>
@@ -4891,7 +4888,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C41" s="19">
         <v>0.19500000000000001</v>
@@ -4959,7 +4956,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C47" s="19">
         <v>-2.3424</v>
@@ -4984,7 +4981,7 @@
         <v>119</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G49" s="23"/>
       <c r="H49" s="19">
@@ -5003,10 +5000,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G51" s="23"/>
       <c r="H51" s="19">
@@ -5029,19 +5026,17 @@
       </c>
       <c r="B53" s="24"/>
       <c r="C53" s="103" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="D53" s="24"/>
       <c r="E53" s="24"/>
       <c r="F53" s="24"/>
       <c r="G53" s="25"/>
       <c r="H53" s="19">
-        <f>122.040362358093/5</f>
-        <v>24.408072471618603</v>
-      </c>
-      <c r="I53" s="19" t="s">
-        <v>180</v>
-      </c>
+        <f>254.527338504791/10</f>
+        <v>25.452733850479099</v>
+      </c>
+      <c r="I53" s="19"/>
     </row>
     <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
@@ -5186,12 +5181,12 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B75" t="s">
         <v>0</v>
@@ -5199,7 +5194,7 @@
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
@@ -5210,24 +5205,24 @@
         <v>50</v>
       </c>
       <c r="C77" s="37" t="s">
+        <v>179</v>
+      </c>
+      <c r="D77" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="E77" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="F77" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="D77" s="37" t="s">
-        <v>183</v>
-      </c>
-      <c r="E77" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="F77" s="48" t="s">
-        <v>185</v>
-      </c>
       <c r="G77" s="33" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B78" s="9">
         <v>6.5773000000000001</v>
@@ -5361,7 +5356,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B84" s="63"/>
       <c r="C84" s="101"/>
@@ -5381,7 +5376,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B86" s="63"/>
       <c r="C86" s="101"/>
@@ -5410,11 +5405,13 @@
         <v>10.8035</v>
       </c>
       <c r="D88" s="101">
-        <v>-7.6268000000000002</v>
-      </c>
-      <c r="E88" s="101"/>
+        <v>-8.0739999999999998</v>
+      </c>
+      <c r="E88" s="101">
+        <v>-17.941099999999999</v>
+      </c>
       <c r="F88" s="105">
-        <v>-27.412500000000001</v>
+        <v>-27.419599999999999</v>
       </c>
       <c r="G88">
         <f>12.0926365852355/200</f>
@@ -5432,16 +5429,18 @@
         <v>8.9991000000000003</v>
       </c>
       <c r="D89" s="101">
-        <v>1.6476999999999999</v>
-      </c>
-      <c r="E89" s="101"/>
+        <v>1.4996</v>
+      </c>
+      <c r="E89" s="101">
+        <v>1.7119</v>
+      </c>
       <c r="F89" s="105">
-        <v>1.5172000000000001</v>
+        <v>1.5708</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B90" s="9"/>
       <c r="C90" s="101"/>

</xml_diff>

<commit_message>
test LMMSE of h
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\RTSNet_Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C89DB7E-8B65-40F6-82DE-D39C9AC87CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75806A9B-37ED-421B-A012-505CA8D55F80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="17020" windowHeight="10120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="187">
   <si>
     <t>N_E=1000, N_CV=100, N_T=200</t>
   </si>
@@ -602,7 +602,10 @@
     <t>On our dataset: -8.47414493560791</t>
   </si>
   <si>
-    <t>3) NL observation (change date 6.23)</t>
+    <t xml:space="preserve">RTSNet 2pass[dB] </t>
+  </si>
+  <si>
+    <t>3) NL observation (change date 6.29)</t>
   </si>
 </sst>
 </file>
@@ -4296,10 +4299,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FAE463-692A-4AB1-8AB9-770196756CC0}">
-  <dimension ref="A1:I92"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5181,7 +5184,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
@@ -5440,30 +5443,58 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
-        <v>177</v>
+        <v>185</v>
       </c>
       <c r="B90" s="9"/>
       <c r="C90" s="101"/>
       <c r="D90" s="101"/>
       <c r="E90" s="101"/>
-      <c r="F90" s="105"/>
-    </row>
-    <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="6" t="s">
+      <c r="F90" s="105">
+        <v>-27.6053</v>
+      </c>
+      <c r="G90">
+        <f>23.5590772628784/200</f>
+        <v>0.117795386314392</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B91" s="31"/>
-      <c r="C91" s="107"/>
-      <c r="D91" s="107"/>
-      <c r="E91" s="107"/>
-      <c r="F91" s="106"/>
+      <c r="B91" s="9"/>
+      <c r="C91" s="101"/>
+      <c r="D91" s="101"/>
+      <c r="E91" s="101"/>
+      <c r="F91" s="105">
+        <v>1.5587</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A92" s="21"/>
-      <c r="B92" s="21"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="21"/>
-      <c r="E92" s="21"/>
+      <c r="A92" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B92" s="9"/>
+      <c r="C92" s="101"/>
+      <c r="D92" s="101"/>
+      <c r="E92" s="101"/>
+      <c r="F92" s="105"/>
+    </row>
+    <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B93" s="31"/>
+      <c r="C93" s="107"/>
+      <c r="D93" s="107"/>
+      <c r="E93" s="107"/>
+      <c r="F93" s="106"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A94" s="21"/>
+      <c r="B94" s="21"/>
+      <c r="C94" s="21"/>
+      <c r="D94" s="21"/>
+      <c r="E94" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
test random length linear for vanilla
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\RTSNet_Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA69B9B-5881-41DD-99A8-4AB6E5C7C084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338902AB-0A30-4EC3-AAB9-2CA09808BAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="17020" windowHeight="10120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="208">
   <si>
     <t>N_E=1000, N_CV=100, N_T=200</t>
   </si>
@@ -309,9 +309,6 @@
     <t>RTSNet partial(F = I) (n_Epochs=2000, n_Batch=1, learningRate=1E-3, weightDecay=1E-9)[dB]</t>
   </si>
   <si>
-    <t xml:space="preserve">2) Gneralization </t>
-  </si>
-  <si>
     <t>Generalization to Random initial conditions(x1 and x2 both uniformly distributed on [0,100) )</t>
   </si>
   <si>
@@ -502,9 +499,6 @@
   </si>
   <si>
     <t>concat RTS(using the -8.1674 as input) [dB]</t>
-  </si>
-  <si>
-    <t>H = H_rot1</t>
   </si>
   <si>
     <t>EKF  partial(H=I) [dB]</t>
@@ -644,10 +638,37 @@
     <t>N_T = 100, m=n=3, T=500, q=-inf</t>
   </si>
   <si>
-    <t>Check Jacobian for linear H(not I)</t>
-  </si>
-  <si>
     <t>prior: truex+q</t>
+  </si>
+  <si>
+    <t>Check Jacobian for linear H(not I): Good</t>
+  </si>
+  <si>
+    <t>H = I_rot1</t>
+  </si>
+  <si>
+    <t>N_T = 200, m=n=3, T=100 (same dataset as 1) obs mismatch and 3) NL obs )</t>
+  </si>
+  <si>
+    <t>Linear H = I_rot1 [dB]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">r,q =[0,0] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">r,q =[0,20] </t>
+  </si>
+  <si>
+    <t>h^-1 method</t>
+  </si>
+  <si>
+    <t>2) Gneralization (change date 7.7)</t>
+  </si>
+  <si>
+    <t>Vanilla [dB]</t>
+  </si>
+  <si>
+    <t>Hybrid [dB]</t>
   </si>
 </sst>
 </file>
@@ -727,7 +748,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -767,6 +788,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -863,7 +896,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1137,6 +1170,16 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1417,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K191"/>
+  <dimension ref="A1:K195"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="E187" sqref="E187"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1511,7 +1554,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B7" s="9">
         <v>8.0853999999999999</v>
@@ -1713,7 +1756,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18" s="9">
         <v>5.2991000000000001</v>
@@ -1914,7 +1957,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B29" s="9">
         <v>2.7555999999999998</v>
@@ -2067,8 +2110,8 @@
       <c r="G36" s="18"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" s="62" t="s">
-        <v>90</v>
+      <c r="A37" s="128" t="s">
+        <v>205</v>
       </c>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -2116,7 +2159,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B41" s="18"/>
       <c r="C41" s="18">
@@ -2189,2211 +2232,2255 @@
         <v>1.4883784604072552</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="13" t="s">
+    <row r="46" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10">
+      <c r="B46" s="18"/>
+      <c r="C46" s="18">
         <v>0.44900000000000001</v>
       </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10"/>
-      <c r="G46" s="11"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" s="18"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
+      <c r="A47" s="129" t="s">
+        <v>206</v>
+      </c>
+      <c r="B47" s="130"/>
+      <c r="C47" s="130"/>
+      <c r="D47" s="130"/>
+      <c r="E47" s="130"/>
+      <c r="F47" s="130"/>
+      <c r="G47" s="131"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A48" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48" s="18"/>
-      <c r="C48" s="18"/>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-    </row>
-    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
-      <c r="D49" s="18"/>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="18"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50" s="20"/>
-      <c r="C50" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="4" t="s">
-        <v>79</v>
-      </c>
+      <c r="A48" s="129" t="s">
+        <v>155</v>
+      </c>
+      <c r="B48" s="130"/>
+      <c r="C48" s="130"/>
+      <c r="D48" s="130"/>
+      <c r="E48" s="130"/>
+      <c r="F48" s="130"/>
+      <c r="G48" s="131"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A49" s="129" t="s">
+        <v>207</v>
+      </c>
+      <c r="B49" s="130"/>
+      <c r="C49" s="130"/>
+      <c r="D49" s="130"/>
+      <c r="E49" s="130"/>
+      <c r="F49" s="130"/>
+      <c r="G49" s="131"/>
+    </row>
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A50" s="132" t="s">
+        <v>155</v>
+      </c>
+      <c r="B50" s="133"/>
+      <c r="C50" s="133"/>
+      <c r="D50" s="133"/>
+      <c r="E50" s="133"/>
+      <c r="F50" s="133"/>
+      <c r="G50" s="134"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A51" s="12" t="s">
-        <v>146</v>
-      </c>
+      <c r="A51" s="18"/>
       <c r="B51" s="18"/>
-      <c r="C51" s="18">
-        <v>-7.2404999999999999</v>
-      </c>
+      <c r="C51" s="18"/>
       <c r="D51" s="18"/>
       <c r="E51" s="18"/>
       <c r="F51" s="18"/>
-      <c r="G51" s="8">
-        <f>9.09574961662292/200</f>
-        <v>4.5478748083114598E-2</v>
-      </c>
+      <c r="G51" s="18"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A52" s="12" t="s">
-        <v>77</v>
+      <c r="A52" s="17" t="s">
+        <v>80</v>
       </c>
       <c r="B52" s="18"/>
-      <c r="C52" s="18">
-        <v>0.54310000000000003</v>
-      </c>
+      <c r="C52" s="18"/>
       <c r="D52" s="18"/>
       <c r="E52" s="18"/>
       <c r="F52" s="18"/>
-      <c r="G52" s="8"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A53" s="12" t="s">
-        <v>7</v>
+      <c r="G52" s="18"/>
+    </row>
+    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A53" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="B53" s="18"/>
-      <c r="C53" s="18">
-        <v>-11.852600000000001</v>
-      </c>
+      <c r="C53" s="18"/>
       <c r="D53" s="18"/>
       <c r="E53" s="18"/>
       <c r="F53" s="18"/>
-      <c r="G53" s="8">
-        <f>19.0591733455657/200</f>
-        <v>9.5295866727828499E-2</v>
-      </c>
+      <c r="G53" s="18"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A54" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="18">
-        <v>0.68740000000000001</v>
-      </c>
-      <c r="D54" s="18"/>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="8"/>
+      <c r="A54" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="20"/>
+      <c r="C54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="B55" s="18"/>
       <c r="C55" s="18">
-        <v>-11.773</v>
+        <v>-7.2404999999999999</v>
       </c>
       <c r="D55" s="18"/>
       <c r="E55" s="18"/>
       <c r="F55" s="18"/>
       <c r="G55" s="8">
-        <f>221.406227111816/200</f>
-        <v>1.1070311355590801</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B56" s="10"/>
-      <c r="C56" s="10">
-        <v>0.68469999999999998</v>
-      </c>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="11"/>
+        <f>9.09574961662292/200</f>
+        <v>4.5478748083114598E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18">
+        <v>0.54310000000000003</v>
+      </c>
+      <c r="D56" s="18"/>
+      <c r="E56" s="18"/>
+      <c r="F56" s="18"/>
+      <c r="G56" s="8"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A57" s="18"/>
+      <c r="A57" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
+      <c r="C57" s="18">
+        <v>-11.852600000000001</v>
+      </c>
       <c r="D57" s="18"/>
       <c r="E57" s="18"/>
       <c r="F57" s="18"/>
-      <c r="G57" s="18"/>
+      <c r="G57" s="8">
+        <f>19.0591733455657/200</f>
+        <v>9.5295866727828499E-2</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A58" s="17" t="s">
-        <v>91</v>
+      <c r="A58" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
+      <c r="C58" s="18">
+        <v>0.68740000000000001</v>
+      </c>
       <c r="D58" s="18"/>
       <c r="E58" s="18"/>
       <c r="F58" s="18"/>
-      <c r="G58" s="18"/>
-    </row>
-    <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="18" t="s">
-        <v>36</v>
+      <c r="G58" s="8"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="B59" s="18"/>
-      <c r="C59" s="18"/>
+      <c r="C59" s="18">
+        <v>-11.773</v>
+      </c>
       <c r="D59" s="18"/>
       <c r="E59" s="18"/>
       <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A60" s="2" t="s">
+      <c r="G59" s="8">
+        <f>221.406227111816/200</f>
+        <v>1.1070311355590801</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A60" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" s="10"/>
+      <c r="C60" s="10">
+        <v>0.68469999999999998</v>
+      </c>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="11"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" s="18"/>
+      <c r="B61" s="18"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="18"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
+      <c r="G61" s="18"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62" s="18"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+      <c r="E62" s="18"/>
+      <c r="F62" s="18"/>
+      <c r="G62" s="18"/>
+    </row>
+    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
+      <c r="G63" s="18"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B60" s="20"/>
-      <c r="C60" s="22" t="s">
+      <c r="B64" s="20"/>
+      <c r="C64" s="22" t="s">
         <v>3</v>
-      </c>
-      <c r="D60" s="18"/>
-      <c r="E60" s="35"/>
-      <c r="F60" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="G60" s="47">
-        <v>30.081099999999999</v>
-      </c>
-      <c r="H60" s="36"/>
-      <c r="I60" s="33"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A61" s="51" t="s">
-        <v>69</v>
-      </c>
-      <c r="B61" s="18"/>
-      <c r="C61" s="52">
-        <v>-1.0999999999999999E-2</v>
-      </c>
-      <c r="D61" s="18"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G61" s="8">
-        <v>26.237500000000001</v>
-      </c>
-      <c r="H61" s="36"/>
-      <c r="I61" s="33"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A62" s="51" t="s">
-        <v>70</v>
-      </c>
-      <c r="B62" s="18"/>
-      <c r="C62" s="52">
-        <v>0.3891</v>
-      </c>
-      <c r="D62" s="18"/>
-      <c r="E62" s="35"/>
-      <c r="F62" s="59"/>
-      <c r="G62" s="60"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="33"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A63" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="B63" s="18"/>
-      <c r="C63" s="30">
-        <v>-7.2916999999999996</v>
-      </c>
-      <c r="D63" s="18"/>
-      <c r="E63" s="35"/>
-      <c r="F63" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G63" s="8">
-        <v>-6.7626999999999997</v>
-      </c>
-      <c r="H63" s="9"/>
-      <c r="I63" s="33"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A64" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="B64" s="18"/>
-      <c r="C64" s="30">
-        <v>0.90980000000000005</v>
       </c>
       <c r="D64" s="18"/>
       <c r="E64" s="35"/>
-      <c r="F64" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G64" s="8">
-        <v>0.88480000000000003</v>
-      </c>
-      <c r="H64" s="9"/>
+      <c r="F64" s="46" t="s">
+        <v>146</v>
+      </c>
+      <c r="G64" s="47">
+        <v>30.081099999999999</v>
+      </c>
+      <c r="H64" s="36"/>
       <c r="I64" s="33"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A65" s="12" t="s">
-        <v>74</v>
+      <c r="A65" s="51" t="s">
+        <v>69</v>
       </c>
       <c r="B65" s="18"/>
-      <c r="C65" s="30">
-        <v>-11.7737</v>
+      <c r="C65" s="52">
+        <v>-1.0999999999999999E-2</v>
       </c>
       <c r="D65" s="18"/>
       <c r="E65" s="35"/>
       <c r="F65" s="12" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="G65" s="8">
-        <v>-11.523199999999999</v>
-      </c>
-      <c r="H65" s="9"/>
+        <v>26.237500000000001</v>
+      </c>
+      <c r="H65" s="36"/>
       <c r="I65" s="33"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A66" s="12" t="s">
-        <v>53</v>
+      <c r="A66" s="51" t="s">
+        <v>70</v>
       </c>
       <c r="B66" s="18"/>
-      <c r="C66" s="30">
-        <v>1.2115</v>
+      <c r="C66" s="52">
+        <v>0.3891</v>
       </c>
       <c r="D66" s="18"/>
       <c r="E66" s="35"/>
-      <c r="F66" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G66" s="8">
-        <v>1.1852</v>
-      </c>
-      <c r="H66" s="9"/>
+      <c r="F66" s="59"/>
+      <c r="G66" s="60"/>
+      <c r="H66" s="36"/>
       <c r="I66" s="33"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A67" s="53" t="s">
-        <v>71</v>
-      </c>
-      <c r="B67" s="35"/>
-      <c r="C67" s="54">
-        <v>-11.471500000000001</v>
+      <c r="A67" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" s="18"/>
+      <c r="C67" s="30">
+        <v>-7.2916999999999996</v>
       </c>
       <c r="D67" s="18"/>
-      <c r="E67" s="33"/>
+      <c r="E67" s="35"/>
       <c r="F67" s="12" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="G67" s="8">
-        <v>9.0884</v>
-      </c>
-      <c r="H67" s="35"/>
+        <v>-6.7626999999999997</v>
+      </c>
+      <c r="H67" s="9"/>
       <c r="I67" s="33"/>
     </row>
-    <row r="68" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="53" t="s">
-        <v>55</v>
-      </c>
-      <c r="B68" s="35"/>
-      <c r="C68" s="54">
-        <v>1.2063999999999999</v>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A68" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B68" s="18"/>
+      <c r="C68" s="30">
+        <v>0.90980000000000005</v>
       </c>
       <c r="D68" s="18"/>
       <c r="E68" s="35"/>
-      <c r="F68" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G68" s="11">
-        <v>2.7212000000000001</v>
-      </c>
-      <c r="H68" s="35"/>
+      <c r="F68" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G68" s="8">
+        <v>0.88480000000000003</v>
+      </c>
+      <c r="H68" s="9"/>
       <c r="I68" s="33"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A69" s="53" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" s="35"/>
-      <c r="C69" s="55">
-        <v>-11.5383</v>
+      <c r="A69" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" s="18"/>
+      <c r="C69" s="30">
+        <v>-11.7737</v>
       </c>
       <c r="D69" s="18"/>
       <c r="E69" s="35"/>
-      <c r="F69" s="35"/>
-      <c r="G69" s="35"/>
-      <c r="H69" s="35"/>
+      <c r="F69" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G69" s="8">
+        <v>-11.523199999999999</v>
+      </c>
+      <c r="H69" s="9"/>
       <c r="I69" s="33"/>
     </row>
-    <row r="70" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="56" t="s">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A70" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B70" s="18"/>
+      <c r="C70" s="30">
+        <v>1.2115</v>
+      </c>
+      <c r="D70" s="18"/>
+      <c r="E70" s="35"/>
+      <c r="F70" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G70" s="8">
+        <v>1.1852</v>
+      </c>
+      <c r="H70" s="9"/>
+      <c r="I70" s="33"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A71" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" s="35"/>
+      <c r="C71" s="54">
+        <v>-11.471500000000001</v>
+      </c>
+      <c r="D71" s="18"/>
+      <c r="E71" s="33"/>
+      <c r="F71" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G71" s="8">
+        <v>9.0884</v>
+      </c>
+      <c r="H71" s="35"/>
+      <c r="I71" s="33"/>
+    </row>
+    <row r="72" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A72" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B72" s="35"/>
+      <c r="C72" s="54">
+        <v>1.2063999999999999</v>
+      </c>
+      <c r="D72" s="18"/>
+      <c r="E72" s="35"/>
+      <c r="F72" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B70" s="57"/>
-      <c r="C70" s="58">
+      <c r="G72" s="11">
+        <v>2.7212000000000001</v>
+      </c>
+      <c r="H72" s="35"/>
+      <c r="I72" s="33"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A73" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73" s="35"/>
+      <c r="C73" s="55">
+        <v>-11.5383</v>
+      </c>
+      <c r="D73" s="18"/>
+      <c r="E73" s="35"/>
+      <c r="F73" s="35"/>
+      <c r="G73" s="35"/>
+      <c r="H73" s="35"/>
+      <c r="I73" s="33"/>
+    </row>
+    <row r="74" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="56" t="s">
+        <v>54</v>
+      </c>
+      <c r="B74" s="57"/>
+      <c r="C74" s="58">
         <v>1.1716</v>
       </c>
-      <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
-      <c r="F70" s="18"/>
-      <c r="G70" s="18"/>
-      <c r="H70" s="18"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A71" s="18"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
-      <c r="F71" s="18"/>
-      <c r="G71" s="18"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A72" s="62" t="s">
-        <v>140</v>
-      </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="18"/>
-      <c r="D72" s="18"/>
-      <c r="E72" s="18"/>
-      <c r="F72" s="18"/>
-      <c r="G72" s="18"/>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A73" s="19" t="s">
+      <c r="D74" s="18"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="18"/>
+      <c r="G74" s="18"/>
+      <c r="H74" s="18"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A75" s="18"/>
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A76" s="62" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76" s="18"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="18"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A77" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D77" s="28"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A78" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="28"/>
+    </row>
+    <row r="79" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B79" s="1"/>
+      <c r="F79" s="28"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A80" s="72"/>
+      <c r="B80" s="73" t="s">
+        <v>98</v>
+      </c>
+      <c r="C80" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D80" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="E80" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F80" s="73" t="s">
+        <v>47</v>
+      </c>
+      <c r="G80" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="D73" s="28"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A74" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74" s="28"/>
-    </row>
-    <row r="75" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B75" s="1"/>
-      <c r="F75" s="28"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A76" s="72"/>
-      <c r="B76" s="73" t="s">
-        <v>99</v>
-      </c>
-      <c r="C76" s="20" t="s">
+      <c r="H80" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="D76" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="E76" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="F76" s="73" t="s">
-        <v>47</v>
-      </c>
-      <c r="G76" s="74" t="s">
-        <v>97</v>
-      </c>
-      <c r="H76" s="73" t="s">
+      <c r="I80" s="74" t="s">
         <v>101</v>
       </c>
-      <c r="I76" s="74" t="s">
-        <v>102</v>
-      </c>
-      <c r="J76" s="73" t="s">
+      <c r="J80" s="73" t="s">
+        <v>106</v>
+      </c>
+      <c r="K80" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="K76" s="75" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A77" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B77" s="9">
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A81" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B81" s="9">
         <v>-7.7907000000000002</v>
       </c>
-      <c r="C77" s="9">
+      <c r="C81" s="9">
         <f>0.38149070739746/200</f>
         <v>1.9074535369873E-3</v>
       </c>
-      <c r="D77" s="9">
+      <c r="D81" s="9">
         <v>-10.930999999999999</v>
       </c>
-      <c r="E77" s="9">
+      <c r="E81" s="9">
         <f>0.393565416336059/200</f>
         <v>1.967827081680295E-3</v>
       </c>
-      <c r="F77" s="9">
+      <c r="F81" s="9">
         <v>-11.0616</v>
       </c>
-      <c r="G77" s="9">
+      <c r="G81" s="9">
         <f>1.41515588760375/200</f>
         <v>7.0757794380187497E-3</v>
       </c>
-      <c r="H77" s="9">
+      <c r="H81" s="9">
         <v>-11.5398</v>
       </c>
-      <c r="I77" s="9">
+      <c r="I81" s="9">
         <f>1.7515857219696/200</f>
         <v>8.7579286098480001E-3</v>
       </c>
-      <c r="J77" s="9">
+      <c r="J81" s="9">
         <v>-11.533899999999999</v>
       </c>
-      <c r="K77" s="30">
+      <c r="K81" s="30">
         <f>1.83847570419311/200</f>
         <v>9.1923785209655495E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A78" s="12" t="s">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A82" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B78" s="9">
+      <c r="B82" s="9">
         <v>2.2039</v>
       </c>
-      <c r="C78" s="9"/>
-      <c r="D78" s="9">
+      <c r="C82" s="9"/>
+      <c r="D82" s="9">
         <v>1.4112</v>
       </c>
-      <c r="E78" s="9"/>
-      <c r="F78" s="9">
+      <c r="E82" s="9"/>
+      <c r="F82" s="9">
         <v>0.95120000000000005</v>
       </c>
-      <c r="G78" s="9"/>
-      <c r="H78" s="9">
+      <c r="G82" s="9"/>
+      <c r="H82" s="9">
         <v>0.77070000000000005</v>
       </c>
-      <c r="I78" s="9"/>
-      <c r="J78" s="9">
+      <c r="I82" s="9"/>
+      <c r="J82" s="9">
         <v>0.59950000000000003</v>
       </c>
-      <c r="K78" s="30"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A79" s="12" t="s">
+      <c r="K82" s="30"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A83" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B79" s="9">
+      <c r="B83" s="9">
         <v>-11.7315</v>
       </c>
-      <c r="C79" s="9">
+      <c r="C83" s="9">
         <f>0.743644952774047/200</f>
         <v>3.7182247638702349E-3</v>
       </c>
-      <c r="D79" s="9">
+      <c r="D83" s="9">
         <v>-12.350300000000001</v>
       </c>
-      <c r="E79" s="9">
+      <c r="E83" s="9">
         <f>0.808241128921508/200</f>
         <v>4.0412056446075401E-3</v>
       </c>
-      <c r="F79" s="9">
+      <c r="F83" s="9">
         <v>-12.4358</v>
       </c>
-      <c r="G79" s="9">
+      <c r="G83" s="9">
         <f xml:space="preserve"> 2.81512689590454/200</f>
         <v>1.4075634479522701E-2</v>
       </c>
-      <c r="H79" s="9">
+      <c r="H83" s="9">
         <v>-12.7623</v>
       </c>
-      <c r="I79" s="9">
+      <c r="I83" s="9">
         <f>3.38718914985656/200</f>
         <v>1.69359457492828E-2</v>
       </c>
-      <c r="J79" s="9">
+      <c r="J83" s="9">
         <v>-12.7544</v>
       </c>
-      <c r="K79" s="30">
+      <c r="K83" s="30">
         <f>3.5751347541809/200</f>
         <v>1.7875673770904502E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="12" t="s">
+    <row r="84" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B80" s="9">
+      <c r="B84" s="9">
         <v>2.4887999999999999</v>
       </c>
-      <c r="C80" s="9"/>
-      <c r="D80" s="9">
+      <c r="C84" s="9"/>
+      <c r="D84" s="9">
         <v>1.5609</v>
       </c>
-      <c r="E80" s="9"/>
-      <c r="F80" s="9">
+      <c r="E84" s="9"/>
+      <c r="F84" s="9">
         <v>1.0578000000000001</v>
       </c>
-      <c r="G80" s="9"/>
-      <c r="H80" s="9">
+      <c r="G84" s="9"/>
+      <c r="H84" s="9">
         <v>0.8075</v>
       </c>
-      <c r="I80" s="9"/>
-      <c r="J80" s="9">
+      <c r="I84" s="9"/>
+      <c r="J84" s="9">
         <v>0.63580000000000003</v>
       </c>
-      <c r="K80" s="30"/>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A81" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="B81" s="9">
+      <c r="K84" s="30"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A85" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="B85" s="9">
         <v>-11.2082</v>
       </c>
-      <c r="C81" s="9">
+      <c r="C85" s="9">
         <f>8.5537621974945/200</f>
         <v>4.2768810987472497E-2</v>
       </c>
-      <c r="D81" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E81" s="9">
+      <c r="D85" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E85" s="9">
         <f>8.43400382995605/200</f>
         <v>4.2170019149780247E-2</v>
       </c>
-      <c r="F81" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="G81" s="9">
+      <c r="F85" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="G85" s="9">
         <f>10.424521446228/200</f>
         <v>5.2122607231140004E-2</v>
       </c>
-      <c r="H81" s="50" t="s">
-        <v>139</v>
-      </c>
-      <c r="I81" s="9">
+      <c r="H85" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="I85" s="9">
         <f>13.5266025066375/200</f>
         <v>6.76330125331875E-2</v>
       </c>
-      <c r="J81" s="9"/>
-      <c r="K81" s="30"/>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A82" s="12" t="s">
+      <c r="J85" s="9"/>
+      <c r="K85" s="30"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A86" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B82" s="9">
+      <c r="B86" s="9">
         <v>2.4382999999999999</v>
       </c>
-      <c r="C82" s="9"/>
-      <c r="D82" s="76">
+      <c r="C86" s="9"/>
+      <c r="D86" s="76">
         <v>1.5407</v>
       </c>
-      <c r="E82" s="9"/>
-      <c r="F82" s="9">
+      <c r="E86" s="9"/>
+      <c r="F86" s="9">
         <v>1.0585</v>
       </c>
-      <c r="G82" s="9"/>
-      <c r="H82" s="50">
+      <c r="G86" s="9"/>
+      <c r="H86" s="50">
         <v>0.79690000000000005</v>
       </c>
-      <c r="I82" s="18"/>
-      <c r="J82" s="18"/>
-      <c r="K82" s="8"/>
-    </row>
-    <row r="83" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A83" s="77" t="s">
-        <v>103</v>
-      </c>
-      <c r="B83" s="78"/>
-      <c r="C83" s="78"/>
-      <c r="D83" s="78" t="s">
-        <v>105</v>
-      </c>
-      <c r="E83" s="78">
+      <c r="I86" s="18"/>
+      <c r="J86" s="18"/>
+      <c r="K86" s="8"/>
+    </row>
+    <row r="87" spans="1:11" s="71" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="B87" s="78"/>
+      <c r="C87" s="78"/>
+      <c r="D87" s="78" t="s">
+        <v>104</v>
+      </c>
+      <c r="E87" s="78">
         <f>8.48960757255554/200</f>
         <v>4.2448037862777704E-2</v>
       </c>
-      <c r="F83" s="78" t="s">
-        <v>106</v>
-      </c>
-      <c r="G83" s="78">
+      <c r="F87" s="78" t="s">
+        <v>105</v>
+      </c>
+      <c r="G87" s="78">
         <f>9.56008505821228/200</f>
         <v>4.7800425291061405E-2</v>
       </c>
-      <c r="H83" s="79" t="s">
-        <v>104</v>
-      </c>
-      <c r="I83" s="78">
+      <c r="H87" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="I87" s="78">
         <f>11.0999789237976/200</f>
         <v>5.5499894618988001E-2</v>
       </c>
-      <c r="J83" s="79" t="s">
-        <v>121</v>
-      </c>
-      <c r="K83" s="80">
+      <c r="J87" s="79" t="s">
+        <v>120</v>
+      </c>
+      <c r="K87" s="80">
         <f>12.9774138927459/200</f>
         <v>6.4887069463729505E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:11" s="71" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="81" t="s">
+    <row r="88" spans="1:11" s="71" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="B84" s="82"/>
-      <c r="C84" s="82"/>
-      <c r="D84" s="83">
+      <c r="B88" s="82"/>
+      <c r="C88" s="82"/>
+      <c r="D88" s="83">
         <v>1.597</v>
       </c>
-      <c r="E84" s="82"/>
-      <c r="F84" s="83">
+      <c r="E88" s="82"/>
+      <c r="F88" s="83">
         <v>1.0552999999999999</v>
       </c>
-      <c r="G84" s="82"/>
-      <c r="H84" s="83">
+      <c r="G88" s="82"/>
+      <c r="H88" s="83">
         <v>0.82789999999999997</v>
       </c>
-      <c r="I84" s="82"/>
-      <c r="J84" s="83">
+      <c r="I88" s="82"/>
+      <c r="J88" s="83">
         <v>0.61240000000000006</v>
       </c>
-      <c r="K84" s="84"/>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A85" s="33"/>
-      <c r="B85" s="21"/>
-      <c r="C85" s="21"/>
-      <c r="D85" s="64"/>
-      <c r="E85" s="21"/>
-      <c r="F85" s="64"/>
-      <c r="G85" s="21"/>
-      <c r="H85" s="64"/>
-      <c r="I85" s="21"/>
-      <c r="J85" s="64"/>
-      <c r="K85" s="21"/>
-    </row>
-    <row r="86" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="B86" s="28"/>
-      <c r="C86" s="28"/>
-      <c r="D86" s="28"/>
-      <c r="E86" s="28"/>
-      <c r="F86" s="28"/>
-      <c r="G86" s="28"/>
-      <c r="H86" s="28"/>
-      <c r="I86" s="28"/>
-      <c r="J86" s="28"/>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A87" s="72"/>
-      <c r="B87" s="73" t="s">
+      <c r="K88" s="84"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A89" s="33"/>
+      <c r="B89" s="21"/>
+      <c r="C89" s="21"/>
+      <c r="D89" s="64"/>
+      <c r="E89" s="21"/>
+      <c r="F89" s="64"/>
+      <c r="G89" s="21"/>
+      <c r="H89" s="64"/>
+      <c r="I89" s="21"/>
+      <c r="J89" s="64"/>
+      <c r="K89" s="21"/>
+    </row>
+    <row r="90" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="35" t="s">
+        <v>137</v>
+      </c>
+      <c r="B90" s="28"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="28"/>
+      <c r="F90" s="28"/>
+      <c r="G90" s="28"/>
+      <c r="H90" s="28"/>
+      <c r="I90" s="28"/>
+      <c r="J90" s="28"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A91" s="72"/>
+      <c r="B91" s="73" t="s">
+        <v>98</v>
+      </c>
+      <c r="C91" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C87" s="20" t="s">
+      <c r="D91" s="73" t="s">
+        <v>46</v>
+      </c>
+      <c r="E91" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="F91" s="73" t="s">
+        <v>47</v>
+      </c>
+      <c r="G91" s="74" t="s">
+        <v>96</v>
+      </c>
+      <c r="H91" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="D87" s="73" t="s">
-        <v>46</v>
-      </c>
-      <c r="E87" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="F87" s="73" t="s">
-        <v>47</v>
-      </c>
-      <c r="G87" s="74" t="s">
-        <v>97</v>
-      </c>
-      <c r="H87" s="73" t="s">
+      <c r="I91" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="I87" s="75" t="s">
-        <v>102</v>
-      </c>
-      <c r="J87" s="85"/>
-      <c r="K87" s="33"/>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A88" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B88" s="86">
+      <c r="J91" s="85"/>
+      <c r="K91" s="33"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A92" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B92" s="86">
         <v>-7.2732999999999999</v>
       </c>
-      <c r="C88" s="86">
+      <c r="C92" s="86">
         <f>3.30510807037353/200</f>
         <v>1.6525540351867648E-2</v>
       </c>
-      <c r="D88" s="86">
+      <c r="D92" s="86">
         <v>-9.4646000000000008</v>
       </c>
-      <c r="E88" s="86">
+      <c r="E92" s="86">
         <f>3.73610782623291/200</f>
         <v>1.8680539131164551E-2</v>
       </c>
-      <c r="F88" s="86">
+      <c r="F92" s="86">
         <v>-9.5103000000000009</v>
       </c>
-      <c r="G88" s="86">
+      <c r="G92" s="86">
         <f>3.9412202835083/200</f>
         <v>1.9706101417541498E-2</v>
       </c>
-      <c r="H88" s="86">
+      <c r="H92" s="86">
         <v>-9.6827000000000005</v>
       </c>
-      <c r="I88" s="87">
+      <c r="I92" s="87">
         <f>4.63441228866577/200</f>
         <v>2.317206144332885E-2</v>
       </c>
-      <c r="J88" s="9"/>
-      <c r="K88" s="63"/>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A89" s="12" t="s">
+      <c r="J92" s="9"/>
+      <c r="K92" s="63"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A93" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B89" s="86">
+      <c r="B93" s="86">
         <v>0.66759999999999997</v>
       </c>
-      <c r="C89" s="86"/>
-      <c r="D89" s="86">
+      <c r="C93" s="86"/>
+      <c r="D93" s="86">
         <v>0.6905</v>
       </c>
-      <c r="E89" s="86"/>
-      <c r="F89" s="86">
+      <c r="E93" s="86"/>
+      <c r="F93" s="86">
         <v>0.68589999999999995</v>
       </c>
-      <c r="G89" s="86"/>
-      <c r="H89" s="86">
+      <c r="G93" s="86"/>
+      <c r="H93" s="86">
         <v>0.49120000000000003</v>
       </c>
-      <c r="I89" s="87"/>
-      <c r="J89" s="9"/>
-      <c r="K89" s="63"/>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A90" s="12" t="s">
+      <c r="I93" s="87"/>
+      <c r="J93" s="9"/>
+      <c r="K93" s="63"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A94" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="86">
+      <c r="B94" s="86">
         <v>-11.763400000000001</v>
       </c>
-      <c r="C90" s="86">
+      <c r="C94" s="86">
         <f>6.93132138252258/200</f>
         <v>3.4656606912612901E-2</v>
       </c>
-      <c r="D90" s="86">
+      <c r="D94" s="86">
         <v>-12.1273</v>
       </c>
-      <c r="E90" s="86">
+      <c r="E94" s="86">
         <f>8.01621603965759/200</f>
         <v>4.0081080198287947E-2</v>
       </c>
-      <c r="F90" s="86">
+      <c r="F94" s="86">
         <v>-12.002599999999999</v>
       </c>
-      <c r="G90" s="86">
+      <c r="G94" s="86">
         <f>8.17840385437011/200</f>
         <v>4.0892019271850551E-2</v>
       </c>
-      <c r="H90" s="86">
+      <c r="H94" s="86">
         <v>-12.107100000000001</v>
       </c>
-      <c r="I90" s="87">
+      <c r="I94" s="87">
         <f>9.89218688011169/200</f>
         <v>4.9460934400558453E-2</v>
       </c>
-      <c r="J90" s="9"/>
-      <c r="K90" s="63"/>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A91" s="12" t="s">
+      <c r="J94" s="9"/>
+      <c r="K94" s="63"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A95" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B91" s="86">
+      <c r="B95" s="86">
         <v>0.9052</v>
       </c>
-      <c r="C91" s="86"/>
-      <c r="D91" s="86">
+      <c r="C95" s="86"/>
+      <c r="D95" s="86">
         <v>0.71509999999999996</v>
       </c>
-      <c r="E91" s="86"/>
-      <c r="F91" s="86">
+      <c r="E95" s="86"/>
+      <c r="F95" s="86">
         <v>0.66969999999999996</v>
       </c>
-      <c r="G91" s="86"/>
-      <c r="H91" s="86">
+      <c r="G95" s="86"/>
+      <c r="H95" s="86">
         <v>0.52600000000000002</v>
       </c>
-      <c r="I91" s="87"/>
-      <c r="J91" s="9"/>
-      <c r="K91" s="63"/>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A92" s="12" t="s">
+      <c r="I95" s="87"/>
+      <c r="J95" s="9"/>
+      <c r="K95" s="63"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A96" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B92" s="86">
+      <c r="B96" s="86">
         <v>-11.6623</v>
       </c>
-      <c r="C92" s="86">
+      <c r="C96" s="86">
         <f>80.5346596240997/200</f>
         <v>0.40267329812049851</v>
       </c>
-      <c r="D92" s="86">
+      <c r="D96" s="86">
         <v>-11.852600000000001</v>
       </c>
-      <c r="E92" s="86">
+      <c r="E96" s="86">
         <f>85.9917159080505/200</f>
         <v>0.42995857954025246</v>
       </c>
-      <c r="F92" s="86">
+      <c r="F96" s="86">
         <v>-11.3972</v>
       </c>
-      <c r="G92" s="86">
+      <c r="G96" s="86">
         <f xml:space="preserve"> 102.554239511489/200</f>
         <v>0.51277119755744505</v>
       </c>
-      <c r="H92" s="86">
+      <c r="H96" s="86">
         <v>-10.0825</v>
       </c>
-      <c r="I92" s="87">
+      <c r="I96" s="87">
         <f xml:space="preserve"> 135.115339517593/200</f>
         <v>0.6755766975879649</v>
       </c>
-      <c r="J92" s="9"/>
-      <c r="K92" s="63"/>
-    </row>
-    <row r="93" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="13" t="s">
+      <c r="J96" s="9"/>
+      <c r="K96" s="63"/>
+    </row>
+    <row r="97" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B93" s="88">
+      <c r="B97" s="88">
         <v>0.89839999999999998</v>
       </c>
-      <c r="C93" s="88"/>
-      <c r="D93" s="89">
+      <c r="C97" s="88"/>
+      <c r="D97" s="89">
         <v>0.70909999999999995</v>
       </c>
-      <c r="E93" s="88"/>
-      <c r="F93" s="88">
+      <c r="E97" s="88"/>
+      <c r="F97" s="88">
         <v>0.80679999999999996</v>
       </c>
-      <c r="G93" s="88"/>
-      <c r="H93" s="88">
+      <c r="G97" s="88"/>
+      <c r="H97" s="88">
         <v>1.3221000000000001</v>
       </c>
-      <c r="I93" s="90"/>
-      <c r="J93" s="18"/>
-      <c r="K93" s="21"/>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A94" s="28"/>
-      <c r="B94" s="28"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="28"/>
-      <c r="E94" s="28"/>
-      <c r="F94" s="28"/>
-      <c r="G94" s="28"/>
-      <c r="H94" s="28"/>
-      <c r="I94" s="28"/>
-      <c r="J94" s="28"/>
-    </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A95" s="28"/>
-      <c r="B95" s="28"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="28"/>
-      <c r="E95" s="28"/>
-      <c r="F95" s="28"/>
-      <c r="G95" s="28"/>
-      <c r="H95" s="28"/>
-      <c r="I95" s="28"/>
-      <c r="J95" s="28"/>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A98" s="7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A99" s="19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A100" s="28" t="s">
+      <c r="I97" s="90"/>
+      <c r="J97" s="18"/>
+      <c r="K97" s="21"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A98" s="28"/>
+      <c r="B98" s="28"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="28"/>
+      <c r="G98" s="28"/>
+      <c r="H98" s="28"/>
+      <c r="I98" s="28"/>
+      <c r="J98" s="28"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A99" s="28"/>
+      <c r="B99" s="28"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="28"/>
+      <c r="F99" s="28"/>
+      <c r="G99" s="28"/>
+      <c r="H99" s="28"/>
+      <c r="I99" s="28"/>
+      <c r="J99" s="28"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A102" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A103" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A104" s="28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A101" t="s">
+    <row r="105" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A105" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A102" s="14" t="s">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A106" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B102" s="37" t="s">
+      <c r="B106" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C102" s="37" t="s">
+      <c r="C106" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D102" s="37" t="s">
+      <c r="D106" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E102" s="37" t="s">
+      <c r="E106" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F102" s="37" t="s">
+      <c r="F106" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G102" s="48" t="s">
+      <c r="G106" s="48" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A103" s="5" t="s">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A107" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B103" s="9">
+      <c r="B107" s="9">
         <v>2.7021000000000002</v>
       </c>
-      <c r="C103" s="9">
+      <c r="C107" s="9">
         <v>-7.3941999999999997</v>
       </c>
-      <c r="D103" s="9">
+      <c r="D107" s="9">
         <v>-17.366499999999998</v>
       </c>
-      <c r="E103" s="9">
+      <c r="E107" s="9">
         <v>-27.2926</v>
       </c>
-      <c r="F103" s="9">
+      <c r="F107" s="9">
         <v>-37.272500000000001</v>
       </c>
-      <c r="G103" s="30">
+      <c r="G107" s="30">
         <f>1.87291026115417/200</f>
         <v>9.3645513057708501E-3</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A104" s="5" t="s">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A108" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B104" s="9">
+      <c r="B108" s="9">
         <v>0.88500000000000001</v>
       </c>
-      <c r="C104" s="9">
+      <c r="C108" s="9">
         <v>0.90100000000000002</v>
       </c>
-      <c r="D104" s="9">
+      <c r="D108" s="9">
         <v>0.95669999999999999</v>
       </c>
-      <c r="E104" s="9">
+      <c r="E108" s="9">
         <v>0.96560000000000001</v>
       </c>
-      <c r="F104" s="9">
+      <c r="F108" s="9">
         <v>1.0293000000000001</v>
       </c>
-      <c r="G104" s="49"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A105" s="5"/>
-      <c r="B105" s="50"/>
-      <c r="C105" s="9"/>
-      <c r="D105" s="9"/>
-      <c r="E105" s="9"/>
-      <c r="F105" s="9"/>
-      <c r="G105" s="49"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A106" s="5" t="s">
+      <c r="G108" s="49"/>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A109" s="5"/>
+      <c r="B109" s="50"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="9"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9"/>
+      <c r="G109" s="49"/>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A110" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B106" s="9">
+      <c r="B110" s="9">
         <v>11.153700000000001</v>
       </c>
-      <c r="C106" s="9">
+      <c r="C110" s="9">
         <v>0.92630000000000001</v>
       </c>
-      <c r="D106" s="9">
+      <c r="D110" s="9">
         <v>-9.1595999999999993</v>
       </c>
-      <c r="E106" s="9">
+      <c r="E110" s="9">
         <v>-18.4282</v>
       </c>
-      <c r="F106" s="9">
+      <c r="F110" s="9">
         <v>-28.785699999999999</v>
       </c>
-      <c r="G106" s="30">
+      <c r="G110" s="30">
         <f>1.73989057540893/200</f>
         <v>8.6994528770446503E-3</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A107" s="5" t="s">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A111" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B107" s="9">
+      <c r="B111" s="9">
         <v>3.0234000000000001</v>
       </c>
-      <c r="C107" s="9">
+      <c r="C111" s="9">
         <v>3.0640999999999998</v>
       </c>
-      <c r="D107" s="9">
+      <c r="D111" s="9">
         <v>3.6509</v>
       </c>
-      <c r="E107" s="9">
+      <c r="E111" s="9">
         <v>3.2534000000000001</v>
       </c>
-      <c r="F107" s="9">
+      <c r="F111" s="9">
         <v>3.3008000000000002</v>
       </c>
-      <c r="G107" s="49"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A108" s="5"/>
-      <c r="B108" s="50"/>
-      <c r="C108" s="9"/>
-      <c r="D108" s="9"/>
-      <c r="E108" s="9"/>
-      <c r="F108" s="9"/>
-      <c r="G108" s="49"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A109" s="5" t="s">
+      <c r="G111" s="49"/>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A112" s="5"/>
+      <c r="B112" s="50"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
+      <c r="G112" s="49"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A113" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B109" s="9">
+      <c r="B113" s="9">
         <v>-1.8754</v>
       </c>
-      <c r="C109" s="9">
+      <c r="C113" s="9">
         <v>-11.879799999999999</v>
       </c>
-      <c r="D109" s="9">
+      <c r="D113" s="9">
         <v>-21.812200000000001</v>
       </c>
-      <c r="E109" s="9">
+      <c r="E113" s="9">
         <v>-31.9605</v>
       </c>
-      <c r="F109" s="9">
+      <c r="F113" s="9">
         <v>-41.809899999999999</v>
       </c>
-      <c r="G109" s="30">
+      <c r="G113" s="30">
         <f>3.64388179779052/200</f>
         <v>1.82194089889526E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A110" s="5" t="s">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A114" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B110" s="9">
+      <c r="B114" s="9">
         <v>1.2853000000000001</v>
       </c>
-      <c r="C110" s="9">
+      <c r="C114" s="9">
         <v>1.2719</v>
       </c>
-      <c r="D110" s="9">
+      <c r="D114" s="9">
         <v>1.1487000000000001</v>
       </c>
-      <c r="E110" s="9">
+      <c r="E114" s="9">
         <v>1.2646999999999999</v>
       </c>
-      <c r="F110" s="9">
+      <c r="F114" s="9">
         <v>1.1558999999999999</v>
       </c>
-      <c r="G110" s="30"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A111" s="5"/>
-      <c r="B111" s="50"/>
-      <c r="C111" s="9"/>
-      <c r="D111" s="9"/>
-      <c r="E111" s="9"/>
-      <c r="F111" s="9"/>
-      <c r="G111" s="30"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A112" s="5" t="s">
+      <c r="G114" s="30"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A115" s="5"/>
+      <c r="B115" s="50"/>
+      <c r="C115" s="9"/>
+      <c r="D115" s="9"/>
+      <c r="E115" s="9"/>
+      <c r="F115" s="9"/>
+      <c r="G115" s="30"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A116" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B112" s="9">
+      <c r="B116" s="9">
         <v>5.5016999999999996</v>
       </c>
-      <c r="C112" s="9">
+      <c r="C116" s="9">
         <v>-4.8254000000000001</v>
       </c>
-      <c r="D112" s="9">
+      <c r="D116" s="9">
         <v>-15.061500000000001</v>
       </c>
-      <c r="E112" s="9">
+      <c r="E116" s="9">
         <v>-24.198</v>
       </c>
-      <c r="F112" s="9">
+      <c r="F116" s="9">
         <v>-34.591799999999999</v>
       </c>
-      <c r="G112" s="30">
+      <c r="G116" s="30">
         <f>3.63707900047302/200</f>
         <v>1.8185395002365098E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A113" s="5" t="s">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A117" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B113" s="9">
+      <c r="B117" s="9">
         <v>2.9416000000000002</v>
       </c>
-      <c r="C113" s="9">
+      <c r="C117" s="9">
         <v>3.2046000000000001</v>
       </c>
-      <c r="D113" s="9">
+      <c r="D117" s="9">
         <v>3.4399000000000002</v>
       </c>
-      <c r="E113" s="9">
+      <c r="E117" s="9">
         <v>3.1190000000000002</v>
       </c>
-      <c r="F113" s="9">
+      <c r="F117" s="9">
         <v>3.133</v>
       </c>
-      <c r="G113" s="49"/>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A114" s="5"/>
-      <c r="B114" s="50"/>
-      <c r="C114" s="50"/>
-      <c r="D114" s="50"/>
-      <c r="E114" s="50"/>
-      <c r="F114" s="50"/>
-      <c r="G114" s="49"/>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A115" s="5" t="s">
+      <c r="G117" s="49"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A118" s="5"/>
+      <c r="B118" s="50"/>
+      <c r="C118" s="50"/>
+      <c r="D118" s="50"/>
+      <c r="E118" s="50"/>
+      <c r="F118" s="50"/>
+      <c r="G118" s="49"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A119" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B115" s="9">
+      <c r="B119" s="9">
         <f>-1.7902</f>
         <v>-1.7902</v>
       </c>
-      <c r="C115" s="9">
+      <c r="C119" s="9">
         <v>-11.8467</v>
       </c>
-      <c r="D115" s="9">
+      <c r="D119" s="9">
         <v>-21.738299999999999</v>
       </c>
-      <c r="E115" s="9">
+      <c r="E119" s="9">
         <v>-31.619900000000001</v>
       </c>
-      <c r="F115" s="9">
+      <c r="F119" s="9">
         <v>-41.830800000000004</v>
       </c>
-      <c r="G115" s="30">
+      <c r="G119" s="30">
         <f>43.5942468643188/200</f>
         <v>0.21797123432159399</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A116" s="5" t="s">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A120" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B116" s="9">
+      <c r="B120" s="9">
         <v>1.2419</v>
       </c>
-      <c r="C116" s="9">
+      <c r="C120" s="9">
         <v>1.1898</v>
       </c>
-      <c r="D116" s="9">
+      <c r="D120" s="9">
         <v>1.2814000000000001</v>
       </c>
-      <c r="E116" s="9">
+      <c r="E120" s="9">
         <v>1.1073</v>
       </c>
-      <c r="F116" s="26">
+      <c r="F120" s="26">
         <v>1.2888999999999999</v>
       </c>
-      <c r="G116" s="30"/>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A117" s="5"/>
-      <c r="B117" s="9"/>
-      <c r="C117" s="9"/>
-      <c r="D117" s="9"/>
-      <c r="E117" s="9"/>
-      <c r="F117" s="9"/>
-      <c r="G117" s="30"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A118" s="5" t="s">
+      <c r="G120" s="30"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A121" s="5"/>
+      <c r="B121" s="9"/>
+      <c r="C121" s="9"/>
+      <c r="D121" s="9"/>
+      <c r="E121" s="9"/>
+      <c r="F121" s="9"/>
+      <c r="G121" s="30"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A122" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B118" s="9">
+      <c r="B122" s="9">
         <v>-0.77390000000000003</v>
       </c>
-      <c r="C118" s="9">
+      <c r="C122" s="9">
         <v>-10.8522</v>
       </c>
-      <c r="D118" s="9">
+      <c r="D122" s="9">
         <v>-21.103899999999999</v>
       </c>
-      <c r="E118" s="9">
+      <c r="E122" s="9">
         <v>-29.667200000000001</v>
       </c>
-      <c r="F118" s="9">
+      <c r="F122" s="9">
         <v>-38.0655</v>
       </c>
-      <c r="G118" s="30"/>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A119" s="5" t="s">
+      <c r="G122" s="30"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A123" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B119" s="9">
+      <c r="B123" s="9">
         <v>1.2433000000000001</v>
       </c>
-      <c r="C119" s="9">
+      <c r="C123" s="9">
         <v>1.1579999999999999</v>
       </c>
-      <c r="D119" s="9">
+      <c r="D123" s="9">
         <v>1.2155</v>
       </c>
-      <c r="E119" s="9">
+      <c r="E123" s="9">
         <v>1.2145999999999999</v>
       </c>
-      <c r="F119" s="9">
+      <c r="F123" s="9">
         <v>1.1361000000000001</v>
       </c>
-      <c r="G119" s="30"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A120" s="5"/>
-      <c r="B120" s="9"/>
-      <c r="C120" s="9"/>
-      <c r="D120" s="9"/>
-      <c r="E120" s="9"/>
-      <c r="F120" s="9"/>
-      <c r="G120" s="30"/>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A121" s="5" t="s">
+      <c r="G123" s="30"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A124" s="5"/>
+      <c r="B124" s="9"/>
+      <c r="C124" s="9"/>
+      <c r="D124" s="9"/>
+      <c r="E124" s="9"/>
+      <c r="F124" s="9"/>
+      <c r="G124" s="30"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A125" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B121" s="9">
+      <c r="B125" s="9">
         <v>-1.7432000000000001</v>
       </c>
-      <c r="C121" s="9">
+      <c r="C125" s="9">
         <v>-11.6966</v>
       </c>
-      <c r="D121" s="9">
+      <c r="D125" s="9">
         <v>-21.720500000000001</v>
       </c>
-      <c r="E121" s="9">
+      <c r="E125" s="9">
         <v>-31.185500000000001</v>
       </c>
-      <c r="F121" s="9">
+      <c r="F125" s="9">
         <v>-40.300899999999999</v>
       </c>
-      <c r="G121" s="30"/>
-    </row>
-    <row r="122" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A122" s="6" t="s">
+      <c r="G125" s="30"/>
+    </row>
+    <row r="126" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A126" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B122" s="31">
+      <c r="B126" s="31">
         <v>1.2693000000000001</v>
       </c>
-      <c r="C122" s="31">
+      <c r="C126" s="31">
         <v>1.2414000000000001</v>
       </c>
-      <c r="D122" s="31">
+      <c r="D126" s="31">
         <v>1.1528</v>
       </c>
-      <c r="E122" s="31">
+      <c r="E126" s="31">
         <v>1.2195</v>
       </c>
-      <c r="F122" s="31">
+      <c r="F126" s="31">
         <v>1.1687000000000001</v>
       </c>
-      <c r="G122" s="32"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A123" s="21"/>
-      <c r="B123" s="17"/>
-      <c r="C123" s="17"/>
-      <c r="D123" s="17"/>
-      <c r="E123" s="17"/>
-      <c r="F123" s="17"/>
-      <c r="G123" s="17"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A124" s="33"/>
-      <c r="B124" s="33" t="s">
+      <c r="G126" s="32"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A127" s="21"/>
+      <c r="B127" s="17"/>
+      <c r="C127" s="17"/>
+      <c r="D127" s="17"/>
+      <c r="E127" s="17"/>
+      <c r="F127" s="17"/>
+      <c r="G127" s="17"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A128" s="33"/>
+      <c r="B128" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="D124" s="17"/>
-      <c r="E124" s="17"/>
-      <c r="F124" s="17"/>
-      <c r="G124" s="17"/>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A125" s="21"/>
-      <c r="B125" s="18" t="s">
+      <c r="D128" s="17"/>
+      <c r="E128" s="17"/>
+      <c r="F128" s="17"/>
+      <c r="G128" s="17"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A129" s="21"/>
+      <c r="B129" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="C125" s="18"/>
-      <c r="D125" s="17"/>
-      <c r="E125" s="17"/>
-      <c r="F125" s="17"/>
-      <c r="G125" s="17"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A128" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C128" s="19"/>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A129" t="s">
+      <c r="C129" s="18"/>
+      <c r="D129" s="17"/>
+      <c r="E129" s="17"/>
+      <c r="F129" s="17"/>
+      <c r="G129" s="17"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A132" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="C132" s="19"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A133" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" t="s">
+    <row r="134" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A134" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A131" s="14" t="s">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A135" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B131" s="37" t="s">
+      <c r="B135" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C131" s="37" t="s">
+      <c r="C135" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="D131" s="37" t="s">
+      <c r="D135" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E131" s="37" t="s">
+      <c r="E135" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="F131" s="37" t="s">
+      <c r="F135" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="G131" s="48" t="s">
+      <c r="G135" s="48" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A132" s="5" t="s">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A136" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B132" s="9">
+      <c r="B136" s="9">
         <v>3.4502999999999999</v>
       </c>
-      <c r="C132" s="9">
+      <c r="C136" s="9">
         <v>-6.5942999999999996</v>
       </c>
-      <c r="D132" s="9">
+      <c r="D136" s="9">
         <v>-16.561499999999999</v>
       </c>
-      <c r="E132" s="9">
+      <c r="E136" s="9">
         <v>-26.6008</v>
       </c>
-      <c r="F132" s="9">
+      <c r="F136" s="9">
         <v>-36.565199999999997</v>
       </c>
-      <c r="G132" s="30">
+      <c r="G136" s="30">
         <f>1.81720042228698/1000</f>
         <v>1.8172004222869801E-3</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A133" s="5" t="s">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A137" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B133" s="9">
+      <c r="B137" s="9">
         <v>1.8456999999999999</v>
       </c>
-      <c r="C133" s="9">
+      <c r="C137" s="9">
         <v>1.8831</v>
       </c>
-      <c r="D133" s="9">
+      <c r="D137" s="9">
         <v>1.8754999999999999</v>
       </c>
-      <c r="E133" s="9">
+      <c r="E137" s="9">
         <v>1.9067000000000001</v>
       </c>
-      <c r="F133" s="9">
+      <c r="F137" s="9">
         <v>1.8309</v>
       </c>
-      <c r="G133" s="49"/>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A134" s="5"/>
-      <c r="B134" s="50"/>
-      <c r="C134" s="9"/>
-      <c r="D134" s="9"/>
-      <c r="E134" s="9"/>
-      <c r="F134" s="9"/>
-      <c r="G134" s="49"/>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A135" s="5" t="s">
+      <c r="G137" s="49"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A138" s="5"/>
+      <c r="B138" s="50"/>
+      <c r="C138" s="9"/>
+      <c r="D138" s="9"/>
+      <c r="E138" s="9"/>
+      <c r="F138" s="9"/>
+      <c r="G138" s="49"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A139" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B135" s="9">
+      <c r="B139" s="9">
         <v>33.961399999999998</v>
       </c>
-      <c r="C135" s="9">
+      <c r="C139" s="9">
         <v>23.832799999999999</v>
       </c>
-      <c r="D135" s="9">
+      <c r="D139" s="9">
         <v>13.8483</v>
       </c>
-      <c r="E135" s="9">
+      <c r="E139" s="9">
         <v>4.1989999999999998</v>
       </c>
-      <c r="F135" s="9">
+      <c r="F139" s="9">
         <v>-6.4336000000000002</v>
       </c>
-      <c r="G135" s="30"/>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A136" s="5" t="s">
+      <c r="G139" s="30"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A140" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B136" s="9">
+      <c r="B140" s="9">
         <v>3.9329999999999998</v>
       </c>
-      <c r="C136" s="9">
+      <c r="C140" s="9">
         <v>3.8573</v>
       </c>
-      <c r="D136" s="9">
+      <c r="D140" s="9">
         <v>3.6829000000000001</v>
       </c>
-      <c r="E136" s="9">
+      <c r="E140" s="9">
         <v>3.8494999999999999</v>
       </c>
-      <c r="F136" s="9">
+      <c r="F140" s="9">
         <v>3.8119000000000001</v>
       </c>
-      <c r="G136" s="49"/>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A137" s="5"/>
-      <c r="B137" s="50"/>
-      <c r="C137" s="9"/>
-      <c r="D137" s="9"/>
-      <c r="E137" s="9"/>
-      <c r="F137" s="9"/>
-      <c r="G137" s="49"/>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A138" s="5" t="s">
+      <c r="G140" s="49"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A141" s="5"/>
+      <c r="B141" s="50"/>
+      <c r="C141" s="9"/>
+      <c r="D141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
+      <c r="G141" s="49"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A142" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B138" s="9">
+      <c r="B142" s="9">
         <v>-3.8433999999999999</v>
       </c>
-      <c r="C138" s="9">
+      <c r="C142" s="9">
         <v>-13.9133</v>
       </c>
-      <c r="D138" s="9">
+      <c r="D142" s="9">
         <v>-23.5916</v>
       </c>
-      <c r="E138" s="9">
+      <c r="E142" s="9">
         <v>-33.8613</v>
       </c>
-      <c r="F138" s="9">
+      <c r="F142" s="9">
         <v>-43.593000000000004</v>
       </c>
-      <c r="G138" s="30">
+      <c r="G142" s="30">
         <f>3.73042225837707/1000</f>
         <v>3.7304222583770699E-3</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A139" s="5" t="s">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A143" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B139" s="9">
+      <c r="B143" s="9">
         <v>2.6547999999999998</v>
       </c>
-      <c r="C139" s="9">
+      <c r="C143" s="9">
         <v>2.7086999999999999</v>
       </c>
-      <c r="D139" s="9">
+      <c r="D143" s="9">
         <v>2.7507000000000001</v>
       </c>
-      <c r="E139" s="9">
+      <c r="E143" s="9">
         <v>2.7532999999999999</v>
       </c>
-      <c r="F139" s="9">
+      <c r="F143" s="9">
         <v>2.7458</v>
       </c>
-      <c r="G139" s="30"/>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A140" s="5"/>
-      <c r="B140" s="50"/>
-      <c r="C140" s="9"/>
-      <c r="D140" s="9"/>
-      <c r="E140" s="9"/>
-      <c r="F140" s="9"/>
-      <c r="G140" s="30"/>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A141" s="5" t="s">
+      <c r="G143" s="30"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A144" s="5"/>
+      <c r="B144" s="50"/>
+      <c r="C144" s="9"/>
+      <c r="D144" s="9"/>
+      <c r="E144" s="9"/>
+      <c r="F144" s="9"/>
+      <c r="G144" s="30"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A145" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B141" s="9">
+      <c r="B145" s="9">
         <v>32.962600000000002</v>
       </c>
-      <c r="C141" s="9">
+      <c r="C145" s="9">
         <v>22.838000000000001</v>
       </c>
-      <c r="D141" s="9">
+      <c r="D145" s="9">
         <v>12.853400000000001</v>
       </c>
-      <c r="E141" s="9">
+      <c r="E145" s="9">
         <v>3.2014</v>
       </c>
-      <c r="F141" s="9">
+      <c r="F145" s="9">
         <v>-7.4305000000000003</v>
       </c>
-      <c r="G141" s="30"/>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A142" s="5" t="s">
+      <c r="G145" s="30"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A146" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B142" s="9">
+      <c r="B146" s="9">
         <v>3.9333999999999998</v>
       </c>
-      <c r="C142" s="9">
+      <c r="C146" s="9">
         <v>3.859</v>
       </c>
-      <c r="D142" s="9">
+      <c r="D146" s="9">
         <v>3.6848999999999998</v>
       </c>
-      <c r="E142" s="9">
+      <c r="E146" s="9">
         <v>3.851</v>
       </c>
-      <c r="F142" s="9">
+      <c r="F146" s="9">
         <v>3.8092000000000001</v>
       </c>
-      <c r="G142" s="49"/>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A143" s="5"/>
-      <c r="B143" s="50"/>
-      <c r="C143" s="50"/>
-      <c r="D143" s="50"/>
-      <c r="E143" s="50"/>
-      <c r="F143" s="50"/>
-      <c r="G143" s="49"/>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A144" s="5" t="s">
+      <c r="G146" s="49"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A147" s="5"/>
+      <c r="B147" s="50"/>
+      <c r="C147" s="50"/>
+      <c r="D147" s="50"/>
+      <c r="E147" s="50"/>
+      <c r="F147" s="50"/>
+      <c r="G147" s="49"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A148" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B144" s="9">
+      <c r="B148" s="9">
         <v>-3.3506</v>
       </c>
-      <c r="C144" s="9">
+      <c r="C148" s="9">
         <v>-13.5854</v>
       </c>
-      <c r="D144" s="9">
+      <c r="D148" s="9">
         <v>-23.3325</v>
       </c>
-      <c r="E144" s="9">
+      <c r="E148" s="9">
         <v>-33.126199999999997</v>
       </c>
-      <c r="F144" s="9">
+      <c r="F148" s="9">
         <v>-43.1599</v>
       </c>
-      <c r="G144" s="30">
+      <c r="G148" s="30">
         <f>44.6756930351257/1000</f>
         <v>4.4675693035125696E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A145" s="5" t="s">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A149" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B145" s="9">
+      <c r="B149" s="9">
         <v>2.6993</v>
       </c>
-      <c r="C145" s="9">
+      <c r="C149" s="9">
         <v>2.6728000000000001</v>
       </c>
-      <c r="D145" s="9">
+      <c r="D149" s="9">
         <v>2.6707000000000001</v>
       </c>
-      <c r="E145" s="9">
+      <c r="E149" s="9">
         <v>2.6284000000000001</v>
       </c>
-      <c r="F145" s="9">
+      <c r="F149" s="9">
         <v>2.6488</v>
       </c>
-      <c r="G145" s="30"/>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A146" s="5"/>
-      <c r="B146" s="9"/>
-      <c r="C146" s="9"/>
-      <c r="D146" s="9"/>
-      <c r="E146" s="9"/>
-      <c r="F146" s="9"/>
-      <c r="G146" s="30"/>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A147" s="5" t="s">
+      <c r="G149" s="30"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A150" s="5"/>
+      <c r="B150" s="9"/>
+      <c r="C150" s="9"/>
+      <c r="D150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
+      <c r="G150" s="30"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A151" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B147" s="9">
+      <c r="B151" s="9">
         <v>10.5525</v>
       </c>
-      <c r="C147" s="9">
+      <c r="C151" s="9">
         <v>-2.0112999999999999</v>
       </c>
-      <c r="D147" s="9">
+      <c r="D151" s="9">
         <v>-10.688499999999999</v>
       </c>
-      <c r="E147" s="9">
+      <c r="E151" s="9">
         <v>-21.682500000000001</v>
       </c>
-      <c r="F147" s="9">
+      <c r="F151" s="9">
         <v>-31.886700000000001</v>
       </c>
-      <c r="G147" s="30"/>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A148" s="5" t="s">
+      <c r="G151" s="30"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A152" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B148" s="9">
+      <c r="B152" s="9">
         <v>3.1505999999999998</v>
       </c>
-      <c r="C148" s="9">
+      <c r="C152" s="9">
         <v>1.9450000000000001</v>
       </c>
-      <c r="D148" s="9">
+      <c r="D152" s="9">
         <v>1.9343999999999999</v>
       </c>
-      <c r="E148" s="9">
+      <c r="E152" s="9">
         <v>1.6428</v>
       </c>
-      <c r="F148" s="9">
+      <c r="F152" s="9">
         <v>1.2435</v>
       </c>
-      <c r="G148" s="30"/>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A149" s="5"/>
-      <c r="B149" s="9"/>
-      <c r="C149" s="9"/>
-      <c r="D149" s="9"/>
-      <c r="E149" s="9"/>
-      <c r="F149" s="9"/>
-      <c r="G149" s="30"/>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A150" s="5" t="s">
+      <c r="G152" s="30"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A153" s="5"/>
+      <c r="B153" s="9"/>
+      <c r="C153" s="9"/>
+      <c r="D153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
+      <c r="G153" s="30"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A154" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B150" s="9">
+      <c r="B154" s="9">
         <v>-3.4333999999999998</v>
       </c>
-      <c r="C150" s="9">
+      <c r="C154" s="9">
         <v>-12.944599999999999</v>
       </c>
-      <c r="D150" s="9">
+      <c r="D154" s="9">
         <v>-23.013100000000001</v>
       </c>
-      <c r="E150" s="9">
+      <c r="E154" s="9">
         <v>-32.932000000000002</v>
       </c>
-      <c r="F150" s="9">
+      <c r="F154" s="9">
         <v>-41.863900000000001</v>
       </c>
-      <c r="G150" s="30"/>
-    </row>
-    <row r="151" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A151" s="6" t="s">
+      <c r="G154" s="30"/>
+    </row>
+    <row r="155" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A155" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B151" s="31">
+      <c r="B155" s="31">
         <v>2.6326999999999998</v>
       </c>
-      <c r="C151" s="31">
+      <c r="C155" s="31">
         <v>2.6817000000000002</v>
       </c>
-      <c r="D151" s="31">
+      <c r="D155" s="31">
         <v>2.7978000000000001</v>
       </c>
-      <c r="E151" s="31">
+      <c r="E155" s="31">
         <v>2.4706999999999999</v>
       </c>
-      <c r="F151" s="31">
+      <c r="F155" s="31">
         <v>2.6570999999999998</v>
       </c>
-      <c r="G151" s="32"/>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B152" s="29"/>
-      <c r="C152" s="29"/>
-      <c r="D152" s="29"/>
-      <c r="E152" s="29"/>
-      <c r="F152" s="29"/>
-      <c r="G152" s="29"/>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B153" s="61" t="s">
+      <c r="G155" s="32"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B156" s="29"/>
+      <c r="C156" s="29"/>
+      <c r="D156" s="29"/>
+      <c r="E156" s="29"/>
+      <c r="F156" s="29"/>
+      <c r="G156" s="29"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B157" s="61" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B154" t="s">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B158" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A157" s="7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A163" s="7" t="s">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A161" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A167" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A168" s="28" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A164" s="28" t="s">
+      <c r="B168" s="28"/>
+      <c r="C168" s="28"/>
+      <c r="D168" s="28"/>
+      <c r="E168" s="28"/>
+      <c r="F168" s="28"/>
+      <c r="G168" s="28"/>
+    </row>
+    <row r="169" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A169" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="B169" s="28"/>
+      <c r="C169" s="28"/>
+      <c r="D169" s="28"/>
+      <c r="E169" s="28"/>
+      <c r="F169" s="28"/>
+      <c r="G169" s="28"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A170" s="72" t="s">
+        <v>141</v>
+      </c>
+      <c r="B170" s="73">
+        <v>-10</v>
+      </c>
+      <c r="C170" s="73">
+        <v>0</v>
+      </c>
+      <c r="D170" s="73">
+        <v>10</v>
+      </c>
+      <c r="E170" s="94">
+        <v>20</v>
+      </c>
+      <c r="F170" s="85"/>
+      <c r="G170" s="85"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A171" s="95" t="s">
+        <v>69</v>
+      </c>
+      <c r="B171" s="76">
+        <v>10.021800000000001</v>
+      </c>
+      <c r="C171" s="76">
+        <v>-1E-4</v>
+      </c>
+      <c r="D171" s="76">
+        <v>-10.0009</v>
+      </c>
+      <c r="E171" s="55">
+        <v>-20.009399999999999</v>
+      </c>
+      <c r="F171" s="76"/>
+      <c r="G171" s="35"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A172" s="95" t="s">
+        <v>70</v>
+      </c>
+      <c r="B172" s="76">
+        <v>0.40789999999999998</v>
+      </c>
+      <c r="C172" s="76">
+        <v>0.41980000000000001</v>
+      </c>
+      <c r="D172" s="76">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="E172" s="55">
+        <v>0.41310000000000002</v>
+      </c>
+      <c r="F172" s="76"/>
+      <c r="G172" s="35"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A173" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="B173" s="9">
+        <v>8.0785</v>
+      </c>
+      <c r="C173" s="9">
+        <v>-0.36620000000000003</v>
+      </c>
+      <c r="D173" s="9">
+        <v>-10.040800000000001</v>
+      </c>
+      <c r="E173" s="30">
+        <v>-20.0139</v>
+      </c>
+      <c r="F173" s="9"/>
+      <c r="G173" s="35"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A174" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B174" s="9">
+        <v>0.4738</v>
+      </c>
+      <c r="C174" s="9">
+        <v>0.41570000000000001</v>
+      </c>
+      <c r="D174" s="9">
+        <v>0.42080000000000001</v>
+      </c>
+      <c r="E174" s="30">
+        <v>0.41360000000000002</v>
+      </c>
+      <c r="F174" s="9"/>
+      <c r="G174" s="35"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A175" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B175" s="9">
+        <v>6.2323000000000004</v>
+      </c>
+      <c r="C175" s="9">
+        <v>-0.8518</v>
+      </c>
+      <c r="D175" s="9">
+        <v>-10.102499999999999</v>
+      </c>
+      <c r="E175" s="30">
+        <v>-20.0198</v>
+      </c>
+      <c r="F175" s="9"/>
+      <c r="G175" s="35"/>
+    </row>
+    <row r="176" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A176" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B176" s="31">
+        <v>0.49349999999999999</v>
+      </c>
+      <c r="C176" s="31">
+        <v>0.41720000000000002</v>
+      </c>
+      <c r="D176" s="31">
+        <v>0.42209999999999998</v>
+      </c>
+      <c r="E176" s="32">
+        <v>0.41389999999999999</v>
+      </c>
+      <c r="F176" s="9"/>
+      <c r="G176" s="35"/>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A177" s="28"/>
+      <c r="B177" s="28"/>
+      <c r="C177" s="28"/>
+      <c r="D177" s="28"/>
+      <c r="E177" s="28"/>
+      <c r="F177" s="28"/>
+      <c r="G177" s="28"/>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A178" s="28"/>
+      <c r="B178" s="28"/>
+      <c r="C178" s="28"/>
+      <c r="D178" s="28"/>
+      <c r="E178" s="28"/>
+      <c r="F178" s="28"/>
+      <c r="G178" s="28"/>
+    </row>
+    <row r="179" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A179" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="B164" s="28"/>
-      <c r="C164" s="28"/>
-      <c r="D164" s="28"/>
-      <c r="E164" s="28"/>
-      <c r="F164" s="28"/>
-      <c r="G164" s="28"/>
-    </row>
-    <row r="165" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A165" s="28" t="s">
+      <c r="B179" s="28"/>
+      <c r="C179" s="28"/>
+      <c r="D179" s="28"/>
+      <c r="E179" s="28"/>
+      <c r="F179" s="28"/>
+      <c r="G179" s="28"/>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A180" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="B165" s="28"/>
-      <c r="C165" s="28"/>
-      <c r="D165" s="28"/>
-      <c r="E165" s="28"/>
-      <c r="F165" s="28"/>
-      <c r="G165" s="28"/>
-    </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A166" s="72" t="s">
-        <v>142</v>
-      </c>
-      <c r="B166" s="73">
+      <c r="B180" s="73">
         <v>-10</v>
       </c>
-      <c r="C166" s="73">
+      <c r="C180" s="73">
         <v>0</v>
       </c>
-      <c r="D166" s="73">
+      <c r="D180" s="73">
         <v>10</v>
       </c>
-      <c r="E166" s="94">
+      <c r="E180" s="73">
         <v>20</v>
       </c>
-      <c r="F166" s="85"/>
-      <c r="G166" s="85"/>
-    </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A167" s="95" t="s">
+      <c r="F180" s="94">
+        <v>30</v>
+      </c>
+      <c r="G180" s="28"/>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A181" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="B167" s="76">
-        <v>10.021800000000001</v>
-      </c>
-      <c r="C167" s="76">
-        <v>-1E-4</v>
-      </c>
-      <c r="D167" s="76">
-        <v>-10.0009</v>
-      </c>
-      <c r="E167" s="55">
-        <v>-20.009399999999999</v>
-      </c>
-      <c r="F167" s="76"/>
-      <c r="G167" s="35"/>
-    </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A168" s="95" t="s">
+      <c r="B181" s="76">
+        <v>9.9992999999999999</v>
+      </c>
+      <c r="C181" s="76">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="D181" s="76">
+        <v>-9.9928000000000008</v>
+      </c>
+      <c r="E181" s="76">
+        <v>-20.0136</v>
+      </c>
+      <c r="F181" s="55">
+        <v>-30.004000000000001</v>
+      </c>
+      <c r="G181" s="28"/>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A182" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="B168" s="76">
-        <v>0.40789999999999998</v>
-      </c>
-      <c r="C168" s="76">
-        <v>0.41980000000000001</v>
-      </c>
-      <c r="D168" s="76">
-        <v>0.42220000000000002</v>
-      </c>
-      <c r="E168" s="55">
-        <v>0.41310000000000002</v>
-      </c>
-      <c r="F168" s="76"/>
-      <c r="G168" s="35"/>
-    </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A169" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="B169" s="9">
-        <v>8.0785</v>
-      </c>
-      <c r="C169" s="9">
-        <v>-0.36620000000000003</v>
-      </c>
-      <c r="D169" s="9">
-        <v>-10.040800000000001</v>
-      </c>
-      <c r="E169" s="30">
-        <v>-20.0139</v>
-      </c>
-      <c r="F169" s="9"/>
-      <c r="G169" s="35"/>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A170" s="39" t="s">
+      <c r="B182" s="76">
+        <v>0.41639999999999999</v>
+      </c>
+      <c r="C182" s="76">
+        <v>0.4022</v>
+      </c>
+      <c r="D182" s="76">
+        <v>0.4098</v>
+      </c>
+      <c r="E182" s="76">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="F182" s="55">
+        <v>0.39079999999999998</v>
+      </c>
+      <c r="G182" s="28"/>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A183" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="B183" s="9">
+        <v>2.6894</v>
+      </c>
+      <c r="C183" s="9">
+        <v>-4.6473000000000004</v>
+      </c>
+      <c r="D183" s="9">
+        <v>-11.911799999999999</v>
+      </c>
+      <c r="E183" s="9">
+        <v>-20.385999999999999</v>
+      </c>
+      <c r="F183" s="30">
+        <v>-30.0456</v>
+      </c>
+      <c r="G183" s="28"/>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A184" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="B170" s="9">
-        <v>0.4738</v>
-      </c>
-      <c r="C170" s="9">
-        <v>0.41570000000000001</v>
-      </c>
-      <c r="D170" s="9">
-        <v>0.42080000000000001</v>
-      </c>
-      <c r="E170" s="30">
-        <v>0.41360000000000002</v>
-      </c>
-      <c r="F170" s="9"/>
-      <c r="G170" s="35"/>
-    </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A171" s="39" t="s">
+      <c r="B184" s="9">
+        <v>0.94330000000000003</v>
+      </c>
+      <c r="C184" s="9">
+        <v>0.70750000000000002</v>
+      </c>
+      <c r="D184" s="9">
+        <v>0.48320000000000002</v>
+      </c>
+      <c r="E184" s="9">
+        <v>0.42049999999999998</v>
+      </c>
+      <c r="F184" s="30">
+        <v>0.39340000000000003</v>
+      </c>
+      <c r="G184" s="28"/>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A185" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B171" s="9">
-        <v>6.2323000000000004</v>
-      </c>
-      <c r="C171" s="9">
-        <v>-0.8518</v>
-      </c>
-      <c r="D171" s="9">
-        <v>-10.102499999999999</v>
-      </c>
-      <c r="E171" s="30">
-        <v>-20.0198</v>
-      </c>
-      <c r="F171" s="9"/>
-      <c r="G171" s="35"/>
-    </row>
-    <row r="172" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A172" s="40" t="s">
+      <c r="B185" s="9">
+        <v>-1.7606999999999999</v>
+      </c>
+      <c r="C185" s="9">
+        <v>-8.1674000000000007</v>
+      </c>
+      <c r="D185" s="9">
+        <v>-13.776999999999999</v>
+      </c>
+      <c r="E185" s="9">
+        <v>-20.873999999999999</v>
+      </c>
+      <c r="F185" s="30">
+        <v>-30.104199999999999</v>
+      </c>
+      <c r="G185" s="28"/>
+    </row>
+    <row r="186" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A186" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B172" s="31">
-        <v>0.49349999999999999</v>
-      </c>
-      <c r="C172" s="31">
-        <v>0.41720000000000002</v>
-      </c>
-      <c r="D172" s="31">
-        <v>0.42209999999999998</v>
-      </c>
-      <c r="E172" s="32">
-        <v>0.41389999999999999</v>
-      </c>
-      <c r="F172" s="9"/>
-      <c r="G172" s="35"/>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A173" s="28"/>
-      <c r="B173" s="28"/>
-      <c r="C173" s="28"/>
-      <c r="D173" s="28"/>
-      <c r="E173" s="28"/>
-      <c r="F173" s="28"/>
-      <c r="G173" s="28"/>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A174" s="28"/>
-      <c r="B174" s="28"/>
-      <c r="C174" s="28"/>
-      <c r="D174" s="28"/>
-      <c r="E174" s="28"/>
-      <c r="F174" s="28"/>
-      <c r="G174" s="28"/>
-    </row>
-    <row r="175" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A175" s="28" t="s">
-        <v>145</v>
-      </c>
-      <c r="B175" s="28"/>
-      <c r="C175" s="28"/>
-      <c r="D175" s="28"/>
-      <c r="E175" s="28"/>
-      <c r="F175" s="28"/>
-      <c r="G175" s="28"/>
-    </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A176" s="72" t="s">
-        <v>142</v>
-      </c>
-      <c r="B176" s="73">
-        <v>-10</v>
-      </c>
-      <c r="C176" s="73">
-        <v>0</v>
-      </c>
-      <c r="D176" s="73">
-        <v>10</v>
-      </c>
-      <c r="E176" s="73">
-        <v>20</v>
-      </c>
-      <c r="F176" s="94">
-        <v>30</v>
-      </c>
-      <c r="G176" s="28"/>
-    </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A177" s="95" t="s">
+      <c r="B186" s="31">
+        <v>1.2151000000000001</v>
+      </c>
+      <c r="C186" s="31">
+        <v>0.77839999999999998</v>
+      </c>
+      <c r="D186" s="31">
+        <v>0.49209999999999998</v>
+      </c>
+      <c r="E186" s="31">
+        <v>0.41810000000000003</v>
+      </c>
+      <c r="F186" s="32">
+        <v>0.3926</v>
+      </c>
+      <c r="G186" s="28"/>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A187" s="28"/>
+      <c r="B187" s="28"/>
+      <c r="C187" s="28"/>
+      <c r="D187" s="28"/>
+      <c r="E187" s="28"/>
+      <c r="F187" s="28"/>
+      <c r="G187" s="28"/>
+    </row>
+    <row r="188" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A189" s="96" t="s">
         <v>69</v>
       </c>
-      <c r="B177" s="76">
-        <v>9.9992999999999999</v>
-      </c>
-      <c r="C177" s="76">
-        <v>9.2999999999999992E-3</v>
-      </c>
-      <c r="D177" s="76">
-        <v>-9.9928000000000008</v>
-      </c>
-      <c r="E177" s="76">
-        <v>-20.0136</v>
-      </c>
-      <c r="F177" s="55">
-        <v>-30.004000000000001</v>
-      </c>
-      <c r="G177" s="28"/>
-    </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A178" s="95" t="s">
+      <c r="B189" s="15"/>
+      <c r="C189" s="97">
+        <v>-8.1576000000000004</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A190" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="B178" s="76">
-        <v>0.41639999999999999</v>
-      </c>
-      <c r="C178" s="76">
-        <v>0.4022</v>
-      </c>
-      <c r="D178" s="76">
-        <v>0.4098</v>
-      </c>
-      <c r="E178" s="76">
-        <v>0.42599999999999999</v>
-      </c>
-      <c r="F178" s="55">
-        <v>0.39079999999999998</v>
-      </c>
-      <c r="G178" s="28"/>
-    </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A179" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="B179" s="9">
-        <v>2.6894</v>
-      </c>
-      <c r="C179" s="9">
-        <v>-4.6473000000000004</v>
-      </c>
-      <c r="D179" s="9">
-        <v>-11.911799999999999</v>
-      </c>
-      <c r="E179" s="9">
-        <v>-20.385999999999999</v>
-      </c>
-      <c r="F179" s="30">
-        <v>-30.0456</v>
-      </c>
-      <c r="G179" s="28"/>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A180" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="B180" s="9">
-        <v>0.94330000000000003</v>
-      </c>
-      <c r="C180" s="9">
-        <v>0.70750000000000002</v>
-      </c>
-      <c r="D180" s="9">
-        <v>0.48320000000000002</v>
-      </c>
-      <c r="E180" s="9">
-        <v>0.42049999999999998</v>
-      </c>
-      <c r="F180" s="30">
-        <v>0.39340000000000003</v>
-      </c>
-      <c r="G180" s="28"/>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A181" s="39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B181" s="9">
-        <v>-1.7606999999999999</v>
-      </c>
-      <c r="C181" s="9">
-        <v>-8.1674000000000007</v>
-      </c>
-      <c r="D181" s="9">
-        <v>-13.776999999999999</v>
-      </c>
-      <c r="E181" s="9">
-        <v>-20.873999999999999</v>
-      </c>
-      <c r="F181" s="30">
-        <v>-30.104199999999999</v>
-      </c>
-      <c r="G181" s="28"/>
-    </row>
-    <row r="182" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A182" s="40" t="s">
+      <c r="B190" s="21"/>
+      <c r="C190" s="98">
+        <v>0.40889999999999999</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A191" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="B191" s="21"/>
+      <c r="C191" s="98">
+        <v>-12.7606</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A192" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="B182" s="31">
-        <v>1.2151000000000001</v>
-      </c>
-      <c r="C182" s="31">
-        <v>0.77839999999999998</v>
-      </c>
-      <c r="D182" s="31">
-        <v>0.49209999999999998</v>
-      </c>
-      <c r="E182" s="31">
-        <v>0.41810000000000003</v>
-      </c>
-      <c r="F182" s="32">
-        <v>0.3926</v>
-      </c>
-      <c r="G182" s="28"/>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A183" s="28"/>
-      <c r="B183" s="28"/>
-      <c r="C183" s="28"/>
-      <c r="D183" s="28"/>
-      <c r="E183" s="28"/>
-      <c r="F183" s="28"/>
-      <c r="G183" s="28"/>
-    </row>
-    <row r="184" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A185" s="96" t="s">
-        <v>69</v>
-      </c>
-      <c r="B185" s="15"/>
-      <c r="C185" s="97">
-        <v>-8.1576000000000004</v>
-      </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A186" s="95" t="s">
-        <v>70</v>
-      </c>
-      <c r="B186" s="21"/>
-      <c r="C186" s="98">
-        <v>0.40889999999999999</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A187" s="39" t="s">
+      <c r="B192" s="21"/>
+      <c r="C192" s="98">
+        <v>0.50029999999999997</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A193" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="B187" s="21"/>
-      <c r="C187" s="98">
-        <v>-12.7606</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A188" s="39" t="s">
+      <c r="B193" s="21"/>
+      <c r="C193" s="98">
+        <v>-8.1062999999999992</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A194" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="B188" s="21"/>
-      <c r="C188" s="98">
-        <v>0.50029999999999997</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A189" s="39" t="s">
-        <v>153</v>
-      </c>
-      <c r="B189" s="21"/>
-      <c r="C189" s="98">
-        <v>-8.1062999999999992</v>
-      </c>
-    </row>
-    <row r="190" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A190" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="B190" s="24"/>
-      <c r="C190" s="99">
+      <c r="B194" s="24"/>
+      <c r="C194" s="99">
         <v>0.77159999999999995</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A191" s="21"/>
-      <c r="B191" s="21"/>
-      <c r="C191" s="21"/>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A195" s="21"/>
+      <c r="B195" s="21"/>
+      <c r="C195" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
@@ -4404,10 +4491,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FAE463-692A-4AB1-8AB9-770196756CC0}">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4420,12 +4507,12 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -4433,7 +4520,7 @@
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -4456,12 +4543,12 @@
         <v>6</v>
       </c>
       <c r="G4" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B5" s="63">
         <v>10.016999999999999</v>
@@ -4481,7 +4568,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B6" s="63">
         <v>0.33400000000000002</v>
@@ -4525,7 +4612,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B8" s="63">
         <v>1.0844</v>
@@ -4545,7 +4632,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B9" s="63">
         <v>-0.25769999999999998</v>
@@ -4565,7 +4652,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B10" s="63">
         <v>1.0732999999999999</v>
@@ -4585,7 +4672,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B11" s="63">
         <v>-3.8923999999999999</v>
@@ -4609,7 +4696,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B12" s="63">
         <v>0.99550000000000005</v>
@@ -4629,7 +4716,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B13" s="63">
         <v>-3.8243</v>
@@ -4649,7 +4736,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B14" s="9">
         <v>0.97599999999999998</v>
@@ -4669,7 +4756,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B15" s="9">
         <v>-2.3456000000000001</v>
@@ -4693,7 +4780,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B16" s="9">
         <v>0.94630000000000003</v>
@@ -4713,7 +4800,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B17" s="9">
         <v>-2.1879</v>
@@ -4733,7 +4820,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B18" s="9">
         <v>1.0165999999999999</v>
@@ -4753,7 +4840,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B19" s="9">
         <v>-2.3359999999999999</v>
@@ -4773,7 +4860,7 @@
     </row>
     <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B20" s="31">
         <v>1.0219</v>
@@ -4801,7 +4888,7 @@
     <row r="22" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A22" s="21"/>
       <c r="B22" s="100" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
@@ -4810,7 +4897,7 @@
     <row r="23" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A23" s="21"/>
       <c r="B23" s="100" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -4834,7 +4921,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B27" s="8">
         <f>68.7835264205932/200</f>
@@ -4852,22 +4939,22 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="65" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" s="66">
         <v>-10</v>
@@ -4888,12 +4975,12 @@
         <v>40</v>
       </c>
       <c r="H34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B35">
         <v>0.64659999999999995</v>
@@ -4916,7 +5003,7 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C36" s="19">
         <v>-10.0745</v>
@@ -4929,7 +5016,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C37" s="19">
         <v>0.19120000000000001</v>
@@ -4938,7 +5025,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B38" s="69">
         <v>3.8721999999999999</v>
@@ -4961,7 +5048,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39">
         <v>0.68859999999999999</v>
@@ -4984,7 +5071,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C40" s="19">
         <v>-10.035600000000001</v>
@@ -4997,7 +5084,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C41" s="19">
         <v>0.19500000000000001</v>
@@ -5006,7 +5093,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B42" s="69">
         <v>3.9794</v>
@@ -5029,7 +5116,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C43">
         <v>-5.3365</v>
@@ -5038,7 +5125,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C44">
         <v>-5.3365</v>
@@ -5047,7 +5134,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C45" s="28">
         <v>-11.2842</v>
@@ -5056,7 +5143,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C46">
         <v>-7.2462999999999997</v>
@@ -5065,7 +5152,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C47" s="19">
         <v>-2.3424</v>
@@ -5078,7 +5165,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C48" s="19">
         <v>9.2100000000000001E-2</v>
@@ -5087,10 +5174,10 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G49" s="23"/>
       <c r="H49" s="19">
@@ -5100,7 +5187,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C50" s="19">
         <v>0.32890000000000003</v>
@@ -5109,10 +5196,10 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C51" s="19" t="s">
         <v>168</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>170</v>
       </c>
       <c r="G51" s="23"/>
       <c r="H51" s="19">
@@ -5122,7 +5209,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C52" s="19">
         <v>0.30059999999999998</v>
@@ -5131,11 +5218,11 @@
     </row>
     <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B53" s="24"/>
       <c r="C53" s="103" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D53" s="24"/>
       <c r="E53" s="24"/>
@@ -5150,7 +5237,7 @@
     <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B56" s="91" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C56" s="92">
         <v>-15.4787</v>
@@ -5160,10 +5247,10 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B57" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" s="87" t="s">
         <v>127</v>
-      </c>
-      <c r="C57" s="87" t="s">
-        <v>128</v>
       </c>
       <c r="D57" s="28"/>
       <c r="E57" s="28"/>
@@ -5176,7 +5263,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B59" s="39" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C59" s="87">
         <v>-15.4361</v>
@@ -5186,10 +5273,10 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B60" s="39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C60" s="87" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D60" s="28"/>
       <c r="E60" s="28"/>
@@ -5202,7 +5289,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B62" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C62" s="87">
         <v>-26.090299999999999</v>
@@ -5212,10 +5299,10 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B63" s="39" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C63" s="87" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D63" s="28"/>
       <c r="E63" s="28"/>
@@ -5228,7 +5315,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B65" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C65" s="87">
         <v>-15.9239</v>
@@ -5238,17 +5325,17 @@
     </row>
     <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B66" s="40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C66" s="90" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D66" s="28"/>
       <c r="E66" s="28"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B67" s="86" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C67" s="86"/>
       <c r="D67" s="28"/>
@@ -5256,7 +5343,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B68" s="93" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C68" s="28"/>
       <c r="D68" s="28"/>
@@ -5264,7 +5351,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B69" s="39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C69" s="102">
         <v>-16.803100000000001</v>
@@ -5274,10 +5361,10 @@
     </row>
     <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B70" s="40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C70" s="90" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D70" s="28"/>
       <c r="E70" s="28"/>
@@ -5290,12 +5377,12 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B75" t="s">
         <v>0</v>
@@ -5303,7 +5390,7 @@
     </row>
     <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
@@ -5314,24 +5401,24 @@
         <v>50</v>
       </c>
       <c r="C77" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="D77" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="E77" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="D77" s="37" t="s">
+      <c r="F77" s="48" t="s">
         <v>180</v>
       </c>
-      <c r="E77" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="F77" s="48" t="s">
-        <v>182</v>
-      </c>
       <c r="G77" s="33" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" s="114" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B78" s="115">
         <v>6.5773000000000001</v>
@@ -5355,7 +5442,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" s="114" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B79" s="115">
         <v>0.76670000000000005</v>
@@ -5400,7 +5487,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B81" s="9">
         <v>4.1466000000000003</v>
@@ -5421,7 +5508,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="110" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B82" s="111">
         <v>24.7393</v>
@@ -5445,7 +5532,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A83" s="110" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B83" s="111">
         <v>4.3129999999999997</v>
@@ -5465,7 +5552,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B84" s="63"/>
       <c r="C84" s="101"/>
@@ -5475,7 +5562,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B85" s="9"/>
       <c r="C85" s="101"/>
@@ -5485,7 +5572,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B86" s="63"/>
       <c r="C86" s="101"/>
@@ -5495,7 +5582,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B87" s="9"/>
       <c r="C87" s="101"/>
@@ -5505,7 +5592,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="68" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B88" s="118">
         <v>21.093800000000002</v>
@@ -5520,7 +5607,7 @@
         <v>-17.941099999999999</v>
       </c>
       <c r="F88" s="120">
-        <v>-27.419599999999999</v>
+        <v>-27.476400000000002</v>
       </c>
       <c r="G88">
         <f>12.0926365852355/200</f>
@@ -5529,7 +5616,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="68" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B89" s="118">
         <v>2.9011</v>
@@ -5544,15 +5631,15 @@
         <v>1.7119</v>
       </c>
       <c r="F89" s="120">
-        <v>1.5708</v>
+        <v>1.5530999999999999</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B90" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="B90" s="9" t="s">
-        <v>195</v>
       </c>
       <c r="C90" s="101"/>
       <c r="D90" s="101">
@@ -5563,7 +5650,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B91" s="9"/>
       <c r="C91" s="101"/>
@@ -5575,7 +5662,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B92" s="9"/>
       <c r="C92" s="101"/>
@@ -5595,16 +5682,20 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A94" s="121" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B94" s="122">
-        <v>20.151</v>
+        <v>19.848700000000001</v>
       </c>
       <c r="C94" s="123">
         <v>6.1003999999999996</v>
       </c>
-      <c r="D94" s="123"/>
-      <c r="E94" s="123"/>
+      <c r="D94" s="123">
+        <v>-8.1217000000000006</v>
+      </c>
+      <c r="E94" s="123">
+        <v>-17.959700000000002</v>
+      </c>
       <c r="F94" s="124">
         <v>-27.630199999999999</v>
       </c>
@@ -5615,23 +5706,27 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="121" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B95" s="122">
-        <v>3.6435</v>
+        <v>4.1829999999999998</v>
       </c>
       <c r="C95" s="123">
         <v>6.6140999999999996</v>
       </c>
-      <c r="D95" s="123"/>
-      <c r="E95" s="123"/>
+      <c r="D95" s="123">
+        <v>1.5213000000000001</v>
+      </c>
+      <c r="E95" s="123">
+        <v>1.6759999999999999</v>
+      </c>
       <c r="F95" s="124">
         <v>1.5582</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B96" s="9"/>
       <c r="C96" s="101"/>
@@ -5641,7 +5736,7 @@
     </row>
     <row r="97" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B97" s="31"/>
       <c r="C97" s="107"/>
@@ -5658,42 +5753,39 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="14" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B102" s="37" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C102" s="48" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B103" s="63" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C103" s="104">
         <v>-1.1000000000000001E-3</v>
       </c>
-      <c r="D103" t="s">
-        <v>199</v>
-      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B104" s="63">
         <v>10.7</v>
@@ -5704,7 +5796,7 @@
     </row>
     <row r="105" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B105" s="108">
         <v>45.5</v>
@@ -5713,9 +5805,80 @@
         <v>60.37</v>
       </c>
     </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A106" s="125" t="s">
+        <v>198</v>
+      </c>
+    </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A109" s="127" t="s">
         <v>200</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A110" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B110" s="48" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A111" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B111" s="104">
+        <v>5.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A112" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B112" s="109">
+        <v>0.37640000000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A113" s="21"/>
+      <c r="B113" s="21"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A114" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B114" s="48" t="s">
+        <v>202</v>
+      </c>
+      <c r="C114" s="29" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A115" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B115" s="104">
+        <v>31.4848</v>
+      </c>
+      <c r="C115" s="29">
+        <v>25.6937</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A116" s="126" t="s">
+        <v>155</v>
+      </c>
+      <c r="B116" s="109">
+        <v>2.2843</v>
+      </c>
+      <c r="C116" s="29">
+        <v>2.0991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rnn train on randinit
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\RTSNet_Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{338902AB-0A30-4EC3-AAB9-2CA09808BAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72457A2-7550-42D7-A874-574C404C4E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="17020" windowHeight="10120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1462,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
update linear CV model
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\RTSNet_Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3CCBCB5-DAD9-4AAE-AB7C-6327EED7E947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0882699-7834-4D23-BAB1-CED757162DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,16 +863,16 @@
     <t>RTSNet (p) [dB]</t>
   </si>
   <si>
-    <t>MSE( train LOSS only on p)</t>
-  </si>
-  <si>
-    <t>MSE(CA model)</t>
-  </si>
-  <si>
-    <t>MSE mismatch(CV model)</t>
-  </si>
-  <si>
-    <t>MSE mismatch( train LOSS only on p)</t>
+    <t>MSE CA model (RTSNet train LOSS on (p,v,a))</t>
+  </si>
+  <si>
+    <t>MSE CV model (RTSNet train LOSS on (p,v,a))</t>
+  </si>
+  <si>
+    <t>MSE CA model ( train LOSS only on p)</t>
+  </si>
+  <si>
+    <t>MSE CV model (train LOSS only on p)</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1644,7 +1644,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1942,13 +1941,13 @@
   <dimension ref="A1:K326"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A273" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B286" sqref="B286"/>
+      <selection activeCell="C291" sqref="C291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="22.453125" customWidth="1"/>
-    <col min="2" max="2" width="27.1796875" customWidth="1"/>
+    <col min="2" max="2" width="34.54296875" customWidth="1"/>
     <col min="3" max="3" width="27.54296875" customWidth="1"/>
     <col min="4" max="4" width="27.81640625" customWidth="1"/>
     <col min="5" max="5" width="35.81640625" customWidth="1"/>
@@ -6465,20 +6464,20 @@
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A277" s="214"/>
-      <c r="B277" s="215" t="s">
+      <c r="A277" s="213"/>
+      <c r="B277" s="214" t="s">
+        <v>272</v>
+      </c>
+      <c r="C277" s="215" t="s">
         <v>273</v>
       </c>
-      <c r="C277" s="216" t="s">
+      <c r="D277" s="215" t="s">
         <v>274</v>
       </c>
-      <c r="D277" s="216" t="s">
-        <v>272</v>
-      </c>
-      <c r="E277" s="216" t="s">
+      <c r="E277" s="215" t="s">
         <v>275</v>
       </c>
-      <c r="F277" s="217" t="s">
+      <c r="F277" s="216" t="s">
         <v>207</v>
       </c>
     </row>
@@ -6489,11 +6488,11 @@
       <c r="B278" s="142">
         <v>-6.1893000000000002</v>
       </c>
-      <c r="C278" s="219"/>
-      <c r="D278" s="218" t="s">
+      <c r="C278" s="218"/>
+      <c r="D278" s="217" t="s">
         <v>45</v>
       </c>
-      <c r="E278" s="218" t="s">
+      <c r="E278" s="217" t="s">
         <v>45</v>
       </c>
       <c r="F278" s="164">
@@ -6508,9 +6507,9 @@
       <c r="B279" s="142">
         <v>2.4106999999999998</v>
       </c>
-      <c r="C279" s="219"/>
-      <c r="D279" s="218"/>
-      <c r="E279" s="218"/>
+      <c r="C279" s="218"/>
+      <c r="D279" s="217"/>
+      <c r="E279" s="217"/>
       <c r="F279" s="164"/>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.35">
@@ -6521,8 +6520,8 @@
         <v>-11.918900000000001</v>
       </c>
       <c r="C280" s="209"/>
-      <c r="D280" s="218"/>
-      <c r="E280" s="218"/>
+      <c r="D280" s="217"/>
+      <c r="E280" s="217"/>
       <c r="F280" s="164"/>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.35">
@@ -6533,8 +6532,8 @@
         <v>1.8574999999999999</v>
       </c>
       <c r="C281" s="209"/>
-      <c r="D281" s="218"/>
-      <c r="E281" s="218"/>
+      <c r="D281" s="217"/>
+      <c r="E281" s="217"/>
       <c r="F281" s="164"/>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.35">
@@ -6544,9 +6543,9 @@
       <c r="B282" s="144">
         <v>-7.2282000000000002</v>
       </c>
-      <c r="C282" s="219"/>
-      <c r="D282" s="218"/>
-      <c r="E282" s="218"/>
+      <c r="C282" s="218"/>
+      <c r="D282" s="217"/>
+      <c r="E282" s="217"/>
       <c r="F282" s="165">
         <f>191.359453678131/200</f>
         <v>0.95679726839065493</v>
@@ -6559,9 +6558,9 @@
       <c r="B283" s="144">
         <v>2.8020999999999998</v>
       </c>
-      <c r="C283" s="219"/>
-      <c r="D283" s="218"/>
-      <c r="E283" s="218"/>
+      <c r="C283" s="218"/>
+      <c r="D283" s="217"/>
+      <c r="E283" s="217"/>
       <c r="F283" s="165"/>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.35">
@@ -6572,8 +6571,8 @@
         <v>-17.249600000000001</v>
       </c>
       <c r="C284" s="210"/>
-      <c r="D284" s="218"/>
-      <c r="E284" s="218"/>
+      <c r="D284" s="217"/>
+      <c r="E284" s="217"/>
       <c r="F284" s="165"/>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.35">
@@ -6584,48 +6583,70 @@
         <v>2.9188999999999998</v>
       </c>
       <c r="C285" s="210"/>
-      <c r="D285" s="218"/>
-      <c r="E285" s="218"/>
+      <c r="D285" s="217"/>
+      <c r="E285" s="217"/>
       <c r="F285" s="165"/>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A286" s="104" t="s">
         <v>268</v>
       </c>
-      <c r="B286" s="146"/>
-      <c r="C286" s="211"/>
-      <c r="D286" s="211"/>
-      <c r="E286" s="219"/>
-      <c r="F286" s="167"/>
+      <c r="B286" s="191">
+        <v>-8.0685000000000002</v>
+      </c>
+      <c r="C286" s="218"/>
+      <c r="D286" s="190">
+        <v>-1.2093</v>
+      </c>
+      <c r="E286" s="217"/>
+      <c r="F286" s="167">
+        <f>41.4165632724761/200</f>
+        <v>0.20708281636238049</v>
+      </c>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A287" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="B287" s="146"/>
-      <c r="C287" s="211"/>
-      <c r="D287" s="211"/>
-      <c r="E287" s="219"/>
+      <c r="B287" s="191">
+        <v>2.8323</v>
+      </c>
+      <c r="C287" s="218"/>
+      <c r="D287" s="190">
+        <v>3.0486</v>
+      </c>
+      <c r="E287" s="217"/>
       <c r="F287" s="167"/>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A288" s="104" t="s">
         <v>271</v>
       </c>
-      <c r="B288" s="146"/>
-      <c r="C288" s="211"/>
-      <c r="D288" s="211"/>
-      <c r="E288" s="211"/>
-      <c r="F288" s="167"/>
+      <c r="B288" s="146">
+        <v>-16.597000000000001</v>
+      </c>
+      <c r="C288" s="218"/>
+      <c r="D288" s="191">
+        <v>-20.6538</v>
+      </c>
+      <c r="E288" s="190"/>
+      <c r="F288" s="167">
+        <f>42.804134607315/200</f>
+        <v>0.21402067303657499</v>
+      </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A289" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="B289" s="146"/>
-      <c r="C289" s="211"/>
-      <c r="D289" s="211"/>
-      <c r="E289" s="211"/>
+      <c r="B289" s="146">
+        <v>3.4449000000000001</v>
+      </c>
+      <c r="C289" s="218"/>
+      <c r="D289" s="191">
+        <v>3.1968999999999999</v>
+      </c>
+      <c r="E289" s="190"/>
       <c r="F289" s="167"/>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.35">
@@ -6633,9 +6654,9 @@
         <v>82</v>
       </c>
       <c r="B290" s="196"/>
-      <c r="C290" s="212"/>
-      <c r="D290" s="212"/>
-      <c r="E290" s="212"/>
+      <c r="C290" s="211"/>
+      <c r="D290" s="211"/>
+      <c r="E290" s="211"/>
       <c r="F290" s="207"/>
     </row>
     <row r="291" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6643,9 +6664,9 @@
         <v>83</v>
       </c>
       <c r="B291" s="80"/>
-      <c r="C291" s="213"/>
-      <c r="D291" s="213"/>
-      <c r="E291" s="213"/>
+      <c r="C291" s="212"/>
+      <c r="D291" s="212"/>
+      <c r="E291" s="212"/>
       <c r="F291" s="208"/>
     </row>
     <row r="299" spans="1:7" x14ac:dyDescent="0.35">
@@ -7047,10 +7068,10 @@
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="D278:D285"/>
-    <mergeCell ref="E278:E285"/>
     <mergeCell ref="C278:C279"/>
     <mergeCell ref="C282:C283"/>
-    <mergeCell ref="E286:E287"/>
+    <mergeCell ref="E278:E287"/>
+    <mergeCell ref="C286:C289"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8936,9 +8957,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9056,19 +9080,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F268FFC7-E0A8-474E-82F2-6EB808EA36C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BCF7BB-2741-482F-B9A7-38B0145EE962}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9090,9 +9110,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BCF7BB-2741-482F-B9A7-38B0145EE962}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F268FFC7-E0A8-474E-82F2-6EB808EA36C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update pendulum model, and test linearCA
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\RTSNet_Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA865E66-9B54-4A2D-8525-B2F4B6FAE60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09757B0-A085-4B51-8800-76C0256DB0E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -836,9 +836,6 @@
     <t>RTSNet[dB]</t>
   </si>
   <si>
-    <t>5) Decimation for linear(change data:9.23)</t>
-  </si>
-  <si>
     <t>Gaussian Random Init N(0,1),  dt=1e-2,   T=100,   H observe only position,   [r,q]=[0,0]dB,         [N_E,N_CV,N_T]=[1000,100,200]</t>
   </si>
   <si>
@@ -888,13 +885,16 @@
   </si>
   <si>
     <t># of parameters Hybrid</t>
+  </si>
+  <si>
+    <t>5) Decimation for linear(change data:10.21)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -971,14 +971,6 @@
       <color rgb="FF212121"/>
       <name val="Courier New"/>
       <family val="3"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1153,7 +1145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="224">
+  <cellXfs count="222">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1681,25 +1673,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1985,7 +1971,7 @@
   <dimension ref="A1:K328"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A275" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E285" sqref="E285"/>
+      <selection activeCell="E284" sqref="E284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6374,12 +6360,12 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A259" s="6" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
     </row>
     <row r="260" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A260" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.35">
@@ -6504,19 +6490,19 @@
     </row>
     <row r="276" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A276" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="277" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A277" s="210"/>
       <c r="B277" s="211" t="s">
+        <v>271</v>
+      </c>
+      <c r="C277" s="212" t="s">
         <v>272</v>
       </c>
-      <c r="C277" s="212" t="s">
+      <c r="D277" s="212" t="s">
         <v>273</v>
-      </c>
-      <c r="D277" s="212" t="s">
-        <v>274</v>
       </c>
       <c r="E277" s="213" t="s">
         <v>207</v>
@@ -6524,15 +6510,15 @@
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A278" s="102" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B278" s="142">
         <v>-6.1395999999999997</v>
       </c>
-      <c r="C278" s="217" t="s">
+      <c r="C278" s="219" t="s">
         <v>45</v>
       </c>
-      <c r="D278" s="221" t="s">
+      <c r="D278" s="220" t="s">
         <v>45</v>
       </c>
       <c r="E278" s="214">
@@ -6547,19 +6533,19 @@
       <c r="B279" s="142">
         <v>2.3812000000000002</v>
       </c>
-      <c r="C279" s="217"/>
-      <c r="D279" s="221"/>
+      <c r="C279" s="219"/>
+      <c r="D279" s="220"/>
       <c r="E279" s="214"/>
     </row>
     <row r="280" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A280" s="102" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B280" s="142">
         <v>-12.827199999999999</v>
       </c>
-      <c r="C280" s="217"/>
-      <c r="D280" s="222">
+      <c r="C280" s="219"/>
+      <c r="D280" s="217">
         <v>-9.1403999999999996</v>
       </c>
       <c r="E280" s="214">
@@ -6567,7 +6553,7 @@
         <v>9.7369945049285492E-3</v>
       </c>
       <c r="F280" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.35">
@@ -6577,21 +6563,21 @@
       <c r="B281" s="142">
         <v>2.0508000000000002</v>
       </c>
-      <c r="C281" s="217"/>
-      <c r="D281" s="222">
+      <c r="C281" s="219"/>
+      <c r="D281" s="217">
         <v>2.6225999999999998</v>
       </c>
       <c r="E281" s="214"/>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A282" s="103" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B282" s="144">
         <v>-7.1355000000000004</v>
       </c>
-      <c r="C282" s="217"/>
-      <c r="D282" s="221" t="s">
+      <c r="C282" s="219"/>
+      <c r="D282" s="220" t="s">
         <v>45</v>
       </c>
       <c r="E282" s="215">
@@ -6606,19 +6592,19 @@
       <c r="B283" s="144">
         <v>2.7795000000000001</v>
       </c>
-      <c r="C283" s="217"/>
-      <c r="D283" s="221"/>
+      <c r="C283" s="219"/>
+      <c r="D283" s="220"/>
       <c r="E283" s="215"/>
     </row>
     <row r="284" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A284" s="103" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B284" s="144">
         <v>-17.0809</v>
       </c>
-      <c r="C284" s="217"/>
-      <c r="D284" s="223">
+      <c r="C284" s="219"/>
+      <c r="D284" s="218">
         <v>-13.8697</v>
       </c>
       <c r="E284" s="215">
@@ -6626,7 +6612,7 @@
         <v>2.0461660623550402E-2</v>
       </c>
       <c r="F284" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.35">
@@ -6636,19 +6622,23 @@
       <c r="B285" s="144">
         <v>2.7237</v>
       </c>
-      <c r="C285" s="217"/>
-      <c r="D285" s="223">
+      <c r="C285" s="219"/>
+      <c r="D285" s="218">
         <v>2.4445999999999999</v>
       </c>
       <c r="E285" s="215"/>
     </row>
     <row r="286" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A286" s="104" t="s">
-        <v>268</v>
-      </c>
-      <c r="B286" s="191"/>
-      <c r="C286" s="190"/>
-      <c r="D286" s="221" t="s">
+        <v>267</v>
+      </c>
+      <c r="B286" s="191">
+        <v>-8.0848999999999993</v>
+      </c>
+      <c r="C286" s="190">
+        <v>-6.8231999999999999</v>
+      </c>
+      <c r="D286" s="220" t="s">
         <v>45</v>
       </c>
       <c r="E286" s="216">
@@ -6660,65 +6650,87 @@
       <c r="A287" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="B287" s="191"/>
-      <c r="C287" s="190"/>
-      <c r="D287" s="221"/>
+      <c r="B287" s="191">
+        <v>2.9264000000000001</v>
+      </c>
+      <c r="C287" s="190">
+        <v>3.2924000000000002</v>
+      </c>
+      <c r="D287" s="220"/>
       <c r="E287" s="216"/>
     </row>
     <row r="288" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A288" s="104" t="s">
-        <v>271</v>
-      </c>
-      <c r="B288" s="146"/>
-      <c r="C288" s="191"/>
-      <c r="D288" s="219"/>
+        <v>270</v>
+      </c>
+      <c r="B288" s="146">
+        <v>-16.892900000000001</v>
+      </c>
+      <c r="C288" s="191">
+        <v>-19.7288</v>
+      </c>
+      <c r="D288" s="146">
+        <v>-14.8301</v>
+      </c>
       <c r="E288" s="216">
         <f>44.0292124748229/200</f>
         <v>0.22014606237411499</v>
       </c>
       <c r="F288" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="289" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A289" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="B289" s="146"/>
-      <c r="C289" s="191"/>
-      <c r="D289" s="219"/>
+      <c r="B289" s="146">
+        <v>2.8605</v>
+      </c>
+      <c r="C289" s="191">
+        <v>3.2919999999999998</v>
+      </c>
+      <c r="D289" s="146">
+        <v>2.0205000000000002</v>
+      </c>
       <c r="E289" s="167"/>
     </row>
     <row r="290" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A290" s="104" t="s">
-        <v>279</v>
-      </c>
-      <c r="B290" s="146"/>
-      <c r="C290" s="146"/>
-      <c r="D290" s="220"/>
+        <v>278</v>
+      </c>
+      <c r="B290" s="146">
+        <v>17010</v>
+      </c>
+      <c r="C290" s="146">
+        <v>17010</v>
+      </c>
+      <c r="D290" s="191">
+        <v>4385</v>
+      </c>
       <c r="E290" s="167"/>
     </row>
     <row r="291" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A291" s="76" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B291" s="196"/>
       <c r="C291" s="209"/>
-      <c r="D291" s="218"/>
+      <c r="D291" s="221"/>
       <c r="E291" s="207"/>
     </row>
     <row r="292" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A292" s="76" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B292" s="196"/>
       <c r="C292" s="209"/>
-      <c r="D292" s="218"/>
+      <c r="D292" s="221"/>
       <c r="E292" s="207"/>
     </row>
     <row r="293" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A293" s="76" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B293" s="196"/>
       <c r="C293" s="209"/>
@@ -6727,7 +6739,7 @@
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A294" s="76" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B294" s="196"/>
       <c r="C294" s="209"/>
@@ -6736,17 +6748,15 @@
     </row>
     <row r="295" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A295" s="79" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B295" s="80">
-        <v>41236</v>
+        <v>40948</v>
       </c>
       <c r="C295" s="80">
-        <v>41236</v>
-      </c>
-      <c r="D295" s="80">
-        <v>41236</v>
-      </c>
+        <v>40948</v>
+      </c>
+      <c r="D295" s="80"/>
       <c r="E295" s="208"/>
     </row>
     <row r="301" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update 2 pass for CA case
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\RTSNet_Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91890CFF-71AD-4923-BCDD-56DB35C97296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E003CC47-FB2A-42B3-B25B-888519A8AB7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="301">
   <si>
     <t>1) Full info, RTSNet converges to RTS</t>
   </si>
@@ -891,13 +891,70 @@
   </si>
   <si>
     <t>CV model (train LOSS only on p)</t>
+  </si>
+  <si>
+    <t>Known Gaussian Random Init N(0,1),  T=100,   H observe only position,   [r,q]=[0,0]dB,         [N_E,N_CV,N_T]=[1000,100,200] (change date: Nov.11 mark blue)</t>
+  </si>
+  <si>
+    <t>dt = 1</t>
+  </si>
+  <si>
+    <t>CA (RTSNet train LOSS on (p,v,a))</t>
+  </si>
+  <si>
+    <t>CA ( train LOSS only on p)</t>
+  </si>
+  <si>
+    <t>CV (train LOSS only on p)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Hybrid Model of Q </t>
+  </si>
+  <si>
+    <t>-8.0957 | -7.6261</t>
+  </si>
+  <si>
+    <t>2.9375 | 2.9337</t>
+  </si>
+  <si>
+    <t>-17.5268 | -15.7456</t>
+  </si>
+  <si>
+    <t>2.6402 | 2.2260</t>
+  </si>
+  <si>
+    <t>Q_diag=[dt/3 dt 3dt] | Q_diag=[dt dt dt]</t>
+  </si>
+  <si>
+    <t>-9.5829 | -10.6739</t>
+  </si>
+  <si>
+    <t>2.0942 | 1.7024</t>
+  </si>
+  <si>
+    <t>20.8838 | 20.8978</t>
+  </si>
+  <si>
+    <t>2.1715 | 2.1728</t>
+  </si>
+  <si>
+    <t>14.3506 | 18.1843</t>
+  </si>
+  <si>
+    <t>2.0113 | 2.7958</t>
+  </si>
+  <si>
+    <t>-11.4561 | -8.8031</t>
+  </si>
+  <si>
+    <t>2.0368 | 1.8078</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -978,6 +1035,29 @@
     <font>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1155,7 +1235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="264">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1667,7 +1747,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1683,12 +1762,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1696,6 +1769,99 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1990,10 +2156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K352"/>
+  <dimension ref="A1:K398"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A275" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B289" sqref="B289"/>
+    <sheetView tabSelected="1" topLeftCell="A293" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C307" sqref="C307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6516,17 +6682,17 @@
       </c>
     </row>
     <row r="278" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A278" s="210"/>
-      <c r="B278" s="211" t="s">
+      <c r="A278" s="209"/>
+      <c r="B278" s="210" t="s">
         <v>279</v>
       </c>
-      <c r="C278" s="212" t="s">
+      <c r="C278" s="211" t="s">
         <v>280</v>
       </c>
-      <c r="D278" s="212" t="s">
+      <c r="D278" s="211" t="s">
         <v>281</v>
       </c>
-      <c r="E278" s="213" t="s">
+      <c r="E278" s="212" t="s">
         <v>207</v>
       </c>
     </row>
@@ -6534,16 +6700,16 @@
       <c r="A279" s="102" t="s">
         <v>263</v>
       </c>
-      <c r="B279" s="220">
+      <c r="B279" s="142">
         <v>-7.6313000000000004</v>
       </c>
-      <c r="C279" s="222" t="s">
+      <c r="C279" s="260" t="s">
         <v>45</v>
       </c>
-      <c r="D279" s="223" t="s">
+      <c r="D279" s="261" t="s">
         <v>45</v>
       </c>
-      <c r="E279" s="214">
+      <c r="E279" s="213">
         <f>1.98006391525268/200</f>
         <v>9.9003195762633993E-3</v>
       </c>
@@ -6552,25 +6718,25 @@
       <c r="A280" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B280" s="220">
+      <c r="B280" s="142">
         <v>2.891</v>
       </c>
-      <c r="C280" s="222"/>
-      <c r="D280" s="223"/>
-      <c r="E280" s="214"/>
+      <c r="C280" s="260"/>
+      <c r="D280" s="261"/>
+      <c r="E280" s="213"/>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A281" s="102" t="s">
         <v>266</v>
       </c>
-      <c r="B281" s="220">
+      <c r="B281" s="142">
         <v>-22.074200000000001</v>
       </c>
-      <c r="C281" s="222"/>
-      <c r="D281" s="220">
+      <c r="C281" s="260"/>
+      <c r="D281" s="142">
         <v>-7.6565000000000003</v>
       </c>
-      <c r="E281" s="214">
+      <c r="E281" s="213">
         <f>1.94739890098571/200</f>
         <v>9.7369945049285492E-3</v>
       </c>
@@ -6582,54 +6748,54 @@
       <c r="A282" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B282" s="220">
+      <c r="B282" s="142">
         <v>3.6943999999999999</v>
       </c>
-      <c r="C282" s="222"/>
-      <c r="D282" s="220">
+      <c r="C282" s="260"/>
+      <c r="D282" s="142">
         <v>3.1446000000000001</v>
       </c>
-      <c r="E282" s="214"/>
+      <c r="E282" s="213"/>
     </row>
     <row r="283" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A283" s="103" t="s">
         <v>264</v>
       </c>
-      <c r="B283" s="221">
+      <c r="B283" s="218">
         <v>-8.7913999999999994</v>
       </c>
-      <c r="C283" s="222"/>
-      <c r="D283" s="223" t="s">
+      <c r="C283" s="260"/>
+      <c r="D283" s="261" t="s">
         <v>45</v>
       </c>
-      <c r="E283" s="215">
+      <c r="E283" s="214">
         <f>4.15544414520263/200</f>
         <v>2.0777220726013148E-2</v>
       </c>
     </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A284" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="B284" s="221">
+      <c r="B284" s="218">
         <v>3.0541</v>
       </c>
-      <c r="C284" s="222"/>
-      <c r="D284" s="223"/>
-      <c r="E284" s="215"/>
+      <c r="C284" s="260"/>
+      <c r="D284" s="261"/>
+      <c r="E284" s="214"/>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A285" s="103" t="s">
         <v>267</v>
       </c>
-      <c r="B285" s="221">
+      <c r="B285" s="218">
         <v>-23.220700000000001</v>
       </c>
-      <c r="C285" s="222"/>
-      <c r="D285" s="221">
+      <c r="C285" s="260"/>
+      <c r="D285" s="218">
         <v>-14.7516</v>
       </c>
-      <c r="E285" s="215">
+      <c r="E285" s="214">
         <f>4.09233212471008/200</f>
         <v>2.0461660623550402E-2</v>
       </c>
@@ -6641,29 +6807,29 @@
       <c r="A286" s="103" t="s">
         <v>14</v>
       </c>
-      <c r="B286" s="221">
+      <c r="B286" s="218">
         <v>4.0807000000000002</v>
       </c>
-      <c r="C286" s="222"/>
-      <c r="D286" s="221">
+      <c r="C286" s="260"/>
+      <c r="D286" s="218">
         <v>3.3081</v>
       </c>
-      <c r="E286" s="215"/>
+      <c r="E286" s="214"/>
     </row>
     <row r="287" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A287" s="104" t="s">
         <v>265</v>
       </c>
-      <c r="B287" s="146">
+      <c r="B287" s="255">
         <v>-8.0848999999999993</v>
       </c>
-      <c r="C287" s="219">
+      <c r="C287" s="146">
         <v>-6.4104000000000001</v>
       </c>
-      <c r="D287" s="225" t="s">
+      <c r="D287" s="263" t="s">
         <v>45</v>
       </c>
-      <c r="E287" s="216">
+      <c r="E287" s="215">
         <f>41.4165632724761/200</f>
         <v>0.20708281636238049</v>
       </c>
@@ -6672,14 +6838,14 @@
       <c r="A288" s="104" t="s">
         <v>16</v>
       </c>
-      <c r="B288" s="146">
+      <c r="B288" s="255">
         <v>2.9264000000000001</v>
       </c>
-      <c r="C288" s="219">
+      <c r="C288" s="146">
         <v>3.2963</v>
       </c>
-      <c r="D288" s="225"/>
-      <c r="E288" s="216"/>
+      <c r="D288" s="263"/>
+      <c r="E288" s="215"/>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A289" s="104" t="s">
@@ -6688,13 +6854,13 @@
       <c r="B289" s="146">
         <v>-16.892900000000001</v>
       </c>
-      <c r="C289" s="219">
+      <c r="C289" s="216">
         <v>-21.4907</v>
       </c>
-      <c r="D289" s="146">
-        <v>-14.8301</v>
-      </c>
-      <c r="E289" s="216">
+      <c r="D289" s="219">
+        <v>-15.788399999999999</v>
+      </c>
+      <c r="E289" s="215">
         <f>44.0292124748229/200</f>
         <v>0.22014606237411449</v>
       </c>
@@ -6709,11 +6875,11 @@
       <c r="B290" s="146">
         <v>2.8605</v>
       </c>
-      <c r="C290" s="219">
+      <c r="C290" s="216">
         <v>3.6055999999999999</v>
       </c>
-      <c r="D290" s="146">
-        <v>2.0205000000000002</v>
+      <c r="D290" s="216">
+        <v>2.5225</v>
       </c>
       <c r="E290" s="167"/>
     </row>
@@ -6736,36 +6902,65 @@
       <c r="A292" s="76" t="s">
         <v>269</v>
       </c>
-      <c r="B292" s="196"/>
-      <c r="C292" s="209"/>
-      <c r="D292" s="224"/>
-      <c r="E292" s="207"/>
+      <c r="B292" s="196">
+        <v>17.337299999999999</v>
+      </c>
+      <c r="C292" s="192">
+        <v>20.891200000000001</v>
+      </c>
+      <c r="D292" s="262"/>
+      <c r="E292" s="207">
+        <f>26.5463798046112/200</f>
+        <v>0.13273189902305599</v>
+      </c>
     </row>
     <row r="293" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A293" s="76" t="s">
         <v>270</v>
       </c>
-      <c r="B293" s="196"/>
-      <c r="C293" s="209"/>
-      <c r="D293" s="224"/>
+      <c r="B293" s="196">
+        <v>2.2875000000000001</v>
+      </c>
+      <c r="C293" s="192">
+        <v>2.1716000000000002</v>
+      </c>
+      <c r="D293" s="262"/>
       <c r="E293" s="207"/>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A294" s="76" t="s">
         <v>271</v>
       </c>
-      <c r="B294" s="196"/>
-      <c r="C294" s="209"/>
-      <c r="D294" s="209"/>
-      <c r="E294" s="207"/>
+      <c r="B294" s="196">
+        <v>-11.1662</v>
+      </c>
+      <c r="C294" s="220">
+        <v>-10.2974</v>
+      </c>
+      <c r="D294" s="220">
+        <v>-7.9599000000000002</v>
+      </c>
+      <c r="E294" s="207">
+        <f>26.4315013885498/200</f>
+        <v>0.132157506942749</v>
+      </c>
+      <c r="F294" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="295" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A295" s="76" t="s">
         <v>270</v>
       </c>
-      <c r="B295" s="196"/>
-      <c r="C295" s="209"/>
-      <c r="D295" s="209"/>
+      <c r="B295" s="196">
+        <v>1.9853000000000001</v>
+      </c>
+      <c r="C295" s="192">
+        <v>1.9888999999999999</v>
+      </c>
+      <c r="D295" s="192">
+        <v>1.6473</v>
+      </c>
       <c r="E295" s="207"/>
     </row>
     <row r="296" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -6773,659 +6968,1195 @@
         <v>274</v>
       </c>
       <c r="B296" s="80">
-        <v>40948</v>
+        <v>41719</v>
       </c>
       <c r="C296" s="80">
-        <v>40948</v>
-      </c>
-      <c r="D296" s="80"/>
+        <v>41719</v>
+      </c>
+      <c r="D296" s="80">
+        <v>41333</v>
+      </c>
       <c r="E296" s="208"/>
     </row>
-    <row r="297" spans="1:6" ht="24.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="299" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A299" t="s">
+    <row r="297" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A297" s="254" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A298" s="209"/>
+      <c r="B298" s="210" t="s">
+        <v>284</v>
+      </c>
+      <c r="C298" s="210" t="s">
+        <v>285</v>
+      </c>
+      <c r="D298" s="210" t="s">
+        <v>286</v>
+      </c>
+      <c r="E298" s="212" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A299" s="102" t="s">
+        <v>263</v>
+      </c>
+      <c r="B299" s="217"/>
+      <c r="C299" s="260" t="s">
+        <v>45</v>
+      </c>
+      <c r="D299" s="261" t="s">
+        <v>45</v>
+      </c>
+      <c r="E299" s="213">
+        <f>1.98006391525268/200</f>
+        <v>9.9003195762633993E-3</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A300" s="102" t="s">
+        <v>12</v>
+      </c>
+      <c r="B300" s="217"/>
+      <c r="C300" s="260"/>
+      <c r="D300" s="261"/>
+      <c r="E300" s="213"/>
+    </row>
+    <row r="301" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A301" s="102" t="s">
+        <v>266</v>
+      </c>
+      <c r="B301" s="217"/>
+      <c r="C301" s="260"/>
+      <c r="D301" s="217"/>
+      <c r="E301" s="213">
+        <f>1.94739890098571/200</f>
+        <v>9.7369945049285492E-3</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A302" s="102" t="s">
+        <v>12</v>
+      </c>
+      <c r="B302" s="217" t="s">
+        <v>292</v>
+      </c>
+      <c r="C302" s="260"/>
+      <c r="D302" s="217"/>
+      <c r="E302" s="213"/>
+    </row>
+    <row r="303" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A303" s="103" t="s">
+        <v>264</v>
+      </c>
+      <c r="B303" s="256" t="s">
+        <v>288</v>
+      </c>
+      <c r="C303" s="260"/>
+      <c r="D303" s="261" t="s">
+        <v>45</v>
+      </c>
+      <c r="E303" s="214">
+        <f>4.15544414520263/200</f>
+        <v>2.0777220726013148E-2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A304" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="B304" s="256" t="s">
+        <v>289</v>
+      </c>
+      <c r="C304" s="260"/>
+      <c r="D304" s="261"/>
+      <c r="E304" s="214"/>
+    </row>
+    <row r="305" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A305" s="103" t="s">
+        <v>267</v>
+      </c>
+      <c r="B305" s="256" t="s">
+        <v>290</v>
+      </c>
+      <c r="C305" s="260"/>
+      <c r="D305" s="218">
+        <v>-14.926600000000001</v>
+      </c>
+      <c r="E305" s="214">
+        <f>4.09233212471008/200</f>
+        <v>2.0461660623550402E-2</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A306" s="103" t="s">
+        <v>14</v>
+      </c>
+      <c r="B306" s="256" t="s">
+        <v>291</v>
+      </c>
+      <c r="C306" s="260"/>
+      <c r="D306" s="218">
+        <v>2.1204999999999998</v>
+      </c>
+      <c r="E306" s="214"/>
+    </row>
+    <row r="307" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A307" s="76" t="s">
+        <v>269</v>
+      </c>
+      <c r="B307" s="220" t="s">
+        <v>297</v>
+      </c>
+      <c r="C307" s="220" t="s">
+        <v>295</v>
+      </c>
+      <c r="D307" s="262"/>
+      <c r="E307" s="207">
+        <f>26.5463798046112/200</f>
+        <v>0.13273189902305599</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A308" s="76" t="s">
+        <v>270</v>
+      </c>
+      <c r="B308" s="220" t="s">
+        <v>298</v>
+      </c>
+      <c r="C308" s="220" t="s">
+        <v>296</v>
+      </c>
+      <c r="D308" s="262"/>
+      <c r="E308" s="207"/>
+    </row>
+    <row r="309" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A309" s="76" t="s">
+        <v>271</v>
+      </c>
+      <c r="B309" s="220" t="s">
+        <v>299</v>
+      </c>
+      <c r="C309" s="220" t="s">
+        <v>293</v>
+      </c>
+      <c r="D309" s="220">
+        <v>-10.732200000000001</v>
+      </c>
+      <c r="E309" s="207">
+        <f>26.4315013885498/200</f>
+        <v>0.132157506942749</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A310" s="76" t="s">
+        <v>270</v>
+      </c>
+      <c r="B310" s="220" t="s">
+        <v>300</v>
+      </c>
+      <c r="C310" s="220" t="s">
+        <v>294</v>
+      </c>
+      <c r="D310" s="192">
+        <v>1.6614</v>
+      </c>
+      <c r="E310" s="207"/>
+    </row>
+    <row r="311" spans="1:6" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A311" s="79" t="s">
+        <v>274</v>
+      </c>
+      <c r="B311" s="80">
+        <v>41719</v>
+      </c>
+      <c r="C311" s="80">
+        <v>41719</v>
+      </c>
+      <c r="D311" s="80">
+        <v>41333</v>
+      </c>
+      <c r="E311" s="208"/>
+    </row>
+    <row r="312" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D312" s="138"/>
+      <c r="E312" s="138"/>
+      <c r="F312" s="138"/>
+    </row>
+    <row r="313" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D313" s="138"/>
+      <c r="E313" s="138"/>
+      <c r="F313" s="138"/>
+    </row>
+    <row r="314" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D314" s="138"/>
+      <c r="E314" s="138"/>
+      <c r="F314" s="138"/>
+    </row>
+    <row r="315" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="316" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A318" s="221" t="s">
+        <v>282</v>
+      </c>
+      <c r="B318" s="221"/>
+      <c r="C318" s="221"/>
+      <c r="D318" s="221"/>
+      <c r="E318" s="221"/>
+      <c r="F318" s="221"/>
+    </row>
+    <row r="319" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A319" s="222" t="s">
+        <v>283</v>
+      </c>
+      <c r="B319" s="221"/>
+      <c r="C319" s="221"/>
+      <c r="D319" s="221"/>
+      <c r="E319" s="221"/>
+      <c r="F319" s="221"/>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A320" s="223"/>
+      <c r="B320" s="224" t="s">
+        <v>279</v>
+      </c>
+      <c r="C320" s="225" t="s">
+        <v>280</v>
+      </c>
+      <c r="D320" s="225" t="s">
+        <v>281</v>
+      </c>
+      <c r="E320" s="226" t="s">
+        <v>207</v>
+      </c>
+      <c r="F320" s="221"/>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A321" s="227" t="s">
+        <v>263</v>
+      </c>
+      <c r="B321" s="228">
+        <v>1.4617</v>
+      </c>
+      <c r="C321" s="257" t="s">
+        <v>45</v>
+      </c>
+      <c r="D321" s="257" t="s">
+        <v>45</v>
+      </c>
+      <c r="E321" s="229">
+        <f>1.98006391525268/200</f>
+        <v>9.9003195762633993E-3</v>
+      </c>
+      <c r="F321" s="221"/>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A322" s="227" t="s">
+        <v>12</v>
+      </c>
+      <c r="B322" s="228">
+        <v>0.57669999999999999</v>
+      </c>
+      <c r="C322" s="257"/>
+      <c r="D322" s="257"/>
+      <c r="E322" s="229"/>
+      <c r="F322" s="221"/>
+    </row>
+    <row r="323" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A323" s="227" t="s">
+        <v>266</v>
+      </c>
+      <c r="B323" s="228"/>
+      <c r="C323" s="257"/>
+      <c r="D323" s="230"/>
+      <c r="E323" s="229">
+        <f>1.94739890098571/200</f>
+        <v>9.7369945049285492E-3</v>
+      </c>
+      <c r="F323" s="221" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A324" s="227" t="s">
+        <v>12</v>
+      </c>
+      <c r="B324" s="228"/>
+      <c r="C324" s="257"/>
+      <c r="D324" s="230"/>
+      <c r="E324" s="229"/>
+      <c r="F324" s="221"/>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A325" s="231" t="s">
+        <v>264</v>
+      </c>
+      <c r="B325" s="232">
+        <v>-5.4771999999999998</v>
+      </c>
+      <c r="C325" s="257"/>
+      <c r="D325" s="257" t="s">
+        <v>45</v>
+      </c>
+      <c r="E325" s="233">
+        <f>4.15544414520263/200</f>
+        <v>2.0777220726013148E-2</v>
+      </c>
+      <c r="F325" s="221"/>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A326" s="231" t="s">
+        <v>14</v>
+      </c>
+      <c r="B326" s="232">
+        <v>0.625</v>
+      </c>
+      <c r="C326" s="257"/>
+      <c r="D326" s="257"/>
+      <c r="E326" s="233"/>
+      <c r="F326" s="221"/>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A327" s="231" t="s">
+        <v>267</v>
+      </c>
+      <c r="B327" s="232"/>
+      <c r="C327" s="257"/>
+      <c r="D327" s="234"/>
+      <c r="E327" s="233">
+        <f>4.09233212471008/200</f>
+        <v>2.0461660623550402E-2</v>
+      </c>
+      <c r="F327" s="221" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A328" s="231" t="s">
+        <v>14</v>
+      </c>
+      <c r="B328" s="232"/>
+      <c r="C328" s="257"/>
+      <c r="D328" s="234"/>
+      <c r="E328" s="233"/>
+      <c r="F328" s="221"/>
+    </row>
+    <row r="329" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A329" s="235" t="s">
+        <v>265</v>
+      </c>
+      <c r="B329" s="236"/>
+      <c r="C329" s="237"/>
+      <c r="D329" s="258" t="s">
+        <v>45</v>
+      </c>
+      <c r="E329" s="238">
+        <f>41.4165632724761/200</f>
+        <v>0.20708281636238049</v>
+      </c>
+      <c r="F329" s="221"/>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A330" s="235" t="s">
+        <v>16</v>
+      </c>
+      <c r="B330" s="236"/>
+      <c r="C330" s="237"/>
+      <c r="D330" s="258"/>
+      <c r="E330" s="238"/>
+      <c r="F330" s="221"/>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A331" s="235" t="s">
+        <v>268</v>
+      </c>
+      <c r="B331" s="236"/>
+      <c r="C331" s="237"/>
+      <c r="D331" s="239"/>
+      <c r="E331" s="238">
+        <f>44.0292124748229/200</f>
+        <v>0.22014606237411449</v>
+      </c>
+      <c r="F331" s="221" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A332" s="235" t="s">
+        <v>16</v>
+      </c>
+      <c r="B332" s="236"/>
+      <c r="C332" s="237"/>
+      <c r="D332" s="237"/>
+      <c r="E332" s="240"/>
+      <c r="F332" s="221"/>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A333" s="235" t="s">
+        <v>273</v>
+      </c>
+      <c r="B333" s="236">
+        <v>17010</v>
+      </c>
+      <c r="C333" s="236">
+        <v>17010</v>
+      </c>
+      <c r="D333" s="236">
+        <v>4385</v>
+      </c>
+      <c r="E333" s="240"/>
+      <c r="F333" s="221"/>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A334" s="241" t="s">
+        <v>269</v>
+      </c>
+      <c r="B334" s="242">
+        <v>27.1051</v>
+      </c>
+      <c r="C334" s="243"/>
+      <c r="D334" s="259"/>
+      <c r="E334" s="244"/>
+      <c r="F334" s="221"/>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A335" s="241" t="s">
+        <v>270</v>
+      </c>
+      <c r="B335" s="242">
+        <v>2.4712000000000001</v>
+      </c>
+      <c r="C335" s="243"/>
+      <c r="D335" s="259"/>
+      <c r="E335" s="244"/>
+      <c r="F335" s="221"/>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A336" s="241" t="s">
+        <v>271</v>
+      </c>
+      <c r="B336" s="242"/>
+      <c r="C336" s="245"/>
+      <c r="D336" s="243"/>
+      <c r="E336" s="244"/>
+      <c r="F336" s="221"/>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A337" s="241" t="s">
+        <v>270</v>
+      </c>
+      <c r="B337" s="242"/>
+      <c r="C337" s="246"/>
+      <c r="D337" s="243"/>
+      <c r="E337" s="244"/>
+      <c r="F337" s="221"/>
+    </row>
+    <row r="338" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A338" s="247" t="s">
+        <v>274</v>
+      </c>
+      <c r="B338" s="248">
+        <v>41719</v>
+      </c>
+      <c r="C338" s="248"/>
+      <c r="D338" s="248"/>
+      <c r="E338" s="249"/>
+      <c r="F338" s="221"/>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A339" s="221"/>
+      <c r="B339" s="221"/>
+      <c r="C339" s="221"/>
+      <c r="D339" s="221"/>
+      <c r="E339" s="221"/>
+      <c r="F339" s="221"/>
+    </row>
+    <row r="341" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="342" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="343" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="345" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A345" s="221" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A300" s="210"/>
-      <c r="B300" s="211" t="s">
+      <c r="B345" s="221"/>
+      <c r="C345" s="221"/>
+      <c r="D345" s="221"/>
+      <c r="E345" s="221"/>
+      <c r="F345" s="221"/>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A346" s="223"/>
+      <c r="B346" s="224" t="s">
         <v>279</v>
       </c>
-      <c r="C300" s="212" t="s">
+      <c r="C346" s="225" t="s">
         <v>280</v>
       </c>
-      <c r="D300" s="212" t="s">
+      <c r="D346" s="225" t="s">
         <v>281</v>
       </c>
-      <c r="E300" s="213" t="s">
+      <c r="E346" s="226" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A301" s="102" t="s">
+      <c r="F346" s="221"/>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A347" s="227" t="s">
         <v>263</v>
       </c>
-      <c r="B301" s="142">
+      <c r="B347" s="228">
         <v>18.8626</v>
       </c>
-      <c r="C301" s="222"/>
-      <c r="D301" s="223"/>
-      <c r="E301" s="214">
+      <c r="C347" s="257"/>
+      <c r="D347" s="257"/>
+      <c r="E347" s="229">
         <f>2.00304269790649/200</f>
         <v>1.0015213489532451E-2</v>
       </c>
-    </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A302" s="102" t="s">
+      <c r="F347" s="221"/>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A348" s="227" t="s">
         <v>12</v>
       </c>
-      <c r="B302" s="142">
+      <c r="B348" s="228">
         <v>1.7168000000000001</v>
       </c>
-      <c r="C302" s="222"/>
-      <c r="D302" s="223"/>
-      <c r="E302" s="214"/>
-    </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A303" s="102" t="s">
+      <c r="C348" s="257"/>
+      <c r="D348" s="257"/>
+      <c r="E348" s="229"/>
+      <c r="F348" s="221"/>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A349" s="227" t="s">
         <v>266</v>
       </c>
-      <c r="B303" s="142">
+      <c r="B349" s="228">
         <v>7.1250999999999998</v>
       </c>
-      <c r="C303" s="222"/>
-      <c r="D303" s="217"/>
-      <c r="E303" s="214"/>
-      <c r="F303" t="s">
+      <c r="C349" s="257"/>
+      <c r="D349" s="250"/>
+      <c r="E349" s="229"/>
+      <c r="F349" s="221" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A304" s="102" t="s">
+    <row r="350" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A350" s="227" t="s">
         <v>12</v>
       </c>
-      <c r="B304" s="142">
+      <c r="B350" s="228">
         <v>1.653</v>
       </c>
-      <c r="C304" s="222"/>
-      <c r="D304" s="217"/>
-      <c r="E304" s="214"/>
-    </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A305" s="103" t="s">
+      <c r="C350" s="257"/>
+      <c r="D350" s="250"/>
+      <c r="E350" s="229"/>
+      <c r="F350" s="221"/>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A351" s="231" t="s">
         <v>264</v>
       </c>
-      <c r="B305" s="144">
+      <c r="B351" s="232">
         <v>16.558399999999999</v>
       </c>
-      <c r="C305" s="222"/>
-      <c r="D305" s="223"/>
-      <c r="E305" s="215">
+      <c r="C351" s="257"/>
+      <c r="D351" s="257"/>
+      <c r="E351" s="233">
         <f>4.2044072151184/200</f>
         <v>2.1022036075592002E-2</v>
       </c>
-    </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A306" s="103" t="s">
+      <c r="F351" s="221"/>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A352" s="231" t="s">
         <v>14</v>
       </c>
-      <c r="B306" s="144">
+      <c r="B352" s="232">
         <v>1.8937999999999999</v>
       </c>
-      <c r="C306" s="222"/>
-      <c r="D306" s="223"/>
-      <c r="E306" s="215"/>
-    </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A307" s="103" t="s">
+      <c r="C352" s="257"/>
+      <c r="D352" s="257"/>
+      <c r="E352" s="233"/>
+      <c r="F352" s="221"/>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A353" s="231" t="s">
         <v>267</v>
       </c>
-      <c r="B307" s="144">
+      <c r="B353" s="232">
         <v>-0.92110000000000003</v>
       </c>
-      <c r="C307" s="222"/>
-      <c r="D307" s="218"/>
-      <c r="E307" s="215"/>
-      <c r="F307" t="s">
+      <c r="C353" s="257"/>
+      <c r="D353" s="251"/>
+      <c r="E353" s="233"/>
+      <c r="F353" s="221" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A308" s="103" t="s">
+    <row r="354" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A354" s="231" t="s">
         <v>14</v>
       </c>
-      <c r="B308" s="144">
+      <c r="B354" s="232">
         <v>1.6444000000000001</v>
       </c>
-      <c r="C308" s="222"/>
-      <c r="D308" s="218"/>
-      <c r="E308" s="215"/>
-    </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A309" s="104" t="s">
+      <c r="C354" s="257"/>
+      <c r="D354" s="251"/>
+      <c r="E354" s="233"/>
+      <c r="F354" s="221"/>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A355" s="235" t="s">
         <v>265</v>
       </c>
-      <c r="B309" s="191">
+      <c r="B355" s="252">
         <v>19.313500000000001</v>
       </c>
-      <c r="C309" s="190">
+      <c r="C355" s="253">
         <v>19.350200000000001</v>
       </c>
-      <c r="D309" s="223"/>
-      <c r="E309" s="216">
+      <c r="D355" s="257"/>
+      <c r="E355" s="238">
         <f>42.8255274295806/200</f>
         <v>0.214127637147903</v>
       </c>
-    </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A310" s="104" t="s">
+      <c r="F355" s="221"/>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A356" s="235" t="s">
         <v>16</v>
       </c>
-      <c r="B310" s="191">
+      <c r="B356" s="252">
         <v>1.4529000000000001</v>
       </c>
-      <c r="C310" s="190">
+      <c r="C356" s="253">
         <v>2.8311999999999999</v>
       </c>
-      <c r="D310" s="223"/>
-      <c r="E310" s="216"/>
-    </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A311" s="104" t="s">
+      <c r="D356" s="257"/>
+      <c r="E356" s="238"/>
+      <c r="F356" s="221"/>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A357" s="235" t="s">
         <v>268</v>
       </c>
-      <c r="B311" s="146">
+      <c r="B357" s="236">
         <v>18.4528</v>
       </c>
-      <c r="C311" s="191">
+      <c r="C357" s="252">
         <v>0.31040000000000001</v>
       </c>
-      <c r="D311" s="146"/>
-      <c r="E311" s="216"/>
-      <c r="F311" t="s">
+      <c r="D357" s="236"/>
+      <c r="E357" s="238"/>
+      <c r="F357" s="221" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A312" s="104" t="s">
+    <row r="358" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A358" s="235" t="s">
         <v>16</v>
       </c>
-      <c r="B312" s="146">
+      <c r="B358" s="236">
         <v>1.8001</v>
       </c>
-      <c r="C312" s="191">
+      <c r="C358" s="252">
         <v>1.6241000000000001</v>
       </c>
-      <c r="D312" s="146"/>
-      <c r="E312" s="167"/>
-    </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A313" s="104" t="s">
+      <c r="D358" s="236"/>
+      <c r="E358" s="240"/>
+      <c r="F358" s="221"/>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A359" s="235" t="s">
         <v>273</v>
       </c>
-      <c r="B313" s="146">
+      <c r="B359" s="236">
         <v>17010</v>
       </c>
-      <c r="C313" s="146">
+      <c r="C359" s="236">
         <v>17010</v>
       </c>
-      <c r="D313" s="191"/>
-      <c r="E313" s="167"/>
-    </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A314" s="76" t="s">
+      <c r="D359" s="252"/>
+      <c r="E359" s="240"/>
+      <c r="F359" s="221"/>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A360" s="241" t="s">
         <v>269</v>
       </c>
-      <c r="B314" s="196"/>
-      <c r="C314" s="209"/>
-      <c r="D314" s="224"/>
-      <c r="E314" s="207"/>
-    </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A315" s="76" t="s">
+      <c r="B360" s="242"/>
+      <c r="C360" s="243"/>
+      <c r="D360" s="259"/>
+      <c r="E360" s="244"/>
+      <c r="F360" s="221"/>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A361" s="241" t="s">
         <v>270</v>
       </c>
-      <c r="B315" s="196"/>
-      <c r="C315" s="209"/>
-      <c r="D315" s="224"/>
-      <c r="E315" s="207"/>
-    </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A316" s="76" t="s">
+      <c r="B361" s="242"/>
+      <c r="C361" s="243"/>
+      <c r="D361" s="259"/>
+      <c r="E361" s="244"/>
+      <c r="F361" s="221"/>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A362" s="241" t="s">
         <v>271</v>
       </c>
-      <c r="B316" s="196"/>
-      <c r="C316" s="209"/>
-      <c r="D316" s="209"/>
-      <c r="E316" s="207"/>
-    </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A317" s="76" t="s">
+      <c r="B362" s="242"/>
+      <c r="C362" s="243"/>
+      <c r="D362" s="243"/>
+      <c r="E362" s="244"/>
+      <c r="F362" s="221"/>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A363" s="241" t="s">
         <v>270</v>
       </c>
-      <c r="B317" s="196"/>
-      <c r="C317" s="209"/>
-      <c r="D317" s="209"/>
-      <c r="E317" s="207"/>
-    </row>
-    <row r="318" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A318" s="79" t="s">
+      <c r="B363" s="242"/>
+      <c r="C363" s="243"/>
+      <c r="D363" s="243"/>
+      <c r="E363" s="244"/>
+      <c r="F363" s="221"/>
+    </row>
+    <row r="364" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A364" s="247" t="s">
         <v>274</v>
       </c>
-      <c r="B318" s="80"/>
-      <c r="C318" s="80"/>
-      <c r="D318" s="80"/>
-      <c r="E318" s="208"/>
-    </row>
-    <row r="325" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A325" s="6" t="s">
+      <c r="B364" s="248"/>
+      <c r="C364" s="248"/>
+      <c r="D364" s="248"/>
+      <c r="E364" s="249"/>
+      <c r="F364" s="221"/>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A365" s="221"/>
+      <c r="B365" s="221"/>
+      <c r="C365" s="221"/>
+      <c r="D365" s="221"/>
+      <c r="E365" s="221"/>
+      <c r="F365" s="221"/>
+    </row>
+    <row r="371" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A371" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="326" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A326" s="15" t="s">
+    <row r="372" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A372" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="B326" s="15"/>
-      <c r="C326" s="15"/>
-      <c r="D326" s="15"/>
-      <c r="E326" s="15"/>
-      <c r="F326" s="15"/>
-      <c r="G326" s="15"/>
-    </row>
-    <row r="327" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A327" s="15" t="s">
+      <c r="B372" s="15"/>
+      <c r="C372" s="15"/>
+      <c r="D372" s="15"/>
+      <c r="E372" s="15"/>
+      <c r="F372" s="15"/>
+      <c r="G372" s="15"/>
+    </row>
+    <row r="373" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A373" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B327" s="15"/>
-      <c r="C327" s="15"/>
-      <c r="D327" s="15"/>
-      <c r="E327" s="15"/>
-      <c r="F327" s="15"/>
-      <c r="G327" s="15"/>
-    </row>
-    <row r="328" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A328" s="42" t="s">
+      <c r="B373" s="15"/>
+      <c r="C373" s="15"/>
+      <c r="D373" s="15"/>
+      <c r="E373" s="15"/>
+      <c r="F373" s="15"/>
+      <c r="G373" s="15"/>
+    </row>
+    <row r="374" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A374" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="B328" s="43">
+      <c r="B374" s="43">
         <v>-10</v>
       </c>
-      <c r="C328" s="43">
+      <c r="C374" s="43">
         <v>0</v>
       </c>
-      <c r="D328" s="43">
+      <c r="D374" s="43">
         <v>10</v>
       </c>
-      <c r="E328" s="50">
+      <c r="E374" s="50">
         <v>20</v>
       </c>
-      <c r="F328" s="44"/>
-      <c r="G328" s="44"/>
-    </row>
-    <row r="329" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A329" s="51" t="s">
+      <c r="F374" s="44"/>
+      <c r="G374" s="44"/>
+    </row>
+    <row r="375" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A375" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B329" s="8">
+      <c r="B375" s="8">
         <v>10.021800000000001</v>
       </c>
-      <c r="C329" s="8">
+      <c r="C375" s="8">
         <v>-1E-4</v>
       </c>
-      <c r="D329" s="8">
+      <c r="D375" s="8">
         <v>-10.0009</v>
       </c>
-      <c r="E329" s="23">
+      <c r="E375" s="23">
         <v>-20.009399999999999</v>
       </c>
-      <c r="F329" s="8"/>
-      <c r="G329" s="15"/>
-    </row>
-    <row r="330" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A330" s="51" t="s">
+      <c r="F375" s="8"/>
+      <c r="G375" s="15"/>
+    </row>
+    <row r="376" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A376" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B330" s="8">
+      <c r="B376" s="8">
         <v>0.40789999999999998</v>
       </c>
-      <c r="C330" s="8">
+      <c r="C376" s="8">
         <v>0.41980000000000001</v>
       </c>
-      <c r="D330" s="8">
+      <c r="D376" s="8">
         <v>0.42220000000000002</v>
       </c>
-      <c r="E330" s="23">
+      <c r="E376" s="23">
         <v>0.41310000000000002</v>
       </c>
-      <c r="F330" s="8"/>
-      <c r="G330" s="15"/>
-    </row>
-    <row r="331" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A331" s="29" t="s">
+      <c r="F376" s="8"/>
+      <c r="G376" s="15"/>
+    </row>
+    <row r="377" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A377" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B331" s="8">
+      <c r="B377" s="8">
         <v>8.0785</v>
       </c>
-      <c r="C331" s="8">
+      <c r="C377" s="8">
         <v>-0.36620000000000003</v>
       </c>
-      <c r="D331" s="8">
+      <c r="D377" s="8">
         <v>-10.040800000000001</v>
       </c>
-      <c r="E331" s="23">
+      <c r="E377" s="23">
         <v>-20.0139</v>
       </c>
-      <c r="F331" s="8"/>
-      <c r="G331" s="15"/>
-    </row>
-    <row r="332" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A332" s="29" t="s">
+      <c r="F377" s="8"/>
+      <c r="G377" s="15"/>
+    </row>
+    <row r="378" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A378" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B332" s="8">
+      <c r="B378" s="8">
         <v>0.4738</v>
       </c>
-      <c r="C332" s="8">
+      <c r="C378" s="8">
         <v>0.41570000000000001</v>
       </c>
-      <c r="D332" s="8">
+      <c r="D378" s="8">
         <v>0.42080000000000001</v>
       </c>
-      <c r="E332" s="23">
+      <c r="E378" s="23">
         <v>0.41360000000000002</v>
       </c>
-      <c r="F332" s="8"/>
-      <c r="G332" s="15"/>
-    </row>
-    <row r="333" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A333" s="29" t="s">
+      <c r="F378" s="8"/>
+      <c r="G378" s="15"/>
+    </row>
+    <row r="379" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A379" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B333" s="8">
+      <c r="B379" s="8">
         <v>6.2323000000000004</v>
       </c>
-      <c r="C333" s="8">
+      <c r="C379" s="8">
         <v>-0.8518</v>
       </c>
-      <c r="D333" s="8">
+      <c r="D379" s="8">
         <v>-10.102499999999999</v>
       </c>
-      <c r="E333" s="23">
+      <c r="E379" s="23">
         <v>-20.0198</v>
       </c>
-      <c r="F333" s="8"/>
-      <c r="G333" s="15"/>
-    </row>
-    <row r="334" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A334" s="30" t="s">
+      <c r="F379" s="8"/>
+      <c r="G379" s="15"/>
+    </row>
+    <row r="380" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A380" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B334" s="24">
+      <c r="B380" s="24">
         <v>0.49349999999999999</v>
       </c>
-      <c r="C334" s="24">
+      <c r="C380" s="24">
         <v>0.41720000000000002</v>
       </c>
-      <c r="D334" s="24">
+      <c r="D380" s="24">
         <v>0.42209999999999998</v>
       </c>
-      <c r="E334" s="25">
+      <c r="E380" s="25">
         <v>0.41389999999999999</v>
       </c>
-      <c r="F334" s="8"/>
-      <c r="G334" s="15"/>
-    </row>
-    <row r="335" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A335" s="15"/>
-      <c r="B335" s="15"/>
-      <c r="C335" s="15"/>
-      <c r="D335" s="15"/>
-      <c r="E335" s="15"/>
-      <c r="F335" s="15"/>
-      <c r="G335" s="15"/>
-    </row>
-    <row r="336" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A336" s="15"/>
-      <c r="B336" s="15"/>
-      <c r="C336" s="15"/>
-      <c r="D336" s="15"/>
-      <c r="E336" s="15"/>
-      <c r="F336" s="15"/>
-      <c r="G336" s="15"/>
-    </row>
-    <row r="337" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A337" s="15" t="s">
+      <c r="F380" s="8"/>
+      <c r="G380" s="15"/>
+    </row>
+    <row r="381" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A381" s="15"/>
+      <c r="B381" s="15"/>
+      <c r="C381" s="15"/>
+      <c r="D381" s="15"/>
+      <c r="E381" s="15"/>
+      <c r="F381" s="15"/>
+      <c r="G381" s="15"/>
+    </row>
+    <row r="382" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A382" s="15"/>
+      <c r="B382" s="15"/>
+      <c r="C382" s="15"/>
+      <c r="D382" s="15"/>
+      <c r="E382" s="15"/>
+      <c r="F382" s="15"/>
+      <c r="G382" s="15"/>
+    </row>
+    <row r="383" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A383" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="B337" s="15"/>
-      <c r="C337" s="15"/>
-      <c r="D337" s="15"/>
-      <c r="E337" s="15"/>
-      <c r="F337" s="15"/>
-      <c r="G337" s="15"/>
-    </row>
-    <row r="338" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A338" s="42" t="s">
+      <c r="B383" s="15"/>
+      <c r="C383" s="15"/>
+      <c r="D383" s="15"/>
+      <c r="E383" s="15"/>
+      <c r="F383" s="15"/>
+      <c r="G383" s="15"/>
+    </row>
+    <row r="384" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A384" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="B338" s="43">
+      <c r="B384" s="43">
         <v>-10</v>
       </c>
-      <c r="C338" s="43">
+      <c r="C384" s="43">
         <v>0</v>
       </c>
-      <c r="D338" s="43">
+      <c r="D384" s="43">
         <v>10</v>
       </c>
-      <c r="E338" s="43">
+      <c r="E384" s="43">
         <v>20</v>
       </c>
-      <c r="F338" s="50">
+      <c r="F384" s="50">
         <v>30</v>
       </c>
-      <c r="G338" s="15"/>
-    </row>
-    <row r="339" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A339" s="51" t="s">
+      <c r="G384" s="15"/>
+    </row>
+    <row r="385" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A385" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B339" s="8">
+      <c r="B385" s="8">
         <v>9.9992999999999999</v>
       </c>
-      <c r="C339" s="8">
+      <c r="C385" s="8">
         <v>9.2999999999999992E-3</v>
       </c>
-      <c r="D339" s="8">
+      <c r="D385" s="8">
         <v>-9.9928000000000008</v>
       </c>
-      <c r="E339" s="8">
+      <c r="E385" s="8">
         <v>-20.0136</v>
       </c>
-      <c r="F339" s="23">
+      <c r="F385" s="23">
         <v>-30.004000000000001</v>
       </c>
-      <c r="G339" s="15"/>
-    </row>
-    <row r="340" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A340" s="51" t="s">
+      <c r="G385" s="15"/>
+    </row>
+    <row r="386" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A386" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B340" s="8">
+      <c r="B386" s="8">
         <v>0.41639999999999999</v>
       </c>
-      <c r="C340" s="8">
+      <c r="C386" s="8">
         <v>0.4022</v>
       </c>
-      <c r="D340" s="8">
+      <c r="D386" s="8">
         <v>0.4098</v>
       </c>
-      <c r="E340" s="8">
+      <c r="E386" s="8">
         <v>0.42599999999999999</v>
       </c>
-      <c r="F340" s="23">
+      <c r="F386" s="23">
         <v>0.39079999999999998</v>
       </c>
-      <c r="G340" s="15"/>
-    </row>
-    <row r="341" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A341" s="29" t="s">
+      <c r="G386" s="15"/>
+    </row>
+    <row r="387" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A387" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B341" s="8">
+      <c r="B387" s="8">
         <v>2.6894</v>
       </c>
-      <c r="C341" s="8">
+      <c r="C387" s="8">
         <v>-4.6473000000000004</v>
       </c>
-      <c r="D341" s="8">
+      <c r="D387" s="8">
         <v>-11.911799999999999</v>
       </c>
-      <c r="E341" s="8">
+      <c r="E387" s="8">
         <v>-20.385999999999999</v>
       </c>
-      <c r="F341" s="23">
+      <c r="F387" s="23">
         <v>-30.0456</v>
       </c>
-      <c r="G341" s="15"/>
-    </row>
-    <row r="342" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A342" s="29" t="s">
+      <c r="G387" s="15"/>
+    </row>
+    <row r="388" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A388" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B342" s="8">
+      <c r="B388" s="8">
         <v>0.94330000000000003</v>
       </c>
-      <c r="C342" s="8">
+      <c r="C388" s="8">
         <v>0.70750000000000002</v>
       </c>
-      <c r="D342" s="8">
+      <c r="D388" s="8">
         <v>0.48320000000000002</v>
       </c>
-      <c r="E342" s="8">
+      <c r="E388" s="8">
         <v>0.42049999999999998</v>
       </c>
-      <c r="F342" s="23">
+      <c r="F388" s="23">
         <v>0.39340000000000003</v>
       </c>
-      <c r="G342" s="15"/>
-    </row>
-    <row r="343" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A343" s="29" t="s">
+      <c r="G388" s="15"/>
+    </row>
+    <row r="389" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A389" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B343" s="8">
+      <c r="B389" s="8">
         <v>-1.7606999999999999</v>
       </c>
-      <c r="C343" s="8">
+      <c r="C389" s="8">
         <v>-8.1674000000000007</v>
       </c>
-      <c r="D343" s="8">
+      <c r="D389" s="8">
         <v>-13.776999999999999</v>
       </c>
-      <c r="E343" s="8">
+      <c r="E389" s="8">
         <v>-20.873999999999999</v>
       </c>
-      <c r="F343" s="23">
+      <c r="F389" s="23">
         <v>-30.104199999999999</v>
       </c>
-      <c r="G343" s="15"/>
-    </row>
-    <row r="344" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A344" s="30" t="s">
+      <c r="G389" s="15"/>
+    </row>
+    <row r="390" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A390" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B344" s="24">
+      <c r="B390" s="24">
         <v>1.2151000000000001</v>
       </c>
-      <c r="C344" s="24">
+      <c r="C390" s="24">
         <v>0.77839999999999998</v>
       </c>
-      <c r="D344" s="24">
+      <c r="D390" s="24">
         <v>0.49209999999999998</v>
       </c>
-      <c r="E344" s="24">
+      <c r="E390" s="24">
         <v>0.41810000000000003</v>
       </c>
-      <c r="F344" s="25">
+      <c r="F390" s="25">
         <v>0.3926</v>
       </c>
-      <c r="G344" s="15"/>
-    </row>
-    <row r="345" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A345" s="15"/>
-      <c r="B345" s="15"/>
-      <c r="C345" s="15"/>
-      <c r="D345" s="15"/>
-      <c r="E345" s="15"/>
-      <c r="F345" s="15"/>
-      <c r="G345" s="15"/>
-    </row>
-    <row r="346" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="347" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A347" s="52" t="s">
+      <c r="G390" s="15"/>
+    </row>
+    <row r="391" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A391" s="15"/>
+      <c r="B391" s="15"/>
+      <c r="C391" s="15"/>
+      <c r="D391" s="15"/>
+      <c r="E391" s="15"/>
+      <c r="F391" s="15"/>
+      <c r="G391" s="15"/>
+    </row>
+    <row r="392" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="393" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A393" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B347" s="13"/>
-      <c r="C347" s="53">
+      <c r="B393" s="13"/>
+      <c r="C393" s="53">
         <v>-8.1576000000000004</v>
       </c>
     </row>
-    <row r="348" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A348" s="51" t="s">
+    <row r="394" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A394" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C348" s="36">
+      <c r="C394" s="36">
         <v>0.40889999999999999</v>
       </c>
     </row>
-    <row r="349" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A349" s="29" t="s">
+    <row r="395" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A395" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="C349" s="36">
+      <c r="C395" s="36">
         <v>-12.7606</v>
       </c>
     </row>
-    <row r="350" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A350" s="29" t="s">
+    <row r="396" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A396" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C350" s="36">
+      <c r="C396" s="36">
         <v>0.50029999999999997</v>
       </c>
     </row>
-    <row r="351" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A351" s="29" t="s">
+    <row r="397" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A397" s="29" t="s">
         <v>108</v>
       </c>
-      <c r="C351" s="36">
+      <c r="C397" s="36">
         <v>-8.1062999999999992</v>
       </c>
     </row>
-    <row r="352" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A352" s="30" t="s">
+    <row r="398" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A398" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B352" s="19"/>
-      <c r="C352" s="54">
+      <c r="B398" s="19"/>
+      <c r="C398" s="54">
         <v>0.77159999999999995</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="C301:C308"/>
-    <mergeCell ref="D301:D302"/>
-    <mergeCell ref="D305:D306"/>
-    <mergeCell ref="D309:D310"/>
-    <mergeCell ref="D314:D315"/>
+  <mergeCells count="19">
+    <mergeCell ref="C299:C306"/>
+    <mergeCell ref="D299:D300"/>
+    <mergeCell ref="D303:D304"/>
+    <mergeCell ref="D307:D308"/>
     <mergeCell ref="C279:C286"/>
     <mergeCell ref="D279:D280"/>
     <mergeCell ref="D283:D284"/>
     <mergeCell ref="D292:D293"/>
     <mergeCell ref="D287:D288"/>
+    <mergeCell ref="C347:C354"/>
+    <mergeCell ref="D347:D348"/>
+    <mergeCell ref="D351:D352"/>
+    <mergeCell ref="D355:D356"/>
+    <mergeCell ref="D360:D361"/>
+    <mergeCell ref="C321:C328"/>
+    <mergeCell ref="D321:D322"/>
+    <mergeCell ref="D325:D326"/>
+    <mergeCell ref="D329:D330"/>
+    <mergeCell ref="D334:D335"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7437,7 +8168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61FAE463-692A-4AB1-8AB9-770196756CC0}">
   <dimension ref="A1:I136"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A95" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
@@ -9311,12 +10042,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9434,15 +10162,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BCF7BB-2741-482F-B9A7-38B0145EE962}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F268FFC7-E0A8-474E-82F2-6EB808EA36C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9464,10 +10196,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F268FFC7-E0A8-474E-82F2-6EB808EA36C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BCF7BB-2741-482F-B9A7-38B0145EE962}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update pass2 for lorDT
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaoy\Documents\RTSNet_Journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8628BC4-6AF0-4F49-92F6-1783A68D3243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB3C5ED-271B-4F82-A978-B3D7A1D7CE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="305">
   <si>
     <t>1) Full info, RTSNet converges to RTS</t>
   </si>
@@ -960,12 +960,6 @@
   </si>
   <si>
     <t># of parameters RTSNet 2 pass</t>
-  </si>
-  <si>
-    <t>-6.4061|-6.4688</t>
-  </si>
-  <si>
-    <t>3.3104|3.3193</t>
   </si>
 </sst>
 </file>
@@ -1875,6 +1869,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1886,18 +1892,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2181,8 +2175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K407"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A289" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C294" sqref="C294"/>
+    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D320" sqref="D320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6726,10 +6720,10 @@
       <c r="B279" s="142">
         <v>-7.6313000000000004</v>
       </c>
-      <c r="C279" s="259" t="s">
+      <c r="C279" s="263" t="s">
         <v>45</v>
       </c>
-      <c r="D279" s="260" t="s">
+      <c r="D279" s="264" t="s">
         <v>45</v>
       </c>
       <c r="E279" s="213">
@@ -6744,8 +6738,8 @@
       <c r="B280" s="142">
         <v>2.891</v>
       </c>
-      <c r="C280" s="259"/>
-      <c r="D280" s="260"/>
+      <c r="C280" s="263"/>
+      <c r="D280" s="264"/>
       <c r="E280" s="213"/>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.35">
@@ -6755,7 +6749,7 @@
       <c r="B281" s="142">
         <v>-22.074200000000001</v>
       </c>
-      <c r="C281" s="259"/>
+      <c r="C281" s="263"/>
       <c r="D281" s="142">
         <v>-7.6565000000000003</v>
       </c>
@@ -6774,7 +6768,7 @@
       <c r="B282" s="142">
         <v>3.6943999999999999</v>
       </c>
-      <c r="C282" s="259"/>
+      <c r="C282" s="263"/>
       <c r="D282" s="142">
         <v>3.1446000000000001</v>
       </c>
@@ -6787,8 +6781,8 @@
       <c r="B283" s="218">
         <v>-8.7913999999999994</v>
       </c>
-      <c r="C283" s="259"/>
-      <c r="D283" s="260" t="s">
+      <c r="C283" s="263"/>
+      <c r="D283" s="264" t="s">
         <v>45</v>
       </c>
       <c r="E283" s="214">
@@ -6803,8 +6797,8 @@
       <c r="B284" s="218">
         <v>3.0541</v>
       </c>
-      <c r="C284" s="259"/>
-      <c r="D284" s="260"/>
+      <c r="C284" s="263"/>
+      <c r="D284" s="264"/>
       <c r="E284" s="214"/>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.35">
@@ -6814,7 +6808,7 @@
       <c r="B285" s="218">
         <v>-23.220700000000001</v>
       </c>
-      <c r="C285" s="259"/>
+      <c r="C285" s="263"/>
       <c r="D285" s="218">
         <v>-14.7516</v>
       </c>
@@ -6833,7 +6827,7 @@
       <c r="B286" s="218">
         <v>4.0807000000000002</v>
       </c>
-      <c r="C286" s="259"/>
+      <c r="C286" s="263"/>
       <c r="D286" s="218">
         <v>3.3081</v>
       </c>
@@ -6847,9 +6841,9 @@
         <v>-8.0848999999999993</v>
       </c>
       <c r="C287" s="146">
-        <v>-6.4104000000000001</v>
-      </c>
-      <c r="D287" s="262" t="s">
+        <v>-7.3674999999999997</v>
+      </c>
+      <c r="D287" s="266" t="s">
         <v>45</v>
       </c>
       <c r="E287" s="215">
@@ -6865,9 +6859,9 @@
         <v>2.9264000000000001</v>
       </c>
       <c r="C288" s="146">
-        <v>3.2963</v>
-      </c>
-      <c r="D288" s="262"/>
+        <v>2.9075000000000002</v>
+      </c>
+      <c r="D288" s="266"/>
       <c r="E288" s="215"/>
     </row>
     <row r="289" spans="1:6" x14ac:dyDescent="0.35">
@@ -6878,7 +6872,7 @@
         <v>-16.892900000000001</v>
       </c>
       <c r="C289" s="216">
-        <v>-21.4907</v>
+        <v>-21.717300000000002</v>
       </c>
       <c r="D289" s="219">
         <v>-15.788399999999999</v>
@@ -6899,7 +6893,7 @@
         <v>2.8605</v>
       </c>
       <c r="C290" s="216">
-        <v>3.6055999999999999</v>
+        <v>3.6478000000000002</v>
       </c>
       <c r="D290" s="216">
         <v>2.5225</v>
@@ -6928,10 +6922,10 @@
       <c r="B292" s="191">
         <v>-8.4316999999999993</v>
       </c>
-      <c r="C292" s="266" t="s">
-        <v>305</v>
-      </c>
-      <c r="D292" s="262" t="s">
+      <c r="C292" s="259">
+        <v>-7.3677000000000001</v>
+      </c>
+      <c r="D292" s="266" t="s">
         <v>45</v>
       </c>
       <c r="E292" s="215">
@@ -6946,10 +6940,10 @@
       <c r="B293" s="191">
         <v>2.9738000000000002</v>
       </c>
-      <c r="C293" s="266" t="s">
-        <v>306</v>
-      </c>
-      <c r="D293" s="262"/>
+      <c r="C293" s="259">
+        <v>2.8527</v>
+      </c>
+      <c r="D293" s="266"/>
       <c r="E293" s="215"/>
     </row>
     <row r="294" spans="1:6" x14ac:dyDescent="0.35">
@@ -6960,7 +6954,7 @@
         <v>-20.327400000000001</v>
       </c>
       <c r="C294" s="191">
-        <v>-21.667200000000001</v>
+        <v>-22.2407</v>
       </c>
       <c r="D294" s="219">
         <v>-15.899699999999999</v>
@@ -6981,7 +6975,7 @@
         <v>3.6972</v>
       </c>
       <c r="C295" s="191">
-        <v>3.6747999999999998</v>
+        <v>3.6762000000000001</v>
       </c>
       <c r="D295" s="216">
         <v>2.5417000000000001</v>
@@ -7013,7 +7007,7 @@
       <c r="C297" s="192">
         <v>20.891200000000001</v>
       </c>
-      <c r="D297" s="261"/>
+      <c r="D297" s="265"/>
       <c r="E297" s="207">
         <f>26.5463798046112/200</f>
         <v>0.13273189902305599</v>
@@ -7029,7 +7023,7 @@
       <c r="C298" s="192">
         <v>2.1716000000000002</v>
       </c>
-      <c r="D298" s="261"/>
+      <c r="D298" s="265"/>
       <c r="E298" s="207"/>
     </row>
     <row r="299" spans="1:6" x14ac:dyDescent="0.35">
@@ -7140,10 +7134,10 @@
         <v>263</v>
       </c>
       <c r="B308" s="217"/>
-      <c r="C308" s="259" t="s">
+      <c r="C308" s="263" t="s">
         <v>45</v>
       </c>
-      <c r="D308" s="260" t="s">
+      <c r="D308" s="264" t="s">
         <v>45</v>
       </c>
       <c r="E308" s="213">
@@ -7156,8 +7150,8 @@
         <v>12</v>
       </c>
       <c r="B309" s="217"/>
-      <c r="C309" s="259"/>
-      <c r="D309" s="260"/>
+      <c r="C309" s="263"/>
+      <c r="D309" s="264"/>
       <c r="E309" s="213"/>
     </row>
     <row r="310" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -7165,7 +7159,7 @@
         <v>266</v>
       </c>
       <c r="B310" s="217"/>
-      <c r="C310" s="259"/>
+      <c r="C310" s="263"/>
       <c r="D310" s="217"/>
       <c r="E310" s="213">
         <f>1.94739890098571/200</f>
@@ -7179,7 +7173,7 @@
       <c r="B311" s="217" t="s">
         <v>292</v>
       </c>
-      <c r="C311" s="259"/>
+      <c r="C311" s="263"/>
       <c r="D311" s="217"/>
       <c r="E311" s="213"/>
     </row>
@@ -7190,8 +7184,8 @@
       <c r="B312" s="256" t="s">
         <v>288</v>
       </c>
-      <c r="C312" s="259"/>
-      <c r="D312" s="260" t="s">
+      <c r="C312" s="263"/>
+      <c r="D312" s="264" t="s">
         <v>45</v>
       </c>
       <c r="E312" s="214">
@@ -7206,8 +7200,8 @@
       <c r="B313" s="256" t="s">
         <v>289</v>
       </c>
-      <c r="C313" s="259"/>
-      <c r="D313" s="260"/>
+      <c r="C313" s="263"/>
+      <c r="D313" s="264"/>
       <c r="E313" s="214"/>
     </row>
     <row r="314" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -7217,7 +7211,7 @@
       <c r="B314" s="256" t="s">
         <v>290</v>
       </c>
-      <c r="C314" s="259"/>
+      <c r="C314" s="263"/>
       <c r="D314" s="218">
         <v>-14.926600000000001</v>
       </c>
@@ -7233,7 +7227,7 @@
       <c r="B315" s="256" t="s">
         <v>291</v>
       </c>
-      <c r="C315" s="259"/>
+      <c r="C315" s="263"/>
       <c r="D315" s="218">
         <v>2.1204999999999998</v>
       </c>
@@ -7249,7 +7243,7 @@
       <c r="C316" s="220" t="s">
         <v>295</v>
       </c>
-      <c r="D316" s="261"/>
+      <c r="D316" s="265"/>
       <c r="E316" s="207">
         <f>26.5463798046112/200</f>
         <v>0.13273189902305599</v>
@@ -7265,7 +7259,7 @@
       <c r="C317" s="220" t="s">
         <v>296</v>
       </c>
-      <c r="D317" s="261"/>
+      <c r="D317" s="265"/>
       <c r="E317" s="207"/>
     </row>
     <row r="318" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -7376,10 +7370,10 @@
       <c r="B330" s="228">
         <v>1.4617</v>
       </c>
-      <c r="C330" s="263" t="s">
+      <c r="C330" s="260" t="s">
         <v>45</v>
       </c>
-      <c r="D330" s="263" t="s">
+      <c r="D330" s="260" t="s">
         <v>45</v>
       </c>
       <c r="E330" s="229">
@@ -7395,8 +7389,8 @@
       <c r="B331" s="228">
         <v>0.57669999999999999</v>
       </c>
-      <c r="C331" s="263"/>
-      <c r="D331" s="263"/>
+      <c r="C331" s="260"/>
+      <c r="D331" s="260"/>
       <c r="E331" s="229"/>
       <c r="F331" s="221"/>
     </row>
@@ -7405,7 +7399,7 @@
         <v>266</v>
       </c>
       <c r="B332" s="228"/>
-      <c r="C332" s="263"/>
+      <c r="C332" s="260"/>
       <c r="D332" s="230"/>
       <c r="E332" s="229">
         <f>1.94739890098571/200</f>
@@ -7420,7 +7414,7 @@
         <v>12</v>
       </c>
       <c r="B333" s="228"/>
-      <c r="C333" s="263"/>
+      <c r="C333" s="260"/>
       <c r="D333" s="230"/>
       <c r="E333" s="229"/>
       <c r="F333" s="221"/>
@@ -7432,8 +7426,8 @@
       <c r="B334" s="232">
         <v>-5.4771999999999998</v>
       </c>
-      <c r="C334" s="263"/>
-      <c r="D334" s="263" t="s">
+      <c r="C334" s="260"/>
+      <c r="D334" s="260" t="s">
         <v>45</v>
       </c>
       <c r="E334" s="233">
@@ -7449,8 +7443,8 @@
       <c r="B335" s="232">
         <v>0.625</v>
       </c>
-      <c r="C335" s="263"/>
-      <c r="D335" s="263"/>
+      <c r="C335" s="260"/>
+      <c r="D335" s="260"/>
       <c r="E335" s="233"/>
       <c r="F335" s="221"/>
     </row>
@@ -7459,7 +7453,7 @@
         <v>267</v>
       </c>
       <c r="B336" s="232"/>
-      <c r="C336" s="263"/>
+      <c r="C336" s="260"/>
       <c r="D336" s="234"/>
       <c r="E336" s="233">
         <f>4.09233212471008/200</f>
@@ -7474,7 +7468,7 @@
         <v>14</v>
       </c>
       <c r="B337" s="232"/>
-      <c r="C337" s="263"/>
+      <c r="C337" s="260"/>
       <c r="D337" s="234"/>
       <c r="E337" s="233"/>
       <c r="F337" s="221"/>
@@ -7485,7 +7479,7 @@
       </c>
       <c r="B338" s="236"/>
       <c r="C338" s="237"/>
-      <c r="D338" s="265" t="s">
+      <c r="D338" s="261" t="s">
         <v>45</v>
       </c>
       <c r="E338" s="238">
@@ -7500,7 +7494,7 @@
       </c>
       <c r="B339" s="236"/>
       <c r="C339" s="237"/>
-      <c r="D339" s="265"/>
+      <c r="D339" s="261"/>
       <c r="E339" s="238"/>
       <c r="F339" s="221"/>
     </row>
@@ -7553,7 +7547,7 @@
         <v>27.1051</v>
       </c>
       <c r="C343" s="243"/>
-      <c r="D343" s="264"/>
+      <c r="D343" s="262"/>
       <c r="E343" s="244"/>
       <c r="F343" s="221"/>
     </row>
@@ -7565,7 +7559,7 @@
         <v>2.4712000000000001</v>
       </c>
       <c r="C344" s="243"/>
-      <c r="D344" s="264"/>
+      <c r="D344" s="262"/>
       <c r="E344" s="244"/>
       <c r="F344" s="221"/>
     </row>
@@ -7645,8 +7639,8 @@
       <c r="B356" s="228">
         <v>18.8626</v>
       </c>
-      <c r="C356" s="263"/>
-      <c r="D356" s="263"/>
+      <c r="C356" s="260"/>
+      <c r="D356" s="260"/>
       <c r="E356" s="229">
         <f>2.00304269790649/200</f>
         <v>1.0015213489532451E-2</v>
@@ -7660,8 +7654,8 @@
       <c r="B357" s="228">
         <v>1.7168000000000001</v>
       </c>
-      <c r="C357" s="263"/>
-      <c r="D357" s="263"/>
+      <c r="C357" s="260"/>
+      <c r="D357" s="260"/>
       <c r="E357" s="229"/>
       <c r="F357" s="221"/>
     </row>
@@ -7672,7 +7666,7 @@
       <c r="B358" s="228">
         <v>7.1250999999999998</v>
       </c>
-      <c r="C358" s="263"/>
+      <c r="C358" s="260"/>
       <c r="D358" s="250"/>
       <c r="E358" s="229"/>
       <c r="F358" s="221" t="s">
@@ -7686,7 +7680,7 @@
       <c r="B359" s="228">
         <v>1.653</v>
       </c>
-      <c r="C359" s="263"/>
+      <c r="C359" s="260"/>
       <c r="D359" s="250"/>
       <c r="E359" s="229"/>
       <c r="F359" s="221"/>
@@ -7698,8 +7692,8 @@
       <c r="B360" s="232">
         <v>16.558399999999999</v>
       </c>
-      <c r="C360" s="263"/>
-      <c r="D360" s="263"/>
+      <c r="C360" s="260"/>
+      <c r="D360" s="260"/>
       <c r="E360" s="233">
         <f>4.2044072151184/200</f>
         <v>2.1022036075592002E-2</v>
@@ -7713,8 +7707,8 @@
       <c r="B361" s="232">
         <v>1.8937999999999999</v>
       </c>
-      <c r="C361" s="263"/>
-      <c r="D361" s="263"/>
+      <c r="C361" s="260"/>
+      <c r="D361" s="260"/>
       <c r="E361" s="233"/>
       <c r="F361" s="221"/>
     </row>
@@ -7725,7 +7719,7 @@
       <c r="B362" s="232">
         <v>-0.92110000000000003</v>
       </c>
-      <c r="C362" s="263"/>
+      <c r="C362" s="260"/>
       <c r="D362" s="251"/>
       <c r="E362" s="233"/>
       <c r="F362" s="221" t="s">
@@ -7739,7 +7733,7 @@
       <c r="B363" s="232">
         <v>1.6444000000000001</v>
       </c>
-      <c r="C363" s="263"/>
+      <c r="C363" s="260"/>
       <c r="D363" s="251"/>
       <c r="E363" s="233"/>
       <c r="F363" s="221"/>
@@ -7754,7 +7748,7 @@
       <c r="C364" s="253">
         <v>19.350200000000001</v>
       </c>
-      <c r="D364" s="263"/>
+      <c r="D364" s="260"/>
       <c r="E364" s="238">
         <f>42.8255274295806/200</f>
         <v>0.214127637147903</v>
@@ -7771,7 +7765,7 @@
       <c r="C365" s="253">
         <v>2.8311999999999999</v>
       </c>
-      <c r="D365" s="263"/>
+      <c r="D365" s="260"/>
       <c r="E365" s="238"/>
       <c r="F365" s="221"/>
     </row>
@@ -7825,7 +7819,7 @@
       </c>
       <c r="B369" s="242"/>
       <c r="C369" s="243"/>
-      <c r="D369" s="264"/>
+      <c r="D369" s="262"/>
       <c r="E369" s="244"/>
       <c r="F369" s="221"/>
     </row>
@@ -7835,7 +7829,7 @@
       </c>
       <c r="B370" s="242"/>
       <c r="C370" s="243"/>
-      <c r="D370" s="264"/>
+      <c r="D370" s="262"/>
       <c r="E370" s="244"/>
       <c r="F370" s="221"/>
     </row>
@@ -8275,16 +8269,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C330:C337"/>
-    <mergeCell ref="D330:D331"/>
-    <mergeCell ref="D334:D335"/>
-    <mergeCell ref="D338:D339"/>
-    <mergeCell ref="D343:D344"/>
-    <mergeCell ref="C356:C363"/>
-    <mergeCell ref="D356:D357"/>
-    <mergeCell ref="D360:D361"/>
-    <mergeCell ref="D364:D365"/>
-    <mergeCell ref="D369:D370"/>
     <mergeCell ref="C308:C315"/>
     <mergeCell ref="D308:D309"/>
     <mergeCell ref="D312:D313"/>
@@ -8295,6 +8279,16 @@
     <mergeCell ref="D297:D298"/>
     <mergeCell ref="D287:D288"/>
     <mergeCell ref="D292:D293"/>
+    <mergeCell ref="C356:C363"/>
+    <mergeCell ref="D356:D357"/>
+    <mergeCell ref="D360:D361"/>
+    <mergeCell ref="D364:D365"/>
+    <mergeCell ref="D369:D370"/>
+    <mergeCell ref="C330:C337"/>
+    <mergeCell ref="D330:D331"/>
+    <mergeCell ref="D334:D335"/>
+    <mergeCell ref="D338:D339"/>
+    <mergeCell ref="D343:D344"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10180,12 +10174,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10303,15 +10294,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BCF7BB-2741-482F-B9A7-38B0145EE962}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F268FFC7-E0A8-474E-82F2-6EB808EA36C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10333,10 +10328,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F268FFC7-E0A8-474E-82F2-6EB808EA36C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2BCF7BB-2741-482F-B9A7-38B0145EE962}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>